<commit_message>
Update automatico via Actualizar 05-05-2020 19-54-40
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{491879EB-6C43-4C97-94A4-7BFBB2C07B8F}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{219918D1-A8A7-4D78-A6E1-F82584E74BA3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="216">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -288,7 +288,7 @@
     <t>HND-0404</t>
   </si>
   <si>
-    <t>Angie 2</t>
+    <t xml:space="preserve">Farmacia Angie </t>
   </si>
   <si>
     <t>0413</t>
@@ -333,13 +333,13 @@
     <t>Farmacia Leyla</t>
   </si>
   <si>
-    <t>Farmacia Santa Bárbaraarbara</t>
-  </si>
-  <si>
-    <t>Farmacia del Ángel</t>
-  </si>
-  <si>
-    <t>Farmacia Maria Auxiliadora</t>
+    <t>Farmacia Santa Bárbara</t>
+  </si>
+  <si>
+    <t>Farmacia El Ángel</t>
+  </si>
+  <si>
+    <t>Farmacia María Auxiliadora</t>
   </si>
   <si>
     <t>Farmacia Fiallos Flores</t>
@@ -351,132 +351,123 @@
     <t>MetroPharma</t>
   </si>
   <si>
+    <t>FarmaCity</t>
+  </si>
+  <si>
+    <t>Farmacias Punto Farma</t>
+  </si>
+  <si>
+    <t>0502</t>
+  </si>
+  <si>
+    <t>Choloma</t>
+  </si>
+  <si>
+    <t>050201</t>
+  </si>
+  <si>
+    <t>HND-0502</t>
+  </si>
+  <si>
+    <t>0511</t>
+  </si>
+  <si>
+    <t>Villanueva</t>
+  </si>
+  <si>
+    <t>051101</t>
+  </si>
+  <si>
+    <t>HND-0511</t>
+  </si>
+  <si>
+    <t>0512</t>
+  </si>
+  <si>
+    <t>La Lima</t>
+  </si>
+  <si>
+    <t>051201</t>
+  </si>
+  <si>
+    <t>HND-0512</t>
+  </si>
+  <si>
+    <t>Farmacia La Fuente</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>Choluteca</t>
+  </si>
+  <si>
+    <t>0601</t>
+  </si>
+  <si>
+    <t>060101</t>
+  </si>
+  <si>
+    <t>HND-0601</t>
+  </si>
+  <si>
+    <t>0606</t>
+  </si>
+  <si>
+    <t>El Triunfo</t>
+  </si>
+  <si>
+    <t>060603</t>
+  </si>
+  <si>
+    <t>El Cedrito</t>
+  </si>
+  <si>
+    <t>HND-0606</t>
+  </si>
+  <si>
+    <t>Farmacia La Fe</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>Francisco Morazán</t>
+  </si>
+  <si>
+    <t>0801</t>
+  </si>
+  <si>
+    <t>Distrito Central</t>
+  </si>
+  <si>
+    <t>080101</t>
+  </si>
+  <si>
+    <t>HND-0801</t>
+  </si>
+  <si>
+    <t>SolFarma</t>
+  </si>
+  <si>
+    <t>Farmacia GMT</t>
+  </si>
+  <si>
+    <t>Rivera Ortiz</t>
+  </si>
+  <si>
+    <t>Punto Farma Kennedy</t>
+  </si>
+  <si>
+    <t>Jehova</t>
+  </si>
+  <si>
+    <t>Farmacia Farmacity</t>
+  </si>
+  <si>
     <t>Farma City</t>
   </si>
   <si>
-    <t>Farmacia Punto Farma</t>
-  </si>
-  <si>
-    <t>0502</t>
-  </si>
-  <si>
-    <t>Choloma</t>
-  </si>
-  <si>
-    <t>050201</t>
-  </si>
-  <si>
-    <t>HND-0502</t>
-  </si>
-  <si>
-    <t>0511</t>
-  </si>
-  <si>
-    <t>Villanueva</t>
-  </si>
-  <si>
-    <t>051101</t>
-  </si>
-  <si>
-    <t>HND-0511</t>
-  </si>
-  <si>
-    <t>0512</t>
-  </si>
-  <si>
-    <t>La Lima</t>
-  </si>
-  <si>
-    <t>051201</t>
-  </si>
-  <si>
-    <t>HND-0512</t>
-  </si>
-  <si>
-    <t>Farmacia La Fuente</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>Choluteca</t>
-  </si>
-  <si>
-    <t>0601</t>
-  </si>
-  <si>
-    <t>060101</t>
-  </si>
-  <si>
-    <t>HND-0601</t>
-  </si>
-  <si>
-    <t>0606</t>
-  </si>
-  <si>
-    <t>El Triunfo</t>
-  </si>
-  <si>
-    <t>060603</t>
-  </si>
-  <si>
-    <t>El Cedrito</t>
-  </si>
-  <si>
-    <t>HND-0606</t>
-  </si>
-  <si>
-    <t>Farmacia La Fe</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>Francisco Morazán</t>
-  </si>
-  <si>
-    <t>0801</t>
-  </si>
-  <si>
-    <t>Distrito Central</t>
-  </si>
-  <si>
-    <t>080101</t>
-  </si>
-  <si>
-    <t>HND-0801</t>
-  </si>
-  <si>
-    <t>FarmCity</t>
-  </si>
-  <si>
-    <t>Punto Farma</t>
-  </si>
-  <si>
-    <t>SolFarma</t>
-  </si>
-  <si>
-    <t>Farmacity</t>
-  </si>
-  <si>
-    <t>Farmacia GMT</t>
-  </si>
-  <si>
-    <t>Rivera Ortiz</t>
-  </si>
-  <si>
-    <t>Punto Farma Kennedy</t>
-  </si>
-  <si>
-    <t>Farmacias Punto Farma</t>
-  </si>
-  <si>
-    <t>Jehova</t>
-  </si>
-  <si>
-    <t>Farmacia Farmacity</t>
-  </si>
-  <si>
     <t>Farmacia Santa Ana</t>
   </si>
   <si>
@@ -501,9 +492,6 @@
     <t>Farmacia Alpha</t>
   </si>
   <si>
-    <t>Punto Farma Quinta Avenida</t>
-  </si>
-  <si>
     <t>Farma Todo</t>
   </si>
   <si>
@@ -568,9 +556,6 @@
   </si>
   <si>
     <t>Farmacia Krisia</t>
-  </si>
-  <si>
-    <t>FarmaCity</t>
   </si>
   <si>
     <t xml:space="preserve">Farmacia Regis </t>
@@ -1670,8 +1655,8 @@
   <dimension ref="A1:W162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="N2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U10" sqref="U10"/>
+      <pane ySplit="1" topLeftCell="O74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U80" sqref="U80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -6930,7 +6915,7 @@
         <v>35</v>
       </c>
       <c r="U77" s="1" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="V77" s="2">
         <v>14.9177</v>
@@ -6998,7 +6983,7 @@
         <v>35</v>
       </c>
       <c r="U78" s="1" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="V78" s="2">
         <v>14.920199999999999</v>
@@ -7134,7 +7119,7 @@
         <v>35</v>
       </c>
       <c r="U80" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="V80" s="2">
         <v>14.923299999999999</v>
@@ -7202,7 +7187,7 @@
         <v>35</v>
       </c>
       <c r="U81" s="1" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="V81" s="2">
         <v>14.927899999999999</v>
@@ -7270,7 +7255,7 @@
         <v>35</v>
       </c>
       <c r="U82" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="V82" s="2">
         <v>14.8439</v>
@@ -7406,7 +7391,7 @@
         <v>35</v>
       </c>
       <c r="U84" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="V84" s="2">
         <v>15.2738</v>
@@ -7542,7 +7527,7 @@
         <v>35</v>
       </c>
       <c r="U86" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="V86" s="2">
         <v>15.3123</v>
@@ -7610,7 +7595,7 @@
         <v>35</v>
       </c>
       <c r="U87" s="1" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="V87" s="2">
         <v>15.3133</v>
@@ -7678,7 +7663,7 @@
         <v>35</v>
       </c>
       <c r="U88" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="V88" s="2">
         <v>15.314</v>
@@ -7746,7 +7731,7 @@
         <v>35</v>
       </c>
       <c r="U89" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="V89" s="2">
         <v>15.314299999999999</v>
@@ -7882,7 +7867,7 @@
         <v>35</v>
       </c>
       <c r="U91" s="1" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="V91" s="2">
         <v>14.8527</v>
@@ -8562,7 +8547,7 @@
         <v>35</v>
       </c>
       <c r="U101" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="V101" s="2">
         <v>13.5337</v>
@@ -8630,7 +8615,7 @@
         <v>35</v>
       </c>
       <c r="U102" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="V102" s="2">
         <v>13.280799999999999</v>
@@ -8698,7 +8683,7 @@
         <v>35</v>
       </c>
       <c r="U103" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="V103" s="2">
         <v>13.2742</v>
@@ -8766,7 +8751,7 @@
         <v>35</v>
       </c>
       <c r="U104" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="V104" s="2">
         <v>13.285</v>
@@ -8834,7 +8819,7 @@
         <v>35</v>
       </c>
       <c r="U105" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="V105" s="2">
         <v>13.3597</v>
@@ -8970,7 +8955,7 @@
         <v>35</v>
       </c>
       <c r="U107" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="V107" s="2">
         <v>13.268700000000001</v>
@@ -9038,7 +9023,7 @@
         <v>35</v>
       </c>
       <c r="U108" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="V108" s="2">
         <v>13.251200000000001</v>
@@ -9106,7 +9091,7 @@
         <v>35</v>
       </c>
       <c r="U109" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="V109" s="2">
         <v>13.254</v>
@@ -9378,7 +9363,7 @@
         <v>35</v>
       </c>
       <c r="U113" s="1" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="V113" s="2">
         <v>13.596299999999999</v>
@@ -9514,7 +9499,7 @@
         <v>35</v>
       </c>
       <c r="U115" s="1" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="V115" s="2">
         <v>13.4175</v>
@@ -9650,7 +9635,7 @@
         <v>35</v>
       </c>
       <c r="U117" s="1" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="V117" s="2">
         <v>13.4306</v>
@@ -9718,7 +9703,7 @@
         <v>35</v>
       </c>
       <c r="U118" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="V118" s="2">
         <v>13.4314</v>
@@ -9786,7 +9771,7 @@
         <v>35</v>
       </c>
       <c r="U119" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="V119" s="2">
         <v>13.4329</v>
@@ -10058,7 +10043,7 @@
         <v>35</v>
       </c>
       <c r="U123" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="V123" s="2">
         <v>13.4544</v>
@@ -10126,7 +10111,7 @@
         <v>35</v>
       </c>
       <c r="U124" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="V124" s="2">
         <v>13.4565</v>
@@ -10194,7 +10179,7 @@
         <v>35</v>
       </c>
       <c r="U125" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="V125" s="2">
         <v>15.132300000000001</v>
@@ -10398,7 +10383,7 @@
         <v>35</v>
       </c>
       <c r="U128" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="V128" s="2">
         <v>15.5343</v>
@@ -10466,7 +10451,7 @@
         <v>35</v>
       </c>
       <c r="U129" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="V129" s="2">
         <v>15.5352</v>
@@ -10534,7 +10519,7 @@
         <v>35</v>
       </c>
       <c r="U130" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="V130" s="2">
         <v>15.536099999999999</v>
@@ -10670,7 +10655,7 @@
         <v>35</v>
       </c>
       <c r="U132" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="V132" s="2">
         <v>15.543200000000001</v>
@@ -10738,7 +10723,7 @@
         <v>35</v>
       </c>
       <c r="U133" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="V133" s="2">
         <v>15.543200000000001</v>
@@ -10806,7 +10791,7 @@
         <v>35</v>
       </c>
       <c r="U134" s="1" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="V134" s="2">
         <v>15.543200000000001</v>
@@ -10912,37 +10897,37 @@
         <v>6</v>
       </c>
       <c r="J136" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K136" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L136" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M136" s="1">
+        <v>1</v>
+      </c>
+      <c r="N136" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O136" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P136" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q136" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="R136" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S136" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U136" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="K136" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="L136" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M136" s="1">
-        <v>1</v>
-      </c>
-      <c r="N136" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="O136" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="P136" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q136" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="R136" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S136" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U136" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="V136" s="2">
         <v>15.55</v>
@@ -10980,37 +10965,37 @@
         <v>6</v>
       </c>
       <c r="J137" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K137" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L137" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M137" s="1">
+        <v>1</v>
+      </c>
+      <c r="N137" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O137" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P137" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q137" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="R137" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S137" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U137" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="L137" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M137" s="1">
-        <v>1</v>
-      </c>
-      <c r="N137" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="O137" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="P137" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q137" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="R137" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S137" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U137" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="V137" s="2">
         <v>15.550800000000001</v>
@@ -11048,10 +11033,10 @@
         <v>6</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K138" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="L138" s="1" t="s">
         <v>30</v>
@@ -11060,16 +11045,16 @@
         <v>1</v>
       </c>
       <c r="N138" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="O138" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="P138" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q138" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="R138" s="1" t="s">
         <v>34</v>
@@ -11104,10 +11089,10 @@
         <v>10</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H139" s="1" t="s">
         <v>27</v>
@@ -11116,10 +11101,10 @@
         <v>7</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K139" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="L139" s="1" t="s">
         <v>30</v>
@@ -11128,16 +11113,16 @@
         <v>1</v>
       </c>
       <c r="N139" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="O139" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="P139" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q139" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="R139" s="1" t="s">
         <v>34</v>
@@ -11172,10 +11157,10 @@
         <v>10</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H140" s="1" t="s">
         <v>27</v>
@@ -11184,37 +11169,37 @@
         <v>7</v>
       </c>
       <c r="J140" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="K140" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="L140" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M140" s="1">
+        <v>1</v>
+      </c>
+      <c r="N140" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O140" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="P140" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q140" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="R140" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S140" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U140" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="K140" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="L140" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M140" s="1">
-        <v>1</v>
-      </c>
-      <c r="N140" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="O140" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="P140" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q140" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="R140" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S140" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U140" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="V140" s="2">
         <v>15.382999999999999</v>
@@ -11240,10 +11225,10 @@
         <v>10</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H141" s="1" t="s">
         <v>27</v>
@@ -11252,10 +11237,10 @@
         <v>7</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K141" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="L141" s="1" t="s">
         <v>30</v>
@@ -11264,16 +11249,16 @@
         <v>1</v>
       </c>
       <c r="N141" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="O141" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="P141" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q141" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="R141" s="1" t="s">
         <v>34</v>
@@ -11282,7 +11267,7 @@
         <v>35</v>
       </c>
       <c r="U141" s="1" t="s">
-        <v>178</v>
+        <v>105</v>
       </c>
       <c r="V141" s="2">
         <v>15.387600000000001</v>
@@ -11308,10 +11293,10 @@
         <v>10</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H142" s="1" t="s">
         <v>27</v>
@@ -11320,10 +11305,10 @@
         <v>7</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="L142" s="1" t="s">
         <v>30</v>
@@ -11332,16 +11317,16 @@
         <v>1</v>
       </c>
       <c r="N142" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="O142" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="P142" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q142" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="R142" s="1" t="s">
         <v>34</v>
@@ -11376,10 +11361,10 @@
         <v>10</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H143" s="1" t="s">
         <v>27</v>
@@ -11388,37 +11373,37 @@
         <v>7</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K143" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="L143" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M143" s="1">
+        <v>1</v>
+      </c>
+      <c r="N143" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O143" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="P143" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q143" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="R143" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S143" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U143" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="L143" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M143" s="1">
-        <v>1</v>
-      </c>
-      <c r="N143" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="O143" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="P143" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q143" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="R143" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S143" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U143" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="V143" s="2">
         <v>15.388400000000001</v>
@@ -11444,49 +11429,49 @@
         <v>11</v>
       </c>
       <c r="F144" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H144" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I144" s="1">
+        <v>1</v>
+      </c>
+      <c r="J144" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="K144" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="L144" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M144" s="1">
+        <v>1</v>
+      </c>
+      <c r="N144" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="O144" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="P144" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q144" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="G144" s="1" t="s">
+      <c r="R144" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S144" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U144" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="H144" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I144" s="1">
-        <v>1</v>
-      </c>
-      <c r="J144" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="K144" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="L144" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M144" s="1">
-        <v>1</v>
-      </c>
-      <c r="N144" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="O144" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="P144" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q144" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="R144" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S144" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U144" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="V144" s="2">
         <v>15.3889</v>
@@ -11512,10 +11497,10 @@
         <v>11</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H145" s="1" t="s">
         <v>27</v>
@@ -11524,10 +11509,10 @@
         <v>2</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="L145" s="1" t="s">
         <v>30</v>
@@ -11536,16 +11521,16 @@
         <v>1</v>
       </c>
       <c r="N145" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="O145" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="P145" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q145" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="R145" s="1" t="s">
         <v>34</v>
@@ -11554,7 +11539,7 @@
         <v>35</v>
       </c>
       <c r="U145" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="V145" s="2">
         <v>15.393000000000001</v>
@@ -11580,10 +11565,10 @@
         <v>12</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>27</v>
@@ -11592,10 +11577,10 @@
         <v>17</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="K146" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="L146" s="1" t="s">
         <v>30</v>
@@ -11604,16 +11589,16 @@
         <v>7</v>
       </c>
       <c r="N146" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="O146" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="P146" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q146" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="R146" s="1" t="s">
         <v>34</v>
@@ -11648,49 +11633,49 @@
         <v>13</v>
       </c>
       <c r="F147" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H147" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I147" s="1">
+        <v>1</v>
+      </c>
+      <c r="J147" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="K147" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L147" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M147" s="1">
+        <v>1</v>
+      </c>
+      <c r="N147" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O147" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="P147" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q147" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G147" s="1" t="s">
+      <c r="R147" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S147" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U147" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="H147" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I147" s="1">
-        <v>1</v>
-      </c>
-      <c r="J147" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="K147" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="L147" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M147" s="1">
-        <v>1</v>
-      </c>
-      <c r="N147" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="O147" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="P147" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q147" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="R147" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S147" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U147" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="V147" s="2">
         <v>15.393599999999999</v>
@@ -11716,49 +11701,49 @@
         <v>13</v>
       </c>
       <c r="F148" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H148" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I148" s="1">
+        <v>1</v>
+      </c>
+      <c r="J148" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="K148" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L148" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M148" s="1">
+        <v>1</v>
+      </c>
+      <c r="N148" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O148" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="P148" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q148" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G148" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H148" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I148" s="1">
-        <v>1</v>
-      </c>
-      <c r="J148" s="1" t="s">
+      <c r="R148" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S148" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U148" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="K148" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="L148" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M148" s="1">
-        <v>1</v>
-      </c>
-      <c r="N148" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="O148" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="P148" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q148" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="R148" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S148" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U148" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="V148" s="2">
         <v>15.395200000000001</v>
@@ -11784,49 +11769,49 @@
         <v>13</v>
       </c>
       <c r="F149" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H149" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I149" s="1">
+        <v>1</v>
+      </c>
+      <c r="J149" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="K149" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L149" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M149" s="1">
+        <v>1</v>
+      </c>
+      <c r="N149" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O149" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="P149" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q149" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G149" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H149" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I149" s="1">
-        <v>1</v>
-      </c>
-      <c r="J149" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="K149" s="1" t="s">
+      <c r="R149" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S149" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U149" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="L149" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M149" s="1">
-        <v>1</v>
-      </c>
-      <c r="N149" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="O149" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="P149" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q149" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="R149" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S149" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U149" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="V149" s="2">
         <v>15.3955</v>
@@ -11852,49 +11837,49 @@
         <v>13</v>
       </c>
       <c r="F150" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H150" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I150" s="1">
+        <v>1</v>
+      </c>
+      <c r="J150" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="K150" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L150" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M150" s="1">
+        <v>1</v>
+      </c>
+      <c r="N150" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O150" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="P150" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q150" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G150" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H150" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I150" s="1">
-        <v>1</v>
-      </c>
-      <c r="J150" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="K150" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="L150" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M150" s="1">
-        <v>1</v>
-      </c>
-      <c r="N150" s="1" t="s">
+      <c r="R150" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S150" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U150" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="O150" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="P150" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q150" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="R150" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S150" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U150" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="V150" s="2">
         <v>15.3956</v>
@@ -11920,49 +11905,49 @@
         <v>13</v>
       </c>
       <c r="F151" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H151" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I151" s="1">
+        <v>1</v>
+      </c>
+      <c r="J151" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="K151" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L151" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M151" s="1">
+        <v>1</v>
+      </c>
+      <c r="N151" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O151" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="P151" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q151" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G151" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H151" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I151" s="1">
-        <v>1</v>
-      </c>
-      <c r="J151" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="K151" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="L151" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M151" s="1">
-        <v>1</v>
-      </c>
-      <c r="N151" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="O151" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="P151" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q151" s="1" t="s">
+      <c r="R151" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S151" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U151" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="R151" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S151" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U151" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="V151" s="2">
         <v>15.3956</v>
@@ -11988,10 +11973,10 @@
         <v>18</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H152" s="1" t="s">
         <v>27</v>
@@ -12000,10 +11985,10 @@
         <v>4</v>
       </c>
       <c r="J152" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="K152" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="L152" s="1" t="s">
         <v>30</v>
@@ -12012,16 +11997,16 @@
         <v>1</v>
       </c>
       <c r="N152" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="O152" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P152" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q152" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="R152" s="1" t="s">
         <v>34</v>
@@ -12056,10 +12041,10 @@
         <v>18</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H153" s="1" t="s">
         <v>27</v>
@@ -12068,10 +12053,10 @@
         <v>4</v>
       </c>
       <c r="J153" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="K153" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="L153" s="1" t="s">
         <v>30</v>
@@ -12080,16 +12065,16 @@
         <v>1</v>
       </c>
       <c r="N153" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="O153" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P153" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q153" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="R153" s="1" t="s">
         <v>34</v>
@@ -12124,10 +12109,10 @@
         <v>18</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H154" s="1" t="s">
         <v>27</v>
@@ -12136,10 +12121,10 @@
         <v>4</v>
       </c>
       <c r="J154" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="K154" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="L154" s="1" t="s">
         <v>30</v>
@@ -12148,16 +12133,16 @@
         <v>1</v>
       </c>
       <c r="N154" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="O154" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P154" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q154" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="R154" s="1" t="s">
         <v>34</v>
@@ -12166,7 +12151,7 @@
         <v>35</v>
       </c>
       <c r="U154" s="1" t="s">
-        <v>178</v>
+        <v>105</v>
       </c>
       <c r="V154" s="2">
         <v>15.3978</v>
@@ -12192,10 +12177,10 @@
         <v>18</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H155" s="1" t="s">
         <v>27</v>
@@ -12204,10 +12189,10 @@
         <v>4</v>
       </c>
       <c r="J155" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="K155" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="L155" s="1" t="s">
         <v>30</v>
@@ -12216,16 +12201,16 @@
         <v>1</v>
       </c>
       <c r="N155" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="O155" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P155" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q155" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="R155" s="1" t="s">
         <v>34</v>
@@ -12260,10 +12245,10 @@
         <v>18</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H156" s="1" t="s">
         <v>27</v>
@@ -12272,10 +12257,10 @@
         <v>4</v>
       </c>
       <c r="J156" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="K156" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="L156" s="1" t="s">
         <v>30</v>
@@ -12284,16 +12269,16 @@
         <v>1</v>
       </c>
       <c r="N156" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="O156" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P156" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q156" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="R156" s="1" t="s">
         <v>34</v>
@@ -12302,7 +12287,7 @@
         <v>35</v>
       </c>
       <c r="U156" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="V156" s="2">
         <v>15.398199999999999</v>
@@ -12328,10 +12313,10 @@
         <v>18</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H157" s="1" t="s">
         <v>27</v>
@@ -12340,37 +12325,37 @@
         <v>4</v>
       </c>
       <c r="J157" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="K157" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="L157" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M157" s="1">
+        <v>1</v>
+      </c>
+      <c r="N157" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="O157" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="P157" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q157" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="R157" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S157" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U157" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="K157" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="L157" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M157" s="1">
-        <v>1</v>
-      </c>
-      <c r="N157" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="O157" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="P157" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q157" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="R157" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S157" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U157" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="V157" s="2">
         <v>15.398300000000001</v>
@@ -12396,10 +12381,10 @@
         <v>18</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H158" s="1" t="s">
         <v>27</v>
@@ -12408,37 +12393,37 @@
         <v>4</v>
       </c>
       <c r="J158" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="K158" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="L158" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M158" s="1">
+        <v>1</v>
+      </c>
+      <c r="N158" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="O158" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="P158" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q158" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="R158" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S158" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U158" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="L158" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M158" s="1">
-        <v>1</v>
-      </c>
-      <c r="N158" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="O158" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="P158" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q158" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="R158" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S158" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U158" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="V158" s="2">
         <v>15.398300000000001</v>
@@ -12464,10 +12449,10 @@
         <v>18</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H159" s="1" t="s">
         <v>27</v>
@@ -12476,10 +12461,10 @@
         <v>4</v>
       </c>
       <c r="J159" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="K159" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="L159" s="1" t="s">
         <v>30</v>
@@ -12488,25 +12473,25 @@
         <v>1</v>
       </c>
       <c r="N159" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="O159" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="P159" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q159" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="R159" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S159" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U159" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="O159" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="P159" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q159" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="R159" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S159" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U159" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="V159" s="2">
         <v>15.399100000000001</v>
@@ -12532,10 +12517,10 @@
         <v>18</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>27</v>
@@ -12544,10 +12529,10 @@
         <v>4</v>
       </c>
       <c r="J160" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="L160" s="1" t="s">
         <v>30</v>
@@ -12556,25 +12541,25 @@
         <v>1</v>
       </c>
       <c r="N160" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="O160" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P160" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q160" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="R160" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S160" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U160" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="R160" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S160" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U160" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="V160" s="2">
         <v>15.3992</v>
@@ -12600,10 +12585,10 @@
         <v>18</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H161" s="1" t="s">
         <v>27</v>
@@ -12612,10 +12597,10 @@
         <v>4</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="K161" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="L161" s="1" t="s">
         <v>30</v>
@@ -12624,16 +12609,16 @@
         <v>1</v>
       </c>
       <c r="N161" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="O161" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P161" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q161" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="R161" s="1" t="s">
         <v>34</v>
@@ -12668,10 +12653,10 @@
         <v>18</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H162" s="1" t="s">
         <v>27</v>
@@ -12680,10 +12665,10 @@
         <v>4</v>
       </c>
       <c r="J162" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="K162" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="L162" s="1" t="s">
         <v>30</v>
@@ -12692,16 +12677,16 @@
         <v>1</v>
       </c>
       <c r="N162" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="O162" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P162" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q162" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="R162" s="1" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-05-2020 16-21-45
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{219918D1-A8A7-4D78-A6E1-F82584E74BA3}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2587EF8E-A057-4063-8073-3B097A435799}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="211">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -453,19 +453,10 @@
     <t>Farmacia GMT</t>
   </si>
   <si>
-    <t>Rivera Ortiz</t>
-  </si>
-  <si>
-    <t>Punto Farma Kennedy</t>
-  </si>
-  <si>
-    <t>Jehova</t>
-  </si>
-  <si>
-    <t>Farmacia Farmacity</t>
-  </si>
-  <si>
-    <t>Farma City</t>
+    <t>Farmacia Rivera Ortiz</t>
+  </si>
+  <si>
+    <t>Farmacia Jehova</t>
   </si>
   <si>
     <t>Farmacia Santa Ana</t>
@@ -474,13 +465,7 @@
     <t>Farmacia El Doctorcito</t>
   </si>
   <si>
-    <t>Editoreal Oceano</t>
-  </si>
-  <si>
-    <t>Farmacia el Doctorcito</t>
-  </si>
-  <si>
-    <t>Laboratorios Medicos</t>
+    <t>Laboratorios Médicos</t>
   </si>
   <si>
     <t>Farmacia Medifarma</t>
@@ -1655,8 +1640,8 @@
   <dimension ref="A1:W162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="O74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U80" sqref="U80"/>
+      <pane ySplit="1" topLeftCell="N98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U108" sqref="U108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -7527,7 +7512,7 @@
         <v>35</v>
       </c>
       <c r="U86" s="1" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="V86" s="2">
         <v>15.3123</v>
@@ -7663,7 +7648,7 @@
         <v>35</v>
       </c>
       <c r="U88" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="V88" s="2">
         <v>15.314</v>
@@ -7731,7 +7716,7 @@
         <v>35</v>
       </c>
       <c r="U89" s="1" t="s">
-        <v>142</v>
+        <v>105</v>
       </c>
       <c r="V89" s="2">
         <v>15.314299999999999</v>
@@ -7867,7 +7852,7 @@
         <v>35</v>
       </c>
       <c r="U91" s="1" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="V91" s="2">
         <v>14.8527</v>
@@ -8547,7 +8532,7 @@
         <v>35</v>
       </c>
       <c r="U101" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="V101" s="2">
         <v>13.5337</v>
@@ -8615,7 +8600,7 @@
         <v>35</v>
       </c>
       <c r="U102" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="V102" s="2">
         <v>13.280799999999999</v>
@@ -8683,7 +8668,7 @@
         <v>35</v>
       </c>
       <c r="U103" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="V103" s="2">
         <v>13.2742</v>
@@ -8751,7 +8736,7 @@
         <v>35</v>
       </c>
       <c r="U104" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="V104" s="2">
         <v>13.285</v>
@@ -8819,7 +8804,7 @@
         <v>35</v>
       </c>
       <c r="U105" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="V105" s="2">
         <v>13.3597</v>
@@ -8955,7 +8940,7 @@
         <v>35</v>
       </c>
       <c r="U107" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="V107" s="2">
         <v>13.268700000000001</v>
@@ -9023,7 +9008,7 @@
         <v>35</v>
       </c>
       <c r="U108" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="V108" s="2">
         <v>13.251200000000001</v>
@@ -9091,7 +9076,7 @@
         <v>35</v>
       </c>
       <c r="U109" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="V109" s="2">
         <v>13.254</v>
@@ -9703,7 +9688,7 @@
         <v>35</v>
       </c>
       <c r="U118" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="V118" s="2">
         <v>13.4314</v>
@@ -9771,7 +9756,7 @@
         <v>35</v>
       </c>
       <c r="U119" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="V119" s="2">
         <v>13.4329</v>
@@ -10043,7 +10028,7 @@
         <v>35</v>
       </c>
       <c r="U123" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="V123" s="2">
         <v>13.4544</v>
@@ -10111,7 +10096,7 @@
         <v>35</v>
       </c>
       <c r="U124" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="V124" s="2">
         <v>13.4565</v>
@@ -10179,7 +10164,7 @@
         <v>35</v>
       </c>
       <c r="U125" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="V125" s="2">
         <v>15.132300000000001</v>
@@ -10383,7 +10368,7 @@
         <v>35</v>
       </c>
       <c r="U128" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="V128" s="2">
         <v>15.5343</v>
@@ -10451,7 +10436,7 @@
         <v>35</v>
       </c>
       <c r="U129" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="V129" s="2">
         <v>15.5352</v>
@@ -10519,7 +10504,7 @@
         <v>35</v>
       </c>
       <c r="U130" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="V130" s="2">
         <v>15.536099999999999</v>
@@ -10655,7 +10640,7 @@
         <v>35</v>
       </c>
       <c r="U132" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="V132" s="2">
         <v>15.543200000000001</v>
@@ -10723,7 +10708,7 @@
         <v>35</v>
       </c>
       <c r="U133" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="V133" s="2">
         <v>15.543200000000001</v>
@@ -10897,10 +10882,10 @@
         <v>6</v>
       </c>
       <c r="J136" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K136" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="L136" s="1" t="s">
         <v>30</v>
@@ -10909,16 +10894,16 @@
         <v>1</v>
       </c>
       <c r="N136" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="O136" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="P136" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q136" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="R136" s="1" t="s">
         <v>34</v>
@@ -10927,7 +10912,7 @@
         <v>35</v>
       </c>
       <c r="U136" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="V136" s="2">
         <v>15.55</v>
@@ -10965,37 +10950,37 @@
         <v>6</v>
       </c>
       <c r="J137" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L137" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M137" s="1">
+        <v>1</v>
+      </c>
+      <c r="N137" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O137" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="P137" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q137" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="R137" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S137" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U137" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="K137" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L137" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M137" s="1">
-        <v>1</v>
-      </c>
-      <c r="N137" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="O137" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="P137" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q137" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="R137" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S137" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U137" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="V137" s="2">
         <v>15.550800000000001</v>
@@ -11033,10 +11018,10 @@
         <v>6</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K138" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="L138" s="1" t="s">
         <v>30</v>
@@ -11045,16 +11030,16 @@
         <v>1</v>
       </c>
       <c r="N138" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="O138" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="P138" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q138" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="R138" s="1" t="s">
         <v>34</v>
@@ -11089,10 +11074,10 @@
         <v>10</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H139" s="1" t="s">
         <v>27</v>
@@ -11101,10 +11086,10 @@
         <v>7</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="K139" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="L139" s="1" t="s">
         <v>30</v>
@@ -11113,16 +11098,16 @@
         <v>1</v>
       </c>
       <c r="N139" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="O139" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="P139" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q139" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="R139" s="1" t="s">
         <v>34</v>
@@ -11157,10 +11142,10 @@
         <v>10</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H140" s="1" t="s">
         <v>27</v>
@@ -11169,10 +11154,10 @@
         <v>7</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="K140" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="L140" s="1" t="s">
         <v>30</v>
@@ -11181,16 +11166,16 @@
         <v>1</v>
       </c>
       <c r="N140" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="O140" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="P140" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q140" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="R140" s="1" t="s">
         <v>34</v>
@@ -11199,7 +11184,7 @@
         <v>35</v>
       </c>
       <c r="U140" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="V140" s="2">
         <v>15.382999999999999</v>
@@ -11225,10 +11210,10 @@
         <v>10</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H141" s="1" t="s">
         <v>27</v>
@@ -11237,10 +11222,10 @@
         <v>7</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="K141" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="L141" s="1" t="s">
         <v>30</v>
@@ -11249,16 +11234,16 @@
         <v>1</v>
       </c>
       <c r="N141" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="O141" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="P141" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q141" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="R141" s="1" t="s">
         <v>34</v>
@@ -11293,10 +11278,10 @@
         <v>10</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H142" s="1" t="s">
         <v>27</v>
@@ -11305,10 +11290,10 @@
         <v>7</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="L142" s="1" t="s">
         <v>30</v>
@@ -11317,16 +11302,16 @@
         <v>1</v>
       </c>
       <c r="N142" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="O142" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="P142" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q142" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="R142" s="1" t="s">
         <v>34</v>
@@ -11361,10 +11346,10 @@
         <v>10</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H143" s="1" t="s">
         <v>27</v>
@@ -11373,37 +11358,37 @@
         <v>7</v>
       </c>
       <c r="J143" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K143" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L143" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M143" s="1">
+        <v>1</v>
+      </c>
+      <c r="N143" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="O143" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="P143" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q143" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R143" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S143" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U143" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="K143" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="L143" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M143" s="1">
-        <v>1</v>
-      </c>
-      <c r="N143" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="O143" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="P143" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q143" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="R143" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S143" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U143" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="V143" s="2">
         <v>15.388400000000001</v>
@@ -11429,49 +11414,49 @@
         <v>11</v>
       </c>
       <c r="F144" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H144" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I144" s="1">
+        <v>1</v>
+      </c>
+      <c r="J144" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K144" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="L144" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M144" s="1">
+        <v>1</v>
+      </c>
+      <c r="N144" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="O144" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="P144" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q144" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G144" s="1" t="s">
+      <c r="R144" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S144" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U144" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="H144" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I144" s="1">
-        <v>1</v>
-      </c>
-      <c r="J144" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="K144" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="L144" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M144" s="1">
-        <v>1</v>
-      </c>
-      <c r="N144" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="O144" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="P144" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q144" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="R144" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S144" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U144" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="V144" s="2">
         <v>15.3889</v>
@@ -11497,10 +11482,10 @@
         <v>11</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H145" s="1" t="s">
         <v>27</v>
@@ -11509,10 +11494,10 @@
         <v>2</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="L145" s="1" t="s">
         <v>30</v>
@@ -11521,16 +11506,16 @@
         <v>1</v>
       </c>
       <c r="N145" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="O145" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="P145" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q145" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="R145" s="1" t="s">
         <v>34</v>
@@ -11539,7 +11524,7 @@
         <v>35</v>
       </c>
       <c r="U145" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="V145" s="2">
         <v>15.393000000000001</v>
@@ -11565,10 +11550,10 @@
         <v>12</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>27</v>
@@ -11577,10 +11562,10 @@
         <v>17</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="K146" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="L146" s="1" t="s">
         <v>30</v>
@@ -11589,16 +11574,16 @@
         <v>7</v>
       </c>
       <c r="N146" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="O146" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="P146" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q146" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="R146" s="1" t="s">
         <v>34</v>
@@ -11633,49 +11618,49 @@
         <v>13</v>
       </c>
       <c r="F147" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H147" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I147" s="1">
+        <v>1</v>
+      </c>
+      <c r="J147" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K147" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="L147" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M147" s="1">
+        <v>1</v>
+      </c>
+      <c r="N147" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="O147" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="P147" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q147" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G147" s="1" t="s">
+      <c r="R147" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S147" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U147" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="H147" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I147" s="1">
-        <v>1</v>
-      </c>
-      <c r="J147" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="K147" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="L147" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M147" s="1">
-        <v>1</v>
-      </c>
-      <c r="N147" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O147" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="P147" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q147" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R147" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S147" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U147" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="V147" s="2">
         <v>15.393599999999999</v>
@@ -11701,49 +11686,49 @@
         <v>13</v>
       </c>
       <c r="F148" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H148" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I148" s="1">
+        <v>1</v>
+      </c>
+      <c r="J148" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K148" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="L148" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M148" s="1">
+        <v>1</v>
+      </c>
+      <c r="N148" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="O148" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="P148" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q148" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G148" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H148" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I148" s="1">
-        <v>1</v>
-      </c>
-      <c r="J148" s="1" t="s">
+      <c r="R148" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S148" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U148" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="K148" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="L148" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M148" s="1">
-        <v>1</v>
-      </c>
-      <c r="N148" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O148" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="P148" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q148" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R148" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S148" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U148" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="V148" s="2">
         <v>15.395200000000001</v>
@@ -11769,49 +11754,49 @@
         <v>13</v>
       </c>
       <c r="F149" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H149" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I149" s="1">
+        <v>1</v>
+      </c>
+      <c r="J149" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K149" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="L149" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M149" s="1">
+        <v>1</v>
+      </c>
+      <c r="N149" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="O149" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="P149" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q149" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G149" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H149" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I149" s="1">
-        <v>1</v>
-      </c>
-      <c r="J149" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="K149" s="1" t="s">
+      <c r="R149" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S149" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U149" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="L149" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M149" s="1">
-        <v>1</v>
-      </c>
-      <c r="N149" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O149" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="P149" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q149" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R149" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S149" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U149" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="V149" s="2">
         <v>15.3955</v>
@@ -11837,49 +11822,49 @@
         <v>13</v>
       </c>
       <c r="F150" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H150" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I150" s="1">
+        <v>1</v>
+      </c>
+      <c r="J150" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K150" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="L150" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M150" s="1">
+        <v>1</v>
+      </c>
+      <c r="N150" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="O150" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="P150" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q150" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G150" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H150" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I150" s="1">
-        <v>1</v>
-      </c>
-      <c r="J150" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="K150" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="L150" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M150" s="1">
-        <v>1</v>
-      </c>
-      <c r="N150" s="1" t="s">
+      <c r="R150" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S150" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U150" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="O150" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="P150" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q150" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R150" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S150" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U150" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="V150" s="2">
         <v>15.3956</v>
@@ -11905,49 +11890,49 @@
         <v>13</v>
       </c>
       <c r="F151" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H151" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I151" s="1">
+        <v>1</v>
+      </c>
+      <c r="J151" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K151" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="L151" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M151" s="1">
+        <v>1</v>
+      </c>
+      <c r="N151" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="O151" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="P151" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q151" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G151" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H151" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I151" s="1">
-        <v>1</v>
-      </c>
-      <c r="J151" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="K151" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="L151" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M151" s="1">
-        <v>1</v>
-      </c>
-      <c r="N151" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O151" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="P151" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q151" s="1" t="s">
+      <c r="R151" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S151" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U151" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="R151" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S151" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U151" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="V151" s="2">
         <v>15.3956</v>
@@ -11973,10 +11958,10 @@
         <v>18</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H152" s="1" t="s">
         <v>27</v>
@@ -11985,10 +11970,10 @@
         <v>4</v>
       </c>
       <c r="J152" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="K152" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L152" s="1" t="s">
         <v>30</v>
@@ -11997,16 +11982,16 @@
         <v>1</v>
       </c>
       <c r="N152" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O152" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="P152" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q152" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="R152" s="1" t="s">
         <v>34</v>
@@ -12041,10 +12026,10 @@
         <v>18</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H153" s="1" t="s">
         <v>27</v>
@@ -12053,10 +12038,10 @@
         <v>4</v>
       </c>
       <c r="J153" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="K153" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L153" s="1" t="s">
         <v>30</v>
@@ -12065,16 +12050,16 @@
         <v>1</v>
       </c>
       <c r="N153" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O153" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="P153" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q153" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="R153" s="1" t="s">
         <v>34</v>
@@ -12109,10 +12094,10 @@
         <v>18</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H154" s="1" t="s">
         <v>27</v>
@@ -12121,10 +12106,10 @@
         <v>4</v>
       </c>
       <c r="J154" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="K154" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L154" s="1" t="s">
         <v>30</v>
@@ -12133,16 +12118,16 @@
         <v>1</v>
       </c>
       <c r="N154" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O154" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="P154" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q154" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="R154" s="1" t="s">
         <v>34</v>
@@ -12177,10 +12162,10 @@
         <v>18</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H155" s="1" t="s">
         <v>27</v>
@@ -12189,10 +12174,10 @@
         <v>4</v>
       </c>
       <c r="J155" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="K155" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L155" s="1" t="s">
         <v>30</v>
@@ -12201,16 +12186,16 @@
         <v>1</v>
       </c>
       <c r="N155" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O155" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="P155" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q155" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="R155" s="1" t="s">
         <v>34</v>
@@ -12245,10 +12230,10 @@
         <v>18</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H156" s="1" t="s">
         <v>27</v>
@@ -12257,10 +12242,10 @@
         <v>4</v>
       </c>
       <c r="J156" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="K156" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L156" s="1" t="s">
         <v>30</v>
@@ -12269,16 +12254,16 @@
         <v>1</v>
       </c>
       <c r="N156" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O156" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="P156" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q156" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="R156" s="1" t="s">
         <v>34</v>
@@ -12287,7 +12272,7 @@
         <v>35</v>
       </c>
       <c r="U156" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="V156" s="2">
         <v>15.398199999999999</v>
@@ -12313,10 +12298,10 @@
         <v>18</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H157" s="1" t="s">
         <v>27</v>
@@ -12325,37 +12310,37 @@
         <v>4</v>
       </c>
       <c r="J157" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="K157" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="L157" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M157" s="1">
+        <v>1</v>
+      </c>
+      <c r="N157" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="O157" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P157" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q157" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="R157" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S157" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U157" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="K157" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="L157" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M157" s="1">
-        <v>1</v>
-      </c>
-      <c r="N157" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="O157" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="P157" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q157" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="R157" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S157" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U157" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="V157" s="2">
         <v>15.398300000000001</v>
@@ -12381,10 +12366,10 @@
         <v>18</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H158" s="1" t="s">
         <v>27</v>
@@ -12393,37 +12378,37 @@
         <v>4</v>
       </c>
       <c r="J158" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="K158" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="L158" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M158" s="1">
+        <v>1</v>
+      </c>
+      <c r="N158" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="O158" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P158" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q158" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="R158" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S158" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U158" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="L158" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M158" s="1">
-        <v>1</v>
-      </c>
-      <c r="N158" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="O158" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="P158" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q158" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="R158" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S158" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U158" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="V158" s="2">
         <v>15.398300000000001</v>
@@ -12449,10 +12434,10 @@
         <v>18</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H159" s="1" t="s">
         <v>27</v>
@@ -12461,10 +12446,10 @@
         <v>4</v>
       </c>
       <c r="J159" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="K159" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L159" s="1" t="s">
         <v>30</v>
@@ -12473,25 +12458,25 @@
         <v>1</v>
       </c>
       <c r="N159" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="O159" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P159" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q159" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="R159" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S159" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U159" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="O159" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="P159" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q159" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="R159" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S159" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U159" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="V159" s="2">
         <v>15.399100000000001</v>
@@ -12517,10 +12502,10 @@
         <v>18</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>27</v>
@@ -12529,10 +12514,10 @@
         <v>4</v>
       </c>
       <c r="J160" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L160" s="1" t="s">
         <v>30</v>
@@ -12541,25 +12526,25 @@
         <v>1</v>
       </c>
       <c r="N160" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O160" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="P160" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q160" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="R160" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S160" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U160" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="R160" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S160" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U160" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="V160" s="2">
         <v>15.3992</v>
@@ -12585,10 +12570,10 @@
         <v>18</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H161" s="1" t="s">
         <v>27</v>
@@ -12597,10 +12582,10 @@
         <v>4</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="K161" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L161" s="1" t="s">
         <v>30</v>
@@ -12609,16 +12594,16 @@
         <v>1</v>
       </c>
       <c r="N161" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O161" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="P161" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q161" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="R161" s="1" t="s">
         <v>34</v>
@@ -12653,10 +12638,10 @@
         <v>18</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H162" s="1" t="s">
         <v>27</v>
@@ -12665,10 +12650,10 @@
         <v>4</v>
       </c>
       <c r="J162" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="K162" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L162" s="1" t="s">
         <v>30</v>
@@ -12677,16 +12662,16 @@
         <v>1</v>
       </c>
       <c r="N162" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O162" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="P162" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q162" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="R162" s="1" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-05-2020 16-38-53
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2587EF8E-A057-4063-8073-3B097A435799}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00961105-4754-42CE-BC05-0FAD7F4569E2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="203">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -471,7 +471,7 @@
     <t>Farmacia Medifarma</t>
   </si>
   <si>
-    <t>America</t>
+    <t>Farmacia America</t>
   </si>
   <si>
     <t>Farmacia Alpha</t>
@@ -483,10 +483,7 @@
     <t>Farmacia Versalles</t>
   </si>
   <si>
-    <t>Farmacia Bio Pharma-E</t>
-  </si>
-  <si>
-    <t>Farmacia Salman</t>
+    <t>Bio Pharma</t>
   </si>
   <si>
     <t>Farmacia Omega</t>
@@ -495,9 +492,6 @@
     <t>Farmacia Divel</t>
   </si>
   <si>
-    <t>Pharmaster</t>
-  </si>
-  <si>
     <t>Farmacias Pharmaster</t>
   </si>
   <si>
@@ -519,9 +513,6 @@
     <t>Farmacias Sandra</t>
   </si>
   <si>
-    <t>Farmacity Guaimaca</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -621,12 +612,6 @@
     <t>HND-1301</t>
   </si>
   <si>
-    <t>Farmacia Alessandra 2</t>
-  </si>
-  <si>
-    <t>Medifarma</t>
-  </si>
-  <si>
     <t>Farmacia Alessandra</t>
   </si>
   <si>
@@ -652,15 +637,6 @@
   </si>
   <si>
     <t>HND-1804</t>
-  </si>
-  <si>
-    <t>San Antonio</t>
-  </si>
-  <si>
-    <t>Farmacia San Antonio #1</t>
-  </si>
-  <si>
-    <t>San Antonio #1</t>
   </si>
   <si>
     <t>Farmacia San Carlos</t>
@@ -812,7 +788,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -992,6 +968,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1153,7 +1135,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1161,6 +1143,7 @@
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1640,8 +1623,8 @@
   <dimension ref="A1:W162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="N98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U108" sqref="U108"/>
+      <pane ySplit="1" topLeftCell="N138" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W148" sqref="W148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -2003,7 +1986,7 @@
       <c r="S5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="7" t="s">
         <v>39</v>
       </c>
       <c r="V5" s="2">
@@ -10096,7 +10079,7 @@
         <v>35</v>
       </c>
       <c r="U124" s="1" t="s">
-        <v>150</v>
+        <v>37</v>
       </c>
       <c r="V124" s="2">
         <v>13.4565</v>
@@ -10368,7 +10351,7 @@
         <v>35</v>
       </c>
       <c r="U128" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V128" s="2">
         <v>15.5343</v>
@@ -10436,7 +10419,7 @@
         <v>35</v>
       </c>
       <c r="U129" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="V129" s="2">
         <v>15.5352</v>
@@ -10504,7 +10487,7 @@
         <v>35</v>
       </c>
       <c r="U130" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="V130" s="2">
         <v>15.536099999999999</v>
@@ -10640,7 +10623,7 @@
         <v>35</v>
       </c>
       <c r="U132" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="V132" s="2">
         <v>15.543200000000001</v>
@@ -10708,7 +10691,7 @@
         <v>35</v>
       </c>
       <c r="U133" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="V133" s="2">
         <v>15.543200000000001</v>
@@ -10882,37 +10865,37 @@
         <v>6</v>
       </c>
       <c r="J136" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K136" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L136" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M136" s="1">
+        <v>1</v>
+      </c>
+      <c r="N136" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K136" s="1" t="s">
+      <c r="O136" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="P136" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q136" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="L136" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M136" s="1">
-        <v>1</v>
-      </c>
-      <c r="N136" s="1" t="s">
+      <c r="R136" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S136" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U136" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="O136" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="P136" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q136" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="R136" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S136" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U136" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="V136" s="2">
         <v>15.55</v>
@@ -10950,29 +10933,29 @@
         <v>6</v>
       </c>
       <c r="J137" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L137" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M137" s="1">
+        <v>1</v>
+      </c>
+      <c r="N137" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K137" s="1" t="s">
+      <c r="O137" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="P137" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q137" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="L137" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M137" s="1">
-        <v>1</v>
-      </c>
-      <c r="N137" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="O137" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="P137" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q137" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="R137" s="1" t="s">
         <v>34</v>
       </c>
@@ -10980,7 +10963,7 @@
         <v>35</v>
       </c>
       <c r="U137" s="1" t="s">
-        <v>161</v>
+        <v>105</v>
       </c>
       <c r="V137" s="2">
         <v>15.550800000000001</v>
@@ -11018,28 +11001,28 @@
         <v>6</v>
       </c>
       <c r="J138" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K138" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L138" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M138" s="1">
+        <v>1</v>
+      </c>
+      <c r="N138" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K138" s="1" t="s">
+      <c r="O138" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="P138" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q138" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="L138" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M138" s="1">
-        <v>1</v>
-      </c>
-      <c r="N138" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="O138" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="P138" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q138" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="R138" s="1" t="s">
         <v>34</v>
@@ -11074,10 +11057,10 @@
         <v>10</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H139" s="1" t="s">
         <v>27</v>
@@ -11086,28 +11069,28 @@
         <v>7</v>
       </c>
       <c r="J139" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K139" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L139" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M139" s="1">
+        <v>1</v>
+      </c>
+      <c r="N139" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O139" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P139" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q139" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="K139" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="L139" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M139" s="1">
-        <v>1</v>
-      </c>
-      <c r="N139" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="O139" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="P139" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q139" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="R139" s="1" t="s">
         <v>34</v>
@@ -11142,10 +11125,10 @@
         <v>10</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H140" s="1" t="s">
         <v>27</v>
@@ -11154,37 +11137,37 @@
         <v>7</v>
       </c>
       <c r="J140" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K140" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L140" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M140" s="1">
+        <v>1</v>
+      </c>
+      <c r="N140" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O140" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P140" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q140" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K140" s="1" t="s">
+      <c r="R140" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S140" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U140" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="L140" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M140" s="1">
-        <v>1</v>
-      </c>
-      <c r="N140" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="O140" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="P140" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q140" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="R140" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S140" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U140" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="V140" s="2">
         <v>15.382999999999999</v>
@@ -11210,10 +11193,10 @@
         <v>10</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H141" s="1" t="s">
         <v>27</v>
@@ -11222,28 +11205,28 @@
         <v>7</v>
       </c>
       <c r="J141" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K141" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L141" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M141" s="1">
+        <v>1</v>
+      </c>
+      <c r="N141" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O141" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P141" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q141" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="K141" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="L141" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M141" s="1">
-        <v>1</v>
-      </c>
-      <c r="N141" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="O141" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="P141" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q141" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="R141" s="1" t="s">
         <v>34</v>
@@ -11278,10 +11261,10 @@
         <v>10</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H142" s="1" t="s">
         <v>27</v>
@@ -11290,28 +11273,28 @@
         <v>7</v>
       </c>
       <c r="J142" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K142" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L142" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M142" s="1">
+        <v>1</v>
+      </c>
+      <c r="N142" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O142" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P142" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q142" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="K142" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="L142" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M142" s="1">
-        <v>1</v>
-      </c>
-      <c r="N142" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="O142" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="P142" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q142" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="R142" s="1" t="s">
         <v>34</v>
@@ -11346,10 +11329,10 @@
         <v>10</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H143" s="1" t="s">
         <v>27</v>
@@ -11358,37 +11341,37 @@
         <v>7</v>
       </c>
       <c r="J143" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K143" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L143" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M143" s="1">
+        <v>1</v>
+      </c>
+      <c r="N143" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O143" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P143" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q143" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K143" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="L143" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M143" s="1">
-        <v>1</v>
-      </c>
-      <c r="N143" s="1" t="s">
+      <c r="R143" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S143" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U143" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="O143" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="P143" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q143" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="R143" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S143" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U143" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="V143" s="2">
         <v>15.388400000000001</v>
@@ -11414,49 +11397,49 @@
         <v>11</v>
       </c>
       <c r="F144" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H144" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I144" s="1">
+        <v>1</v>
+      </c>
+      <c r="J144" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="K144" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="G144" s="1" t="s">
+      <c r="L144" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M144" s="1">
+        <v>1</v>
+      </c>
+      <c r="N144" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H144" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I144" s="1">
-        <v>1</v>
-      </c>
-      <c r="J144" s="1" t="s">
+      <c r="O144" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="P144" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q144" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="K144" s="1" t="s">
+      <c r="R144" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S144" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U144" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="L144" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M144" s="1">
-        <v>1</v>
-      </c>
-      <c r="N144" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="O144" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="P144" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q144" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="R144" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S144" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U144" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="V144" s="2">
         <v>15.3889</v>
@@ -11482,10 +11465,10 @@
         <v>11</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H145" s="1" t="s">
         <v>27</v>
@@ -11494,37 +11477,37 @@
         <v>2</v>
       </c>
       <c r="J145" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="K145" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L145" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M145" s="1">
+        <v>1</v>
+      </c>
+      <c r="N145" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="O145" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="P145" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q145" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="K145" s="1" t="s">
+      <c r="R145" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S145" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U145" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="L145" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M145" s="1">
-        <v>1</v>
-      </c>
-      <c r="N145" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="O145" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="P145" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q145" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="R145" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S145" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U145" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="V145" s="2">
         <v>15.393000000000001</v>
@@ -11550,10 +11533,10 @@
         <v>12</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>27</v>
@@ -11562,10 +11545,10 @@
         <v>17</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K146" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="L146" s="1" t="s">
         <v>30</v>
@@ -11574,16 +11557,16 @@
         <v>7</v>
       </c>
       <c r="N146" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="O146" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="P146" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q146" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="R146" s="1" t="s">
         <v>34</v>
@@ -11591,7 +11574,7 @@
       <c r="S146" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U146" s="1" t="s">
+      <c r="U146" s="7" t="s">
         <v>39</v>
       </c>
       <c r="V146" s="2">
@@ -11618,49 +11601,49 @@
         <v>13</v>
       </c>
       <c r="F147" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H147" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I147" s="1">
+        <v>1</v>
+      </c>
+      <c r="J147" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K147" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G147" s="1" t="s">
+      <c r="L147" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M147" s="1">
+        <v>1</v>
+      </c>
+      <c r="N147" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="H147" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I147" s="1">
-        <v>1</v>
-      </c>
-      <c r="J147" s="1" t="s">
+      <c r="O147" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P147" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q147" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="K147" s="1" t="s">
+      <c r="R147" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S147" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U147" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="L147" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M147" s="1">
-        <v>1</v>
-      </c>
-      <c r="N147" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="O147" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="P147" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q147" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="R147" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S147" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U147" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="V147" s="2">
         <v>15.393599999999999</v>
@@ -11686,41 +11669,41 @@
         <v>13</v>
       </c>
       <c r="F148" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H148" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I148" s="1">
+        <v>1</v>
+      </c>
+      <c r="J148" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K148" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G148" s="1" t="s">
+      <c r="L148" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M148" s="1">
+        <v>1</v>
+      </c>
+      <c r="N148" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="H148" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I148" s="1">
-        <v>1</v>
-      </c>
-      <c r="J148" s="1" t="s">
+      <c r="O148" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P148" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q148" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="K148" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="L148" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M148" s="1">
-        <v>1</v>
-      </c>
-      <c r="N148" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="O148" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="P148" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q148" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="R148" s="1" t="s">
         <v>34</v>
       </c>
@@ -11728,7 +11711,7 @@
         <v>35</v>
       </c>
       <c r="U148" s="1" t="s">
-        <v>196</v>
+        <v>144</v>
       </c>
       <c r="V148" s="2">
         <v>15.395200000000001</v>
@@ -11754,49 +11737,49 @@
         <v>13</v>
       </c>
       <c r="F149" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H149" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I149" s="1">
+        <v>1</v>
+      </c>
+      <c r="J149" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K149" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G149" s="1" t="s">
+      <c r="L149" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M149" s="1">
+        <v>1</v>
+      </c>
+      <c r="N149" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="H149" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I149" s="1">
-        <v>1</v>
-      </c>
-      <c r="J149" s="1" t="s">
+      <c r="O149" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P149" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q149" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="K149" s="1" t="s">
+      <c r="R149" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S149" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U149" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="L149" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M149" s="1">
-        <v>1</v>
-      </c>
-      <c r="N149" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="O149" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="P149" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q149" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="R149" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S149" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U149" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="V149" s="2">
         <v>15.3955</v>
@@ -11822,49 +11805,49 @@
         <v>13</v>
       </c>
       <c r="F150" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H150" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I150" s="1">
+        <v>1</v>
+      </c>
+      <c r="J150" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K150" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G150" s="1" t="s">
+      <c r="L150" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M150" s="1">
+        <v>1</v>
+      </c>
+      <c r="N150" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="H150" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I150" s="1">
-        <v>1</v>
-      </c>
-      <c r="J150" s="1" t="s">
+      <c r="O150" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P150" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q150" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="K150" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="L150" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M150" s="1">
-        <v>1</v>
-      </c>
-      <c r="N150" s="1" t="s">
+      <c r="R150" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S150" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U150" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="O150" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="P150" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q150" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="R150" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S150" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U150" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="V150" s="2">
         <v>15.3956</v>
@@ -11890,49 +11873,49 @@
         <v>13</v>
       </c>
       <c r="F151" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H151" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I151" s="1">
+        <v>1</v>
+      </c>
+      <c r="J151" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K151" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G151" s="1" t="s">
+      <c r="L151" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M151" s="1">
+        <v>1</v>
+      </c>
+      <c r="N151" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="H151" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I151" s="1">
-        <v>1</v>
-      </c>
-      <c r="J151" s="1" t="s">
+      <c r="O151" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P151" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q151" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="K151" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="L151" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M151" s="1">
-        <v>1</v>
-      </c>
-      <c r="N151" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="O151" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="P151" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q151" s="1" t="s">
+      <c r="R151" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S151" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U151" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="R151" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S151" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U151" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="V151" s="2">
         <v>15.3956</v>
@@ -11958,10 +11941,10 @@
         <v>18</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H152" s="1" t="s">
         <v>27</v>
@@ -11970,10 +11953,10 @@
         <v>4</v>
       </c>
       <c r="J152" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K152" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L152" s="1" t="s">
         <v>30</v>
@@ -11982,16 +11965,16 @@
         <v>1</v>
       </c>
       <c r="N152" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="O152" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="P152" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q152" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="R152" s="1" t="s">
         <v>34</v>
@@ -12026,10 +12009,10 @@
         <v>18</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H153" s="1" t="s">
         <v>27</v>
@@ -12038,10 +12021,10 @@
         <v>4</v>
       </c>
       <c r="J153" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K153" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L153" s="1" t="s">
         <v>30</v>
@@ -12050,16 +12033,16 @@
         <v>1</v>
       </c>
       <c r="N153" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="O153" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="P153" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q153" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="R153" s="1" t="s">
         <v>34</v>
@@ -12094,10 +12077,10 @@
         <v>18</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H154" s="1" t="s">
         <v>27</v>
@@ -12106,10 +12089,10 @@
         <v>4</v>
       </c>
       <c r="J154" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K154" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L154" s="1" t="s">
         <v>30</v>
@@ -12118,16 +12101,16 @@
         <v>1</v>
       </c>
       <c r="N154" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="O154" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="P154" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q154" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="R154" s="1" t="s">
         <v>34</v>
@@ -12162,10 +12145,10 @@
         <v>18</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H155" s="1" t="s">
         <v>27</v>
@@ -12174,10 +12157,10 @@
         <v>4</v>
       </c>
       <c r="J155" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K155" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L155" s="1" t="s">
         <v>30</v>
@@ -12186,16 +12169,16 @@
         <v>1</v>
       </c>
       <c r="N155" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="O155" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="P155" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q155" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="R155" s="1" t="s">
         <v>34</v>
@@ -12230,10 +12213,10 @@
         <v>18</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H156" s="1" t="s">
         <v>27</v>
@@ -12242,10 +12225,10 @@
         <v>4</v>
       </c>
       <c r="J156" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K156" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L156" s="1" t="s">
         <v>30</v>
@@ -12254,16 +12237,16 @@
         <v>1</v>
       </c>
       <c r="N156" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="O156" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="P156" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q156" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="R156" s="1" t="s">
         <v>34</v>
@@ -12272,7 +12255,7 @@
         <v>35</v>
       </c>
       <c r="U156" s="1" t="s">
-        <v>206</v>
+        <v>103</v>
       </c>
       <c r="V156" s="2">
         <v>15.398199999999999</v>
@@ -12298,10 +12281,10 @@
         <v>18</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H157" s="1" t="s">
         <v>27</v>
@@ -12310,10 +12293,10 @@
         <v>4</v>
       </c>
       <c r="J157" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K157" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L157" s="1" t="s">
         <v>30</v>
@@ -12322,16 +12305,16 @@
         <v>1</v>
       </c>
       <c r="N157" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="O157" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="P157" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q157" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="R157" s="1" t="s">
         <v>34</v>
@@ -12340,7 +12323,7 @@
         <v>35</v>
       </c>
       <c r="U157" s="1" t="s">
-        <v>207</v>
+        <v>103</v>
       </c>
       <c r="V157" s="2">
         <v>15.398300000000001</v>
@@ -12366,10 +12349,10 @@
         <v>18</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H158" s="1" t="s">
         <v>27</v>
@@ -12378,10 +12361,10 @@
         <v>4</v>
       </c>
       <c r="J158" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K158" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L158" s="1" t="s">
         <v>30</v>
@@ -12390,16 +12373,16 @@
         <v>1</v>
       </c>
       <c r="N158" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="O158" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="P158" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q158" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="R158" s="1" t="s">
         <v>34</v>
@@ -12408,7 +12391,7 @@
         <v>35</v>
       </c>
       <c r="U158" s="1" t="s">
-        <v>208</v>
+        <v>103</v>
       </c>
       <c r="V158" s="2">
         <v>15.398300000000001</v>
@@ -12434,10 +12417,10 @@
         <v>18</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H159" s="1" t="s">
         <v>27</v>
@@ -12446,10 +12429,10 @@
         <v>4</v>
       </c>
       <c r="J159" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K159" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L159" s="1" t="s">
         <v>30</v>
@@ -12458,16 +12441,16 @@
         <v>1</v>
       </c>
       <c r="N159" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="O159" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="P159" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q159" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="R159" s="1" t="s">
         <v>34</v>
@@ -12476,7 +12459,7 @@
         <v>35</v>
       </c>
       <c r="U159" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="V159" s="2">
         <v>15.399100000000001</v>
@@ -12502,10 +12485,10 @@
         <v>18</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>27</v>
@@ -12514,37 +12497,37 @@
         <v>4</v>
       </c>
       <c r="J160" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K160" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="L160" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M160" s="1">
+        <v>1</v>
+      </c>
+      <c r="N160" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O160" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P160" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q160" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="R160" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S160" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U160" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="K160" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="L160" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M160" s="1">
-        <v>1</v>
-      </c>
-      <c r="N160" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="O160" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="P160" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q160" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="R160" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S160" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U160" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="V160" s="2">
         <v>15.3992</v>
@@ -12570,10 +12553,10 @@
         <v>18</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H161" s="1" t="s">
         <v>27</v>
@@ -12582,10 +12565,10 @@
         <v>4</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K161" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L161" s="1" t="s">
         <v>30</v>
@@ -12594,16 +12577,16 @@
         <v>1</v>
       </c>
       <c r="N161" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="O161" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="P161" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q161" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="R161" s="1" t="s">
         <v>34</v>
@@ -12638,10 +12621,10 @@
         <v>18</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H162" s="1" t="s">
         <v>27</v>
@@ -12650,10 +12633,10 @@
         <v>4</v>
       </c>
       <c r="J162" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K162" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L162" s="1" t="s">
         <v>30</v>
@@ -12662,16 +12645,16 @@
         <v>1</v>
       </c>
       <c r="N162" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="O162" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="P162" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q162" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="R162" s="1" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-05-2020 20-59-20
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00961105-4754-42CE-BC05-0FAD7F4569E2}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{15344633-F86A-4A39-87F2-70BA326B4232}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1623,8 +1623,8 @@
   <dimension ref="A1:W162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="N138" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W148" sqref="W148"/>
+      <pane ySplit="1" topLeftCell="N144" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X147" sqref="X147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-19-2020 17-04-57
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -1626,8 +1626,8 @@
   <dimension ref="A1:W162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="T12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W22" sqref="W22"/>
+      <pane ySplit="1" topLeftCell="O2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-19-2020 18-12-45
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F83CAD7E-D42F-4826-8299-7A10BD477BF9}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{099C6D1D-A6DD-495C-963E-DB8EBAF5DF82}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1626,8 +1626,8 @@
   <dimension ref="A1:W162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="O2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W5" sqref="W5"/>
+      <pane ySplit="1" topLeftCell="S3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -1789,10 +1789,10 @@
         <v>36</v>
       </c>
       <c r="V2" s="2">
-        <v>14.5923</v>
+        <v>15.5989</v>
       </c>
       <c r="W2" s="2">
-        <v>-88.5822</v>
+        <v>-87.208799999999997</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -1857,10 +1857,10 @@
         <v>37</v>
       </c>
       <c r="V3" s="2">
-        <v>14.5924</v>
+        <v>15.7836</v>
       </c>
       <c r="W3" s="2">
-        <v>-88.582700000000003</v>
+        <v>-86.792500000000004</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -1925,10 +1925,10 @@
         <v>38</v>
       </c>
       <c r="V4" s="2">
-        <v>14.594900000000001</v>
+        <v>15.784800000000001</v>
       </c>
       <c r="W4" s="2">
-        <v>-88.581699999999998</v>
+        <v>-86.792900000000003</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -1993,10 +1993,10 @@
         <v>39</v>
       </c>
       <c r="V5" s="2">
-        <v>14.5952</v>
+        <v>15.7849</v>
       </c>
       <c r="W5" s="2">
-        <v>-88.581599999999995</v>
+        <v>-86.791899999999998</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -2061,10 +2061,10 @@
         <v>45</v>
       </c>
       <c r="V6" s="2">
-        <v>14.547599999999999</v>
+        <v>15.5989</v>
       </c>
       <c r="W6" s="2">
-        <v>-88.669700000000006</v>
+        <v>-87.208799999999997</v>
       </c>
     </row>
     <row r="7" spans="1:23">
@@ -2129,7 +2129,7 @@
         <v>46</v>
       </c>
       <c r="V7" s="2">
-        <v>14.550800000000001</v>
+        <v>15.599</v>
       </c>
       <c r="W7" s="2">
         <v>-88.659800000000004</v>
@@ -2197,10 +2197,10 @@
         <v>51</v>
       </c>
       <c r="V8" s="2">
-        <v>14.6058</v>
+        <v>15.7738</v>
       </c>
       <c r="W8" s="2">
-        <v>-88.583200000000005</v>
+        <v>-87.475499999999997</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -2265,10 +2265,10 @@
         <v>52</v>
       </c>
       <c r="V9" s="2">
-        <v>14.4788</v>
+        <v>15.7744</v>
       </c>
       <c r="W9" s="2">
-        <v>-88.595200000000006</v>
+        <v>-87.446799999999996</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -2333,10 +2333,10 @@
         <v>53</v>
       </c>
       <c r="V10" s="2">
-        <v>14.4823</v>
+        <v>15.781700000000001</v>
       </c>
       <c r="W10" s="2">
-        <v>-88.591300000000004</v>
+        <v>-87.453400000000002</v>
       </c>
     </row>
     <row r="11" spans="1:23">
@@ -2401,10 +2401,10 @@
         <v>54</v>
       </c>
       <c r="V11" s="2">
-        <v>14.806699999999999</v>
+        <v>15.783300000000001</v>
       </c>
       <c r="W11" s="2">
-        <v>-88.415999999999997</v>
+        <v>-87.452100000000002</v>
       </c>
     </row>
     <row r="12" spans="1:23">
@@ -2469,10 +2469,10 @@
         <v>37</v>
       </c>
       <c r="V12" s="2">
-        <v>14.809799999999999</v>
+        <v>15.7834</v>
       </c>
       <c r="W12" s="2">
-        <v>-88.410499999999999</v>
+        <v>-87.449399999999997</v>
       </c>
     </row>
     <row r="13" spans="1:23">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-20-2020 15-08-48
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="169" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{099C6D1D-A6DD-495C-963E-DB8EBAF5DF82}"/>
+  <xr:revisionPtr revIDLastSave="476" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BBFBB4FF-40AE-482C-91A4-7AC0A7377D76}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="203">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -571,9 +571,6 @@
   </si>
   <si>
     <t>HND-1102</t>
-  </si>
-  <si>
-    <t>pharmacy</t>
   </si>
   <si>
     <t>12</t>
@@ -655,7 +652,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -786,6 +783,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1138,7 +1143,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1147,6 +1152,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1623,11 +1629,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W162"/>
+  <dimension ref="A1:AA162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="S3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
+      <pane ySplit="1" topLeftCell="S137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA147" sqref="AA147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -2537,10 +2543,10 @@
         <v>55</v>
       </c>
       <c r="V13" s="2">
-        <v>14.8119</v>
+        <v>15.783899999999999</v>
       </c>
       <c r="W13" s="2">
-        <v>-88.41</v>
+        <v>-87.449700000000007</v>
       </c>
     </row>
     <row r="14" spans="1:23">
@@ -2605,10 +2611,10 @@
         <v>37</v>
       </c>
       <c r="V14" s="2">
-        <v>14.8123</v>
+        <v>15.7841</v>
       </c>
       <c r="W14" s="2">
-        <v>-88.409099999999995</v>
+        <v>-87.450699999999998</v>
       </c>
     </row>
     <row r="15" spans="1:23">
@@ -2673,10 +2679,10 @@
         <v>56</v>
       </c>
       <c r="V15" s="2">
-        <v>14.8123</v>
+        <v>15.7845</v>
       </c>
       <c r="W15" s="2">
-        <v>-88.411100000000005</v>
+        <v>-87.451599999999999</v>
       </c>
     </row>
     <row r="16" spans="1:23">
@@ -2741,10 +2747,10 @@
         <v>62</v>
       </c>
       <c r="V16" s="2">
-        <v>14.8126</v>
+        <v>14.447100000000001</v>
       </c>
       <c r="W16" s="2">
-        <v>-88.408600000000007</v>
+        <v>-87.633300000000006</v>
       </c>
     </row>
     <row r="17" spans="1:23">
@@ -2809,10 +2815,10 @@
         <v>36</v>
       </c>
       <c r="V17" s="2">
-        <v>14.8131</v>
+        <v>14.4542</v>
       </c>
       <c r="W17" s="2">
-        <v>-88.410700000000006</v>
+        <v>-87.643900000000002</v>
       </c>
     </row>
     <row r="18" spans="1:23">
@@ -2877,10 +2883,10 @@
         <v>62</v>
       </c>
       <c r="V18" s="2">
-        <v>14.813499999999999</v>
+        <v>14.454499999999999</v>
       </c>
       <c r="W18" s="2">
-        <v>-88.409599999999998</v>
+        <v>-87.643500000000003</v>
       </c>
     </row>
     <row r="19" spans="1:23">
@@ -2945,10 +2951,10 @@
         <v>63</v>
       </c>
       <c r="V19" s="2">
-        <v>14.8431</v>
+        <v>14.4549</v>
       </c>
       <c r="W19" s="2">
-        <v>-88.456699999999998</v>
+        <v>-87.639200000000002</v>
       </c>
     </row>
     <row r="20" spans="1:23">
@@ -3013,10 +3019,10 @@
         <v>64</v>
       </c>
       <c r="V20" s="2">
-        <v>14.8437</v>
+        <v>14.4573</v>
       </c>
       <c r="W20" s="2">
-        <v>-88.458200000000005</v>
+        <v>-87.642300000000006</v>
       </c>
     </row>
     <row r="21" spans="1:23">
@@ -3081,10 +3087,10 @@
         <v>64</v>
       </c>
       <c r="V21" s="2">
-        <v>14.0588</v>
+        <v>14.458</v>
       </c>
       <c r="W21" s="2">
-        <v>-88.6922</v>
+        <v>-87.640900000000002</v>
       </c>
     </row>
     <row r="22" spans="1:23">
@@ -3149,10 +3155,10 @@
         <v>37</v>
       </c>
       <c r="V22" s="2">
-        <v>14.7813</v>
+        <v>14.596399999999999</v>
       </c>
       <c r="W22" s="2">
-        <v>-88.585999999999999</v>
+        <v>-87.831199999999995</v>
       </c>
     </row>
     <row r="23" spans="1:23">
@@ -3217,10 +3223,10 @@
         <v>69</v>
       </c>
       <c r="V23" s="2">
-        <v>14.599460000000001</v>
+        <v>14.596500000000001</v>
       </c>
       <c r="W23" s="2">
-        <v>-87.843118000000004</v>
+        <v>-87.832300000000004</v>
       </c>
     </row>
     <row r="24" spans="1:23">
@@ -3285,10 +3291,10 @@
         <v>37</v>
       </c>
       <c r="V24" s="2">
-        <v>14.433299999999999</v>
+        <v>14.598699999999999</v>
       </c>
       <c r="W24" s="2">
-        <v>-89.182699999999997</v>
+        <v>-87.831400000000002</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -3353,10 +3359,10 @@
         <v>51</v>
       </c>
       <c r="V25" s="2">
-        <v>14.4337</v>
+        <v>14.767799999999999</v>
       </c>
       <c r="W25" s="2">
-        <v>-89.180400000000006</v>
+        <v>-88.779300000000006</v>
       </c>
     </row>
     <row r="26" spans="1:23">
@@ -3421,10 +3427,10 @@
         <v>62</v>
       </c>
       <c r="V26" s="2">
-        <v>14.433999999999999</v>
+        <v>14.7681</v>
       </c>
       <c r="W26" s="2">
-        <v>-89.183000000000007</v>
+        <v>-88.777600000000007</v>
       </c>
     </row>
     <row r="27" spans="1:23">
@@ -3489,10 +3495,10 @@
         <v>62</v>
       </c>
       <c r="V27" s="2">
-        <v>14.434699999999999</v>
+        <v>14.7681</v>
       </c>
       <c r="W27" s="2">
-        <v>-89.183300000000003</v>
+        <v>-88.777500000000003</v>
       </c>
     </row>
     <row r="28" spans="1:23">
@@ -3557,10 +3563,10 @@
         <v>80</v>
       </c>
       <c r="V28" s="2">
-        <v>14.434699999999999</v>
+        <v>14.832100000000001</v>
       </c>
       <c r="W28" s="2">
-        <v>-89.183000000000007</v>
+        <v>-89094</v>
       </c>
     </row>
     <row r="29" spans="1:23">
@@ -3625,10 +3631,10 @@
         <v>85</v>
       </c>
       <c r="V29" s="2">
-        <v>14.4351</v>
+        <v>14.8384</v>
       </c>
       <c r="W29" s="2">
-        <v>-89.183700000000002</v>
+        <v>-89.1554</v>
       </c>
     </row>
     <row r="30" spans="1:23">
@@ -3693,10 +3699,10 @@
         <v>36</v>
       </c>
       <c r="V30" s="2">
-        <v>14.4352</v>
+        <v>15.065799999999999</v>
       </c>
       <c r="W30" s="2">
-        <v>-89.182699999999997</v>
+        <v>-88.747100000000003</v>
       </c>
     </row>
     <row r="31" spans="1:23">
@@ -3761,10 +3767,10 @@
         <v>37</v>
       </c>
       <c r="V31" s="2">
-        <v>14.4352</v>
+        <v>15.477399999999999</v>
       </c>
       <c r="W31" s="2">
-        <v>-89.182000000000002</v>
+        <v>-87.985699999999994</v>
       </c>
     </row>
     <row r="32" spans="1:23">
@@ -3829,10 +3835,10 @@
         <v>62</v>
       </c>
       <c r="V32" s="2">
-        <v>14.4354</v>
+        <v>15.4787</v>
       </c>
       <c r="W32" s="2">
-        <v>-89.183000000000007</v>
+        <v>-87.975099999999998</v>
       </c>
     </row>
     <row r="33" spans="1:23">
@@ -3897,10 +3903,10 @@
         <v>97</v>
       </c>
       <c r="V33" s="2">
-        <v>14.435600000000001</v>
+        <v>15.4796</v>
       </c>
       <c r="W33" s="2">
-        <v>-89.182100000000005</v>
+        <v>-88.011200000000002</v>
       </c>
     </row>
     <row r="34" spans="1:23">
@@ -3965,10 +3971,10 @@
         <v>55</v>
       </c>
       <c r="V34" s="2">
-        <v>14.435600000000001</v>
+        <v>15.4854</v>
       </c>
       <c r="W34" s="2">
-        <v>-89.183599999999998</v>
+        <v>-88.034099999999995</v>
       </c>
     </row>
     <row r="35" spans="1:23">
@@ -4033,10 +4039,10 @@
         <v>98</v>
       </c>
       <c r="V35" s="2">
-        <v>14.436</v>
+        <v>15.4855</v>
       </c>
       <c r="W35" s="2">
-        <v>-89.182100000000005</v>
+        <v>-87.984399999999994</v>
       </c>
     </row>
     <row r="36" spans="1:23">
@@ -4101,10 +4107,10 @@
         <v>99</v>
       </c>
       <c r="V36" s="2">
-        <v>14.436299999999999</v>
+        <v>15.489800000000001</v>
       </c>
       <c r="W36" s="2">
-        <v>-89.182299999999998</v>
+        <v>-87.986000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:23">
@@ -4169,10 +4175,10 @@
         <v>100</v>
       </c>
       <c r="V37" s="2">
-        <v>14.4368</v>
+        <v>15.492599999999999</v>
       </c>
       <c r="W37" s="2">
-        <v>-89.182900000000004</v>
+        <v>-88.011499999999998</v>
       </c>
     </row>
     <row r="38" spans="1:23">
@@ -4237,10 +4243,10 @@
         <v>37</v>
       </c>
       <c r="V38" s="2">
-        <v>14.4369</v>
+        <v>15.492699999999999</v>
       </c>
       <c r="W38" s="2">
-        <v>-89.182900000000004</v>
+        <v>-88.016499999999994</v>
       </c>
     </row>
     <row r="39" spans="1:23">
@@ -4305,10 +4311,10 @@
         <v>37</v>
       </c>
       <c r="V39" s="2">
-        <v>14.4369</v>
+        <v>15.4933</v>
       </c>
       <c r="W39" s="2">
-        <v>-89.1828</v>
+        <v>-87.986500000000007</v>
       </c>
     </row>
     <row r="40" spans="1:23">
@@ -4373,10 +4379,10 @@
         <v>37</v>
       </c>
       <c r="V40" s="2">
-        <v>14.437099999999999</v>
+        <v>15.493399999999999</v>
       </c>
       <c r="W40" s="2">
-        <v>-89.182400000000001</v>
+        <v>-87.984800000000007</v>
       </c>
     </row>
     <row r="41" spans="1:23">
@@ -4441,10 +4447,10 @@
         <v>37</v>
       </c>
       <c r="V41" s="2">
-        <v>14.438000000000001</v>
+        <v>15.493600000000001</v>
       </c>
       <c r="W41" s="2">
-        <v>-89.182299999999998</v>
+        <v>-87.984099999999998</v>
       </c>
     </row>
     <row r="42" spans="1:23">
@@ -4509,10 +4515,10 @@
         <v>36</v>
       </c>
       <c r="V42" s="2">
-        <v>14.438000000000001</v>
+        <v>15.494300000000001</v>
       </c>
       <c r="W42" s="2">
-        <v>-89.182100000000005</v>
+        <v>-88.034099999999995</v>
       </c>
     </row>
     <row r="43" spans="1:23">
@@ -4577,10 +4583,10 @@
         <v>101</v>
       </c>
       <c r="V43" s="2">
-        <v>14.438499999999999</v>
+        <v>15.499700000000001</v>
       </c>
       <c r="W43" s="2">
-        <v>-89.183300000000003</v>
+        <v>-88.025000000000006</v>
       </c>
     </row>
     <row r="44" spans="1:23">
@@ -4645,10 +4651,10 @@
         <v>102</v>
       </c>
       <c r="V44" s="2">
-        <v>14.3742</v>
+        <v>15.4999</v>
       </c>
       <c r="W44" s="2">
-        <v>-89.209400000000002</v>
+        <v>-88.037499999999994</v>
       </c>
     </row>
     <row r="45" spans="1:23">
@@ -4713,10 +4719,10 @@
         <v>103</v>
       </c>
       <c r="V45" s="2">
-        <v>14.3748</v>
+        <v>15.5</v>
       </c>
       <c r="W45" s="2">
-        <v>-89.209299999999999</v>
+        <v>-88.020700000000005</v>
       </c>
     </row>
     <row r="46" spans="1:23">
@@ -4781,10 +4787,10 @@
         <v>37</v>
       </c>
       <c r="V46" s="2">
-        <v>14.3749</v>
+        <v>15.500299999999999</v>
       </c>
       <c r="W46" s="2">
-        <v>-89.209400000000002</v>
+        <v>-88.038399999999996</v>
       </c>
     </row>
     <row r="47" spans="1:23">
@@ -4849,10 +4855,10 @@
         <v>104</v>
       </c>
       <c r="V47" s="2">
-        <v>14.3788</v>
+        <v>15.501799999999999</v>
       </c>
       <c r="W47" s="2">
-        <v>-89.128399999999999</v>
+        <v>-88.027100000000004</v>
       </c>
     </row>
     <row r="48" spans="1:23">
@@ -4917,10 +4923,10 @@
         <v>62</v>
       </c>
       <c r="V48" s="2">
-        <v>14.380699999999999</v>
+        <v>15.504099999999999</v>
       </c>
       <c r="W48" s="2">
-        <v>-89.130899999999997</v>
+        <v>-88.014200000000002</v>
       </c>
     </row>
     <row r="49" spans="1:23">
@@ -4985,10 +4991,10 @@
         <v>105</v>
       </c>
       <c r="V49" s="2">
-        <v>14.4985</v>
+        <v>15.505100000000001</v>
       </c>
       <c r="W49" s="2">
-        <v>-88.753500000000003</v>
+        <v>-88.022300000000001</v>
       </c>
     </row>
     <row r="50" spans="1:23">
@@ -5053,10 +5059,10 @@
         <v>106</v>
       </c>
       <c r="V50" s="2">
-        <v>14.5349</v>
+        <v>15.5061</v>
       </c>
       <c r="W50" s="2">
-        <v>-89.279399999999995</v>
+        <v>-88.027199999999993</v>
       </c>
     </row>
     <row r="51" spans="1:23">
@@ -5121,10 +5127,10 @@
         <v>63</v>
       </c>
       <c r="V51" s="2">
-        <v>14.4854</v>
+        <v>15.5105</v>
       </c>
       <c r="W51" s="2">
-        <v>-88.978999999999999</v>
+        <v>-88.012699999999995</v>
       </c>
     </row>
     <row r="52" spans="1:23">
@@ -5189,10 +5195,10 @@
         <v>37</v>
       </c>
       <c r="V52" s="2">
-        <v>14.658099999999999</v>
+        <v>15.5124</v>
       </c>
       <c r="W52" s="2">
-        <v>-86.214799999999997</v>
+        <v>-88.037000000000006</v>
       </c>
     </row>
     <row r="53" spans="1:23">
@@ -5257,10 +5263,10 @@
         <v>62</v>
       </c>
       <c r="V53" s="2">
-        <v>14.662800000000001</v>
+        <v>15.5146</v>
       </c>
       <c r="W53" s="2">
-        <v>-86.216300000000004</v>
+        <v>-88.033600000000007</v>
       </c>
     </row>
     <row r="54" spans="1:23">
@@ -5325,10 +5331,10 @@
         <v>37</v>
       </c>
       <c r="V54" s="2">
-        <v>14.664300000000001</v>
+        <v>15.5159</v>
       </c>
       <c r="W54" s="2">
-        <v>-86.2166</v>
+        <v>-88.028400000000005</v>
       </c>
     </row>
     <row r="55" spans="1:23">
@@ -5393,10 +5399,10 @@
         <v>36</v>
       </c>
       <c r="V55" s="2">
-        <v>14.664300000000001</v>
+        <v>15.5244</v>
       </c>
       <c r="W55" s="2">
-        <v>-86.216300000000004</v>
+        <v>-88.038499999999999</v>
       </c>
     </row>
     <row r="56" spans="1:23">
@@ -5461,10 +5467,10 @@
         <v>107</v>
       </c>
       <c r="V56" s="2">
-        <v>14.664999999999999</v>
+        <v>15.5298</v>
       </c>
       <c r="W56" s="2">
-        <v>-86.215699999999998</v>
+        <v>-88.032700000000006</v>
       </c>
     </row>
     <row r="57" spans="1:23">
@@ -5529,10 +5535,10 @@
         <v>37</v>
       </c>
       <c r="V57" s="2">
-        <v>14.670400000000001</v>
+        <v>15.5299</v>
       </c>
       <c r="W57" s="2">
-        <v>-86.218900000000005</v>
+        <v>-88.026499999999999</v>
       </c>
     </row>
     <row r="58" spans="1:23">
@@ -5597,10 +5603,10 @@
         <v>36</v>
       </c>
       <c r="V58" s="2">
-        <v>14.6706</v>
+        <v>15.5299</v>
       </c>
       <c r="W58" s="2">
-        <v>-86.222300000000004</v>
+        <v>-88.025499999999994</v>
       </c>
     </row>
     <row r="59" spans="1:23">
@@ -5665,10 +5671,10 @@
         <v>36</v>
       </c>
       <c r="V59" s="2">
-        <v>14.6706</v>
+        <v>15.5306</v>
       </c>
       <c r="W59" s="2">
-        <v>-86.221199999999996</v>
+        <v>-88.029399999999995</v>
       </c>
     </row>
     <row r="60" spans="1:23">
@@ -5733,10 +5739,10 @@
         <v>37</v>
       </c>
       <c r="V60" s="2">
-        <v>14.6767</v>
+        <v>15.5341</v>
       </c>
       <c r="W60" s="2">
-        <v>-86.205299999999994</v>
+        <v>-88.019300000000001</v>
       </c>
     </row>
     <row r="61" spans="1:23">
@@ -5801,10 +5807,10 @@
         <v>36</v>
       </c>
       <c r="V61" s="2">
-        <v>14.7057</v>
+        <v>15.537100000000001</v>
       </c>
       <c r="W61" s="2">
-        <v>-86.167599999999993</v>
+        <v>-88.014899999999997</v>
       </c>
     </row>
     <row r="62" spans="1:23">
@@ -5869,10 +5875,10 @@
         <v>37</v>
       </c>
       <c r="V62" s="2">
-        <v>14.6373</v>
+        <v>15.542899999999999</v>
       </c>
       <c r="W62" s="2">
-        <v>-86.219200000000001</v>
+        <v>-88.023099999999999</v>
       </c>
     </row>
     <row r="63" spans="1:23">
@@ -5937,10 +5943,10 @@
         <v>37</v>
       </c>
       <c r="V63" s="2">
-        <v>14.7018</v>
+        <v>15.549099999999999</v>
       </c>
       <c r="W63" s="2">
-        <v>-86.034400000000005</v>
+        <v>-88.035899999999998</v>
       </c>
     </row>
     <row r="64" spans="1:23">
@@ -6005,10 +6011,10 @@
         <v>37</v>
       </c>
       <c r="V64" s="2">
-        <v>14.7232</v>
+        <v>15.5505</v>
       </c>
       <c r="W64" s="2">
-        <v>-86.138099999999994</v>
+        <v>-88.004800000000003</v>
       </c>
     </row>
     <row r="65" spans="1:23">
@@ -6073,10 +6079,10 @@
         <v>62</v>
       </c>
       <c r="V65" s="2">
-        <v>14.8385</v>
+        <v>15.6119</v>
       </c>
       <c r="W65" s="2">
-        <v>-85.882800000000003</v>
+        <v>-87.956299999999999</v>
       </c>
     </row>
     <row r="66" spans="1:23">
@@ -6141,10 +6147,10 @@
         <v>62</v>
       </c>
       <c r="V66" s="2">
-        <v>14.840999999999999</v>
+        <v>15.316800000000001</v>
       </c>
       <c r="W66" s="2">
-        <v>-85.904200000000003</v>
+        <v>-87.990300000000005</v>
       </c>
     </row>
     <row r="67" spans="1:23">
@@ -6209,10 +6215,10 @@
         <v>37</v>
       </c>
       <c r="V67" s="2">
-        <v>14.8454</v>
+        <v>15.4361</v>
       </c>
       <c r="W67" s="2">
-        <v>-85.900700000000001</v>
+        <v>-87.921099999999996</v>
       </c>
     </row>
     <row r="68" spans="1:23">
@@ -6277,10 +6283,10 @@
         <v>62</v>
       </c>
       <c r="V68" s="2">
-        <v>15.083600000000001</v>
+        <v>15.436500000000001</v>
       </c>
       <c r="W68" s="2">
-        <v>-85.558899999999994</v>
+        <v>-87.924300000000002</v>
       </c>
     </row>
     <row r="69" spans="1:23">
@@ -6345,10 +6351,10 @@
         <v>37</v>
       </c>
       <c r="V69" s="2">
-        <v>15.0847</v>
+        <v>15.438499999999999</v>
       </c>
       <c r="W69" s="2">
-        <v>-85.557900000000004</v>
+        <v>-87.926900000000003</v>
       </c>
     </row>
     <row r="70" spans="1:23">
@@ -6413,10 +6419,10 @@
         <v>120</v>
       </c>
       <c r="V70" s="2">
-        <v>15.030799999999999</v>
+        <v>15.4405</v>
       </c>
       <c r="W70" s="2">
-        <v>-86.068600000000004</v>
+        <v>-87.929100000000005</v>
       </c>
     </row>
     <row r="71" spans="1:23">
@@ -6481,10 +6487,10 @@
         <v>37</v>
       </c>
       <c r="V71" s="2">
-        <v>15.5166</v>
+        <v>13.309900000000001</v>
       </c>
       <c r="W71" s="2">
-        <v>-85.866600000000005</v>
+        <v>-87.179100000000005</v>
       </c>
     </row>
     <row r="72" spans="1:23">
@@ -6549,10 +6555,10 @@
         <v>37</v>
       </c>
       <c r="V72" s="2">
-        <v>15.518599999999999</v>
+        <v>13.3125</v>
       </c>
       <c r="W72" s="2">
-        <v>-85.873000000000005</v>
+        <v>-87.175299999999993</v>
       </c>
     </row>
     <row r="73" spans="1:23">
@@ -6617,10 +6623,10 @@
         <v>131</v>
       </c>
       <c r="V73" s="2">
-        <v>15.198499999999999</v>
+        <v>13.095800000000001</v>
       </c>
       <c r="W73" s="2">
-        <v>-85.772199999999998</v>
+        <v>-87.057100000000005</v>
       </c>
     </row>
     <row r="74" spans="1:23">
@@ -6685,10 +6691,10 @@
         <v>36</v>
       </c>
       <c r="V74" s="2">
-        <v>15.259399999999999</v>
+        <v>14.0412</v>
       </c>
       <c r="W74" s="2">
-        <v>-85.746200000000002</v>
+        <v>-87.232399999999998</v>
       </c>
     </row>
     <row r="75" spans="1:23">
@@ -6753,10 +6759,10 @@
         <v>55</v>
       </c>
       <c r="V75" s="2">
-        <v>14.869400000000001</v>
+        <v>14.0457</v>
       </c>
       <c r="W75" s="2">
-        <v>-86.183800000000005</v>
+        <v>-87.211399999999998</v>
       </c>
     </row>
     <row r="76" spans="1:23">
@@ -6821,10 +6827,10 @@
         <v>36</v>
       </c>
       <c r="V76" s="2">
-        <v>14.351000000000001</v>
+        <v>14.0543</v>
       </c>
       <c r="W76" s="2">
-        <v>-85.887799999999999</v>
+        <v>-87.2226</v>
       </c>
     </row>
     <row r="77" spans="1:23">
@@ -6889,10 +6895,10 @@
         <v>106</v>
       </c>
       <c r="V77" s="2">
-        <v>14.9177</v>
+        <v>14.055099999999999</v>
       </c>
       <c r="W77" s="2">
-        <v>-88.237200000000001</v>
+        <v>-87.222300000000004</v>
       </c>
     </row>
     <row r="78" spans="1:23">
@@ -6957,10 +6963,10 @@
         <v>107</v>
       </c>
       <c r="V78" s="2">
-        <v>14.920199999999999</v>
+        <v>14.055400000000001</v>
       </c>
       <c r="W78" s="2">
-        <v>-88.245099999999994</v>
+        <v>-87.222099999999998</v>
       </c>
     </row>
     <row r="79" spans="1:23">
@@ -7025,10 +7031,10 @@
         <v>37</v>
       </c>
       <c r="V79" s="2">
-        <v>14.9216</v>
+        <v>14.0558</v>
       </c>
       <c r="W79" s="2">
-        <v>-88.237200000000001</v>
+        <v>-87.229299999999995</v>
       </c>
     </row>
     <row r="80" spans="1:23">
@@ -7093,10 +7099,10 @@
         <v>138</v>
       </c>
       <c r="V80" s="2">
-        <v>14.923299999999999</v>
+        <v>14.0588</v>
       </c>
       <c r="W80" s="2">
-        <v>-88.244500000000002</v>
+        <v>-87.189599999999999</v>
       </c>
     </row>
     <row r="81" spans="1:23">
@@ -7161,10 +7167,10 @@
         <v>106</v>
       </c>
       <c r="V81" s="2">
-        <v>14.927899999999999</v>
+        <v>14.058999999999999</v>
       </c>
       <c r="W81" s="2">
-        <v>-88.236900000000006</v>
+        <v>-87.189400000000006</v>
       </c>
     </row>
     <row r="82" spans="1:23">
@@ -7229,10 +7235,10 @@
         <v>139</v>
       </c>
       <c r="V82" s="2">
-        <v>14.8439</v>
+        <v>14.059100000000001</v>
       </c>
       <c r="W82" s="2">
-        <v>-88.461799999999997</v>
+        <v>-87.220600000000005</v>
       </c>
     </row>
     <row r="83" spans="1:23">
@@ -7297,10 +7303,10 @@
         <v>36</v>
       </c>
       <c r="V83" s="2">
-        <v>15.2621</v>
+        <v>14.0601</v>
       </c>
       <c r="W83" s="2">
-        <v>-88.541700000000006</v>
+        <v>-83.400400000000005</v>
       </c>
     </row>
     <row r="84" spans="1:23">
@@ -7365,10 +7371,10 @@
         <v>140</v>
       </c>
       <c r="V84" s="2">
-        <v>15.2738</v>
+        <v>14.064</v>
       </c>
       <c r="W84" s="2">
-        <v>-88.282899999999998</v>
+        <v>-87.209599999999995</v>
       </c>
     </row>
     <row r="85" spans="1:23">
@@ -7433,10 +7439,10 @@
         <v>37</v>
       </c>
       <c r="V85" s="2">
-        <v>15.3117</v>
+        <v>14.0655</v>
       </c>
       <c r="W85" s="2">
-        <v>-88.439599999999999</v>
+        <v>-87.1785</v>
       </c>
     </row>
     <row r="86" spans="1:23">
@@ -7501,10 +7507,10 @@
         <v>107</v>
       </c>
       <c r="V86" s="2">
-        <v>15.3123</v>
+        <v>14.0655</v>
       </c>
       <c r="W86" s="2">
-        <v>-88.439700000000002</v>
+        <v>-87.179299999999998</v>
       </c>
     </row>
     <row r="87" spans="1:23">
@@ -7569,10 +7575,10 @@
         <v>107</v>
       </c>
       <c r="V87" s="2">
-        <v>15.3133</v>
+        <v>14.0655</v>
       </c>
       <c r="W87" s="2">
-        <v>-88.436899999999994</v>
+        <v>-87.179599999999994</v>
       </c>
     </row>
     <row r="88" spans="1:23">
@@ -7637,10 +7643,10 @@
         <v>141</v>
       </c>
       <c r="V88" s="2">
-        <v>15.314</v>
+        <v>14.0665</v>
       </c>
       <c r="W88" s="2">
-        <v>-88.440200000000004</v>
+        <v>-87.210700000000003</v>
       </c>
     </row>
     <row r="89" spans="1:23">
@@ -7705,10 +7711,10 @@
         <v>106</v>
       </c>
       <c r="V89" s="2">
-        <v>15.314299999999999</v>
+        <v>14.0692</v>
       </c>
       <c r="W89" s="2">
-        <v>-88.437200000000004</v>
+        <v>-87.185000000000002</v>
       </c>
     </row>
     <row r="90" spans="1:23">
@@ -7773,10 +7779,10 @@
         <v>37</v>
       </c>
       <c r="V90" s="2">
-        <v>15.371499999999999</v>
+        <v>14.081799999999999</v>
       </c>
       <c r="W90" s="2">
-        <v>-88.299599999999998</v>
+        <v>-87.209599999999995</v>
       </c>
     </row>
     <row r="91" spans="1:23">
@@ -7841,10 +7847,10 @@
         <v>106</v>
       </c>
       <c r="V91" s="2">
-        <v>14.8527</v>
+        <v>14.083399999999999</v>
       </c>
       <c r="W91" s="2">
-        <v>-88.419799999999995</v>
+        <v>-87.174999999999997</v>
       </c>
     </row>
     <row r="92" spans="1:23">
@@ -7909,10 +7915,10 @@
         <v>36</v>
       </c>
       <c r="V92" s="2">
-        <v>14.7552</v>
+        <v>14.0837</v>
       </c>
       <c r="W92" s="2">
-        <v>-88.114400000000003</v>
+        <v>-87.210099999999997</v>
       </c>
     </row>
     <row r="93" spans="1:23">
@@ -7977,10 +7983,10 @@
         <v>36</v>
       </c>
       <c r="V93" s="2">
-        <v>14.769399999999999</v>
+        <v>14.0844</v>
       </c>
       <c r="W93" s="2">
-        <v>-88.145799999999994</v>
+        <v>-87.182699999999997</v>
       </c>
     </row>
     <row r="94" spans="1:23">
@@ -8045,10 +8051,10 @@
         <v>37</v>
       </c>
       <c r="V94" s="2">
-        <v>15.1439</v>
+        <v>14.085000000000001</v>
       </c>
       <c r="W94" s="2">
-        <v>-88.234700000000004</v>
+        <v>-87.186999999999998</v>
       </c>
     </row>
     <row r="95" spans="1:23">
@@ -8113,10 +8119,10 @@
         <v>62</v>
       </c>
       <c r="V95" s="2">
-        <v>14.8727</v>
+        <v>14.085900000000001</v>
       </c>
       <c r="W95" s="2">
-        <v>-88.072199999999995</v>
+        <v>-87.174400000000006</v>
       </c>
     </row>
     <row r="96" spans="1:23">
@@ -8181,10 +8187,10 @@
         <v>51</v>
       </c>
       <c r="V96" s="2">
-        <v>13.5328</v>
+        <v>14.0869</v>
       </c>
       <c r="W96" s="2">
-        <v>-87.552300000000002</v>
+        <v>-87.184899999999999</v>
       </c>
     </row>
     <row r="97" spans="1:23">
@@ -8249,10 +8255,10 @@
         <v>36</v>
       </c>
       <c r="V97" s="2">
-        <v>13.378299999999999</v>
+        <v>14.088200000000001</v>
       </c>
       <c r="W97" s="2">
-        <v>-87.575900000000004</v>
+        <v>-87.183400000000006</v>
       </c>
     </row>
     <row r="98" spans="1:23">
@@ -8317,10 +8323,10 @@
         <v>36</v>
       </c>
       <c r="V98" s="2">
-        <v>13.4994</v>
+        <v>14.089600000000001</v>
       </c>
       <c r="W98" s="2">
-        <v>-87.442599999999999</v>
+        <v>-87.188500000000005</v>
       </c>
     </row>
     <row r="99" spans="1:23">
@@ -8385,10 +8391,10 @@
         <v>37</v>
       </c>
       <c r="V99" s="2">
-        <v>13.5281</v>
+        <v>14.09</v>
       </c>
       <c r="W99" s="2">
-        <v>-87.490200000000002</v>
+        <v>-87.206500000000005</v>
       </c>
     </row>
     <row r="100" spans="1:23">
@@ -8453,10 +8459,10 @@
         <v>106</v>
       </c>
       <c r="V100" s="2">
-        <v>13.532400000000001</v>
+        <v>14.090199999999999</v>
       </c>
       <c r="W100" s="2">
-        <v>-87.501300000000001</v>
+        <v>-87.197199999999995</v>
       </c>
     </row>
     <row r="101" spans="1:23">
@@ -8521,10 +8527,10 @@
         <v>142</v>
       </c>
       <c r="V101" s="2">
-        <v>13.5337</v>
+        <v>14.090400000000001</v>
       </c>
       <c r="W101" s="2">
-        <v>-87.496300000000005</v>
+        <v>-87.196799999999996</v>
       </c>
     </row>
     <row r="102" spans="1:23">
@@ -8589,10 +8595,10 @@
         <v>143</v>
       </c>
       <c r="V102" s="2">
-        <v>13.280799999999999</v>
+        <v>14.092599999999999</v>
       </c>
       <c r="W102" s="2">
-        <v>-87.655299999999997</v>
+        <v>-87.2393</v>
       </c>
     </row>
     <row r="103" spans="1:23">
@@ -8657,10 +8663,10 @@
         <v>143</v>
       </c>
       <c r="V103" s="2">
-        <v>13.2742</v>
+        <v>14.092700000000001</v>
       </c>
       <c r="W103" s="2">
-        <v>-87.613799999999998</v>
+        <v>-87.194100000000006</v>
       </c>
     </row>
     <row r="104" spans="1:23">
@@ -8725,10 +8731,10 @@
         <v>143</v>
       </c>
       <c r="V104" s="2">
-        <v>13.285</v>
+        <v>14.0928</v>
       </c>
       <c r="W104" s="2">
-        <v>-87.621499999999997</v>
+        <v>-87.218500000000006</v>
       </c>
     </row>
     <row r="105" spans="1:23">
@@ -8793,10 +8799,10 @@
         <v>144</v>
       </c>
       <c r="V105" s="2">
-        <v>13.3597</v>
+        <v>14.0947</v>
       </c>
       <c r="W105" s="2">
-        <v>-87.599599999999995</v>
+        <v>-87.1952</v>
       </c>
     </row>
     <row r="106" spans="1:23">
@@ -8861,10 +8867,10 @@
         <v>62</v>
       </c>
       <c r="V106" s="2">
-        <v>13.2681</v>
+        <v>14.095700000000001</v>
       </c>
       <c r="W106" s="2">
-        <v>-87.658199999999994</v>
+        <v>-87.182699999999997</v>
       </c>
     </row>
     <row r="107" spans="1:23">
@@ -8929,10 +8935,10 @@
         <v>145</v>
       </c>
       <c r="V107" s="2">
-        <v>13.268700000000001</v>
+        <v>14.095700000000001</v>
       </c>
       <c r="W107" s="2">
-        <v>-87.657600000000002</v>
+        <v>-87.211200000000005</v>
       </c>
     </row>
     <row r="108" spans="1:23">
@@ -8997,10 +9003,10 @@
         <v>146</v>
       </c>
       <c r="V108" s="2">
-        <v>13.251200000000001</v>
+        <v>14.097</v>
       </c>
       <c r="W108" s="2">
-        <v>-87.6511</v>
+        <v>-87.207499999999996</v>
       </c>
     </row>
     <row r="109" spans="1:23">
@@ -9065,10 +9071,10 @@
         <v>147</v>
       </c>
       <c r="V109" s="2">
-        <v>13.254</v>
+        <v>14.097</v>
       </c>
       <c r="W109" s="2">
-        <v>-87.649000000000001</v>
+        <v>-87.222499999999997</v>
       </c>
     </row>
     <row r="110" spans="1:23">
@@ -9133,10 +9139,10 @@
         <v>37</v>
       </c>
       <c r="V110" s="2">
-        <v>13.595599999999999</v>
+        <v>14.099600000000001</v>
       </c>
       <c r="W110" s="2">
-        <v>-87.761899999999997</v>
+        <v>-87.194500000000005</v>
       </c>
     </row>
     <row r="111" spans="1:23">
@@ -9201,10 +9207,10 @@
         <v>51</v>
       </c>
       <c r="V111" s="2">
-        <v>13.5961</v>
+        <v>14.0998</v>
       </c>
       <c r="W111" s="2">
-        <v>-87.764600000000002</v>
+        <v>-87.189599999999999</v>
       </c>
     </row>
     <row r="112" spans="1:23">
@@ -9269,10 +9275,10 @@
         <v>36</v>
       </c>
       <c r="V112" s="2">
-        <v>13.5962</v>
+        <v>14.0999</v>
       </c>
       <c r="W112" s="2">
-        <v>-87.764700000000005</v>
+        <v>-87.187100000000001</v>
       </c>
     </row>
     <row r="113" spans="1:23">
@@ -9337,10 +9343,10 @@
         <v>107</v>
       </c>
       <c r="V113" s="2">
-        <v>13.596299999999999</v>
+        <v>14.1004</v>
       </c>
       <c r="W113" s="2">
-        <v>-87.763400000000004</v>
+        <v>-87.208500000000001</v>
       </c>
     </row>
     <row r="114" spans="1:23">
@@ -9405,10 +9411,10 @@
         <v>37</v>
       </c>
       <c r="V114" s="2">
-        <v>13.593</v>
+        <v>14.1004</v>
       </c>
       <c r="W114" s="2">
-        <v>-87.750600000000006</v>
+        <v>-87.183999999999997</v>
       </c>
     </row>
     <row r="115" spans="1:23">
@@ -9473,10 +9479,10 @@
         <v>107</v>
       </c>
       <c r="V115" s="2">
-        <v>13.4175</v>
+        <v>14.1006</v>
       </c>
       <c r="W115" s="2">
-        <v>-87.448099999999997</v>
+        <v>-87.182199999999995</v>
       </c>
     </row>
     <row r="116" spans="1:23">
@@ -9541,10 +9547,10 @@
         <v>36</v>
       </c>
       <c r="V116" s="2">
-        <v>13.4191</v>
+        <v>14.1007</v>
       </c>
       <c r="W116" s="2">
-        <v>-87.448300000000003</v>
+        <v>-87.180599999999998</v>
       </c>
     </row>
     <row r="117" spans="1:23">
@@ -9609,10 +9615,10 @@
         <v>106</v>
       </c>
       <c r="V117" s="2">
-        <v>13.4306</v>
+        <v>14.1007</v>
       </c>
       <c r="W117" s="2">
-        <v>-87.4285</v>
+        <v>-87.183400000000006</v>
       </c>
     </row>
     <row r="118" spans="1:23">
@@ -9677,10 +9683,10 @@
         <v>148</v>
       </c>
       <c r="V118" s="2">
-        <v>13.4314</v>
+        <v>14.101000000000001</v>
       </c>
       <c r="W118" s="2">
-        <v>-87.449700000000007</v>
+        <v>-87.182699999999997</v>
       </c>
     </row>
     <row r="119" spans="1:23">
@@ -9745,10 +9751,10 @@
         <v>149</v>
       </c>
       <c r="V119" s="2">
-        <v>13.4329</v>
+        <v>14.1014</v>
       </c>
       <c r="W119" s="2">
-        <v>-87.450699999999998</v>
+        <v>-87.207800000000006</v>
       </c>
     </row>
     <row r="120" spans="1:23">
@@ -9813,10 +9819,10 @@
         <v>36</v>
       </c>
       <c r="V120" s="2">
-        <v>13.434200000000001</v>
+        <v>14.102600000000001</v>
       </c>
       <c r="W120" s="2">
-        <v>-87.427700000000002</v>
+        <v>-87.184799999999996</v>
       </c>
     </row>
     <row r="121" spans="1:23">
@@ -9881,10 +9887,10 @@
         <v>37</v>
       </c>
       <c r="V121" s="2">
-        <v>13.436299999999999</v>
+        <v>14.1028</v>
       </c>
       <c r="W121" s="2">
-        <v>-87.4512</v>
+        <v>-87.178899999999999</v>
       </c>
     </row>
     <row r="122" spans="1:23">
@@ -9949,10 +9955,10 @@
         <v>107</v>
       </c>
       <c r="V122" s="2">
-        <v>13.439500000000001</v>
+        <v>14.1029</v>
       </c>
       <c r="W122" s="2">
-        <v>-87.451400000000007</v>
+        <v>-87.196799999999996</v>
       </c>
     </row>
     <row r="123" spans="1:23">
@@ -10017,10 +10023,10 @@
         <v>150</v>
       </c>
       <c r="V123" s="2">
-        <v>13.4544</v>
+        <v>14.1043</v>
       </c>
       <c r="W123" s="2">
-        <v>-87.453800000000001</v>
+        <v>-87.198599999999999</v>
       </c>
     </row>
     <row r="124" spans="1:23">
@@ -10085,10 +10091,10 @@
         <v>37</v>
       </c>
       <c r="V124" s="2">
-        <v>13.4565</v>
+        <v>14.1045</v>
       </c>
       <c r="W124" s="2">
-        <v>-87.453800000000001</v>
+        <v>-87.199200000000005</v>
       </c>
     </row>
     <row r="125" spans="1:23">
@@ -10153,10 +10159,10 @@
         <v>143</v>
       </c>
       <c r="V125" s="2">
-        <v>15.132300000000001</v>
+        <v>14.1046</v>
       </c>
       <c r="W125" s="2">
-        <v>-87.130200000000002</v>
+        <v>-87.236400000000003</v>
       </c>
     </row>
     <row r="126" spans="1:23">
@@ -10221,10 +10227,10 @@
         <v>36</v>
       </c>
       <c r="V126" s="2">
-        <v>15.130599999999999</v>
+        <v>14.1052</v>
       </c>
       <c r="W126" s="2">
-        <v>-87.147199999999998</v>
+        <v>-87.205399999999997</v>
       </c>
     </row>
     <row r="127" spans="1:23">
@@ -10289,10 +10295,10 @@
         <v>37</v>
       </c>
       <c r="V127" s="2">
-        <v>15.5138</v>
+        <v>14.106299999999999</v>
       </c>
       <c r="W127" s="2">
-        <v>-87.6691</v>
+        <v>-87.204499999999996</v>
       </c>
     </row>
     <row r="128" spans="1:23">
@@ -10357,10 +10363,10 @@
         <v>151</v>
       </c>
       <c r="V128" s="2">
-        <v>15.5343</v>
+        <v>14.1065</v>
       </c>
       <c r="W128" s="2">
-        <v>-87.653300000000002</v>
+        <v>-87.205399999999997</v>
       </c>
     </row>
     <row r="129" spans="1:23">
@@ -10425,10 +10431,10 @@
         <v>152</v>
       </c>
       <c r="V129" s="2">
-        <v>15.5352</v>
+        <v>14.1067</v>
       </c>
       <c r="W129" s="2">
-        <v>-87.652600000000007</v>
+        <v>-87.206800000000001</v>
       </c>
     </row>
     <row r="130" spans="1:23">
@@ -10493,10 +10499,10 @@
         <v>153</v>
       </c>
       <c r="V130" s="2">
-        <v>15.536099999999999</v>
+        <v>14.1068</v>
       </c>
       <c r="W130" s="2">
-        <v>-87.653099999999995</v>
+        <v>-87.205799999999996</v>
       </c>
     </row>
     <row r="131" spans="1:23">
@@ -10561,10 +10567,10 @@
         <v>36</v>
       </c>
       <c r="V131" s="2">
-        <v>15.5425</v>
+        <v>14.107900000000001</v>
       </c>
       <c r="W131" s="2">
-        <v>-87.6524</v>
+        <v>-87.205299999999994</v>
       </c>
     </row>
     <row r="132" spans="1:23">
@@ -10629,10 +10635,10 @@
         <v>153</v>
       </c>
       <c r="V132" s="2">
-        <v>15.543200000000001</v>
+        <v>14.1082</v>
       </c>
       <c r="W132" s="2">
-        <v>-87.652199999999993</v>
+        <v>-87.2059</v>
       </c>
     </row>
     <row r="133" spans="1:23">
@@ -10697,10 +10703,10 @@
         <v>154</v>
       </c>
       <c r="V133" s="2">
-        <v>15.543200000000001</v>
+        <v>14.1089</v>
       </c>
       <c r="W133" s="2">
-        <v>-87.652199999999993</v>
+        <v>-87.2089</v>
       </c>
     </row>
     <row r="134" spans="1:23">
@@ -10765,10 +10771,10 @@
         <v>107</v>
       </c>
       <c r="V134" s="2">
-        <v>15.543200000000001</v>
+        <v>14.1137</v>
       </c>
       <c r="W134" s="2">
-        <v>-87.652199999999993</v>
+        <v>-87.193799999999996</v>
       </c>
     </row>
     <row r="135" spans="1:23">
@@ -10833,10 +10839,10 @@
         <v>37</v>
       </c>
       <c r="V135" s="2">
-        <v>15.549799999999999</v>
+        <v>14.1287</v>
       </c>
       <c r="W135" s="2">
-        <v>-87.651600000000002</v>
+        <v>-87.227800000000002</v>
       </c>
     </row>
     <row r="136" spans="1:23">
@@ -10901,10 +10907,10 @@
         <v>159</v>
       </c>
       <c r="V136" s="2">
-        <v>15.55</v>
+        <v>14.5402</v>
       </c>
       <c r="W136" s="2">
-        <v>-87.651600000000002</v>
+        <v>-86.831100000000006</v>
       </c>
     </row>
     <row r="137" spans="1:23">
@@ -10969,10 +10975,10 @@
         <v>106</v>
       </c>
       <c r="V137" s="2">
-        <v>15.550800000000001</v>
+        <v>14.541600000000001</v>
       </c>
       <c r="W137" s="2">
-        <v>-87.651399999999995</v>
+        <v>-86.830799999999996</v>
       </c>
     </row>
     <row r="138" spans="1:23">
@@ -11037,10 +11043,10 @@
         <v>55</v>
       </c>
       <c r="V138" s="2">
-        <v>15.552</v>
+        <v>14.5555</v>
       </c>
       <c r="W138" s="2">
-        <v>-87.651300000000006</v>
+        <v>-86.827200000000005</v>
       </c>
     </row>
     <row r="139" spans="1:23">
@@ -11105,10 +11111,10 @@
         <v>55</v>
       </c>
       <c r="V139" s="2">
-        <v>15.3794</v>
+        <v>14.4832</v>
       </c>
       <c r="W139" s="2">
-        <v>-87.807299999999998</v>
+        <v>-87.982100000000003</v>
       </c>
     </row>
     <row r="140" spans="1:23">
@@ -11173,10 +11179,10 @@
         <v>166</v>
       </c>
       <c r="V140" s="2">
-        <v>15.382999999999999</v>
+        <v>14.4839</v>
       </c>
       <c r="W140" s="2">
-        <v>-87.804599999999994</v>
+        <v>-87.982100000000003</v>
       </c>
     </row>
     <row r="141" spans="1:23">
@@ -11241,10 +11247,10 @@
         <v>106</v>
       </c>
       <c r="V141" s="2">
-        <v>15.387600000000001</v>
+        <v>14.4841</v>
       </c>
       <c r="W141" s="2">
-        <v>-87.805400000000006</v>
+        <v>-87.981499999999997</v>
       </c>
     </row>
     <row r="142" spans="1:23">
@@ -11309,10 +11315,10 @@
         <v>55</v>
       </c>
       <c r="V142" s="2">
-        <v>15.3881</v>
+        <v>14.4849</v>
       </c>
       <c r="W142" s="2">
-        <v>-87.811000000000007</v>
+        <v>-87.982100000000003</v>
       </c>
     </row>
     <row r="143" spans="1:23">
@@ -11377,10 +11383,10 @@
         <v>167</v>
       </c>
       <c r="V143" s="2">
-        <v>15.388400000000001</v>
+        <v>14.4855</v>
       </c>
       <c r="W143" s="2">
-        <v>-87.8108</v>
+        <v>-87.981499999999997</v>
       </c>
     </row>
     <row r="144" spans="1:23">
@@ -11445,13 +11451,13 @@
         <v>174</v>
       </c>
       <c r="V144" s="2">
-        <v>15.3889</v>
+        <v>16.319299999999998</v>
       </c>
       <c r="W144" s="2">
-        <v>-87.805899999999994</v>
-      </c>
-    </row>
-    <row r="145" spans="1:23">
+        <v>-86.538700000000006</v>
+      </c>
+    </row>
+    <row r="145" spans="1:27">
       <c r="A145" s="1">
         <v>35879</v>
       </c>
@@ -11510,16 +11516,16 @@
         <v>35</v>
       </c>
       <c r="U145" s="7" t="s">
-        <v>179</v>
+        <v>39</v>
       </c>
       <c r="V145" s="2">
-        <v>15.393000000000001</v>
+        <v>16.442499999999999</v>
       </c>
       <c r="W145" s="2">
-        <v>-87.806200000000004</v>
-      </c>
-    </row>
-    <row r="146" spans="1:23">
+        <v>-85.887699999999995</v>
+      </c>
+    </row>
+    <row r="146" spans="1:27">
       <c r="A146" s="1">
         <v>25855</v>
       </c>
@@ -11536,10 +11542,10 @@
         <v>12</v>
       </c>
       <c r="F146" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G146" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="G146" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>27</v>
@@ -11548,10 +11554,10 @@
         <v>17</v>
       </c>
       <c r="J146" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="K146" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="K146" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="L146" s="1" t="s">
         <v>30</v>
@@ -11560,16 +11566,16 @@
         <v>7</v>
       </c>
       <c r="N146" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O146" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="O146" s="1" t="s">
+      <c r="P146" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q146" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="P146" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q146" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="R146" s="1" t="s">
         <v>34</v>
@@ -11581,13 +11587,13 @@
         <v>39</v>
       </c>
       <c r="V146" s="2">
-        <v>15.393599999999999</v>
+        <v>14.245100000000001</v>
       </c>
       <c r="W146" s="2">
-        <v>-87.807100000000005</v>
-      </c>
-    </row>
-    <row r="147" spans="1:23">
+        <v>-87.898399999999995</v>
+      </c>
+    </row>
+    <row r="147" spans="1:27" ht="15">
       <c r="A147" s="1">
         <v>28037</v>
       </c>
@@ -11604,58 +11610,59 @@
         <v>13</v>
       </c>
       <c r="F147" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G147" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G147" s="1" t="s">
+      <c r="H147" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I147" s="1">
+        <v>1</v>
+      </c>
+      <c r="J147" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H147" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I147" s="1">
-        <v>1</v>
-      </c>
-      <c r="J147" s="1" t="s">
+      <c r="K147" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="K147" s="1" t="s">
+      <c r="L147" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M147" s="1">
+        <v>1</v>
+      </c>
+      <c r="N147" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L147" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M147" s="1">
-        <v>1</v>
-      </c>
-      <c r="N147" s="1" t="s">
+      <c r="O147" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P147" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q147" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="O147" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="P147" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q147" s="1" t="s">
+      <c r="R147" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S147" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U147" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="R147" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S147" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U147" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="V147" s="2">
-        <v>15.393599999999999</v>
+        <v>14.5839</v>
       </c>
       <c r="W147" s="2">
-        <v>-87.7898</v>
-      </c>
-    </row>
-    <row r="148" spans="1:23">
+        <v>-88.584599999999995</v>
+      </c>
+      <c r="AA147" s="8"/>
+    </row>
+    <row r="148" spans="1:27">
       <c r="A148" s="1">
         <v>28151</v>
       </c>
@@ -11672,40 +11679,40 @@
         <v>13</v>
       </c>
       <c r="F148" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G148" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G148" s="1" t="s">
+      <c r="H148" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I148" s="1">
+        <v>1</v>
+      </c>
+      <c r="J148" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H148" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I148" s="1">
-        <v>1</v>
-      </c>
-      <c r="J148" s="1" t="s">
+      <c r="K148" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="K148" s="1" t="s">
+      <c r="L148" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M148" s="1">
+        <v>1</v>
+      </c>
+      <c r="N148" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L148" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M148" s="1">
-        <v>1</v>
-      </c>
-      <c r="N148" s="1" t="s">
+      <c r="O148" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P148" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q148" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="O148" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="P148" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q148" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="R148" s="1" t="s">
         <v>34</v>
@@ -11717,13 +11724,13 @@
         <v>145</v>
       </c>
       <c r="V148" s="2">
-        <v>15.395200000000001</v>
+        <v>14.587899999999999</v>
       </c>
       <c r="W148" s="2">
-        <v>-87.808099999999996</v>
-      </c>
-    </row>
-    <row r="149" spans="1:23">
+        <v>-88.582999999999998</v>
+      </c>
+    </row>
+    <row r="149" spans="1:27">
       <c r="A149" s="1">
         <v>28156</v>
       </c>
@@ -11740,58 +11747,58 @@
         <v>13</v>
       </c>
       <c r="F149" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G149" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G149" s="1" t="s">
+      <c r="H149" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I149" s="1">
+        <v>1</v>
+      </c>
+      <c r="J149" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H149" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I149" s="1">
-        <v>1</v>
-      </c>
-      <c r="J149" s="1" t="s">
+      <c r="K149" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="K149" s="1" t="s">
+      <c r="L149" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M149" s="1">
+        <v>1</v>
+      </c>
+      <c r="N149" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L149" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M149" s="1">
-        <v>1</v>
-      </c>
-      <c r="N149" s="1" t="s">
+      <c r="O149" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P149" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q149" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="O149" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="P149" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q149" s="1" t="s">
+      <c r="R149" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S149" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U149" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="R149" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S149" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U149" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="V149" s="2">
-        <v>15.3955</v>
+        <v>14.588200000000001</v>
       </c>
       <c r="W149" s="2">
-        <v>-87.797700000000006</v>
-      </c>
-    </row>
-    <row r="150" spans="1:23">
+        <v>-88.582700000000003</v>
+      </c>
+    </row>
+    <row r="150" spans="1:27">
       <c r="A150" s="1">
         <v>28181</v>
       </c>
@@ -11808,41 +11815,41 @@
         <v>13</v>
       </c>
       <c r="F150" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G150" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G150" s="1" t="s">
+      <c r="H150" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I150" s="1">
+        <v>1</v>
+      </c>
+      <c r="J150" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H150" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I150" s="1">
-        <v>1</v>
-      </c>
-      <c r="J150" s="1" t="s">
+      <c r="K150" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="K150" s="1" t="s">
+      <c r="L150" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M150" s="1">
+        <v>1</v>
+      </c>
+      <c r="N150" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L150" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M150" s="1">
-        <v>1</v>
-      </c>
-      <c r="N150" s="1" t="s">
+      <c r="O150" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P150" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q150" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="O150" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="P150" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q150" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="R150" s="1" t="s">
         <v>34</v>
       </c>
@@ -11850,16 +11857,16 @@
         <v>35</v>
       </c>
       <c r="U150" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="V150" s="2">
-        <v>15.3956</v>
+        <v>14.588800000000001</v>
       </c>
       <c r="W150" s="2">
-        <v>-87.808400000000006</v>
-      </c>
-    </row>
-    <row r="151" spans="1:23">
+        <v>-88.581699999999998</v>
+      </c>
+    </row>
+    <row r="151" spans="1:27">
       <c r="A151" s="1">
         <v>28327</v>
       </c>
@@ -11876,41 +11883,41 @@
         <v>13</v>
       </c>
       <c r="F151" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G151" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G151" s="1" t="s">
+      <c r="H151" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I151" s="1">
+        <v>1</v>
+      </c>
+      <c r="J151" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H151" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I151" s="1">
-        <v>1</v>
-      </c>
-      <c r="J151" s="1" t="s">
+      <c r="K151" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="K151" s="1" t="s">
+      <c r="L151" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M151" s="1">
+        <v>1</v>
+      </c>
+      <c r="N151" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L151" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M151" s="1">
-        <v>1</v>
-      </c>
-      <c r="N151" s="1" t="s">
+      <c r="O151" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P151" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q151" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="O151" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="P151" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q151" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="R151" s="1" t="s">
         <v>34</v>
       </c>
@@ -11918,16 +11925,16 @@
         <v>35</v>
       </c>
       <c r="U151" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="V151" s="2">
-        <v>15.3956</v>
+        <v>14.5922</v>
       </c>
       <c r="W151" s="2">
-        <v>-87.808499999999995</v>
-      </c>
-    </row>
-    <row r="152" spans="1:23">
+        <v>-88.5822</v>
+      </c>
+    </row>
+    <row r="152" spans="1:27">
       <c r="A152" s="1">
         <v>33574</v>
       </c>
@@ -11944,10 +11951,10 @@
         <v>18</v>
       </c>
       <c r="F152" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G152" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G152" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H152" s="1" t="s">
         <v>27</v>
@@ -11956,28 +11963,28 @@
         <v>4</v>
       </c>
       <c r="J152" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K152" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K152" s="1" t="s">
+      <c r="L152" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M152" s="1">
+        <v>1</v>
+      </c>
+      <c r="N152" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L152" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M152" s="1">
-        <v>1</v>
-      </c>
-      <c r="N152" s="1" t="s">
+      <c r="O152" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P152" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q152" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O152" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P152" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q152" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R152" s="1" t="s">
         <v>34</v>
@@ -11989,13 +11996,13 @@
         <v>37</v>
       </c>
       <c r="V152" s="2">
-        <v>15.396100000000001</v>
+        <v>15.3992</v>
       </c>
       <c r="W152" s="2">
-        <v>-87.802400000000006</v>
-      </c>
-    </row>
-    <row r="153" spans="1:23">
+        <v>-87.804299999999998</v>
+      </c>
+    </row>
+    <row r="153" spans="1:27">
       <c r="A153" s="1">
         <v>33581</v>
       </c>
@@ -12012,10 +12019,10 @@
         <v>18</v>
       </c>
       <c r="F153" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G153" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G153" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H153" s="1" t="s">
         <v>27</v>
@@ -12024,28 +12031,28 @@
         <v>4</v>
       </c>
       <c r="J153" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K153" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K153" s="1" t="s">
+      <c r="L153" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M153" s="1">
+        <v>1</v>
+      </c>
+      <c r="N153" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L153" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M153" s="1">
-        <v>1</v>
-      </c>
-      <c r="N153" s="1" t="s">
+      <c r="O153" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P153" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q153" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O153" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P153" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q153" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R153" s="1" t="s">
         <v>34</v>
@@ -12057,13 +12064,13 @@
         <v>104</v>
       </c>
       <c r="V153" s="2">
-        <v>15.3971</v>
+        <v>15.400499999999999</v>
       </c>
       <c r="W153" s="2">
-        <v>-87.814599999999999</v>
-      </c>
-    </row>
-    <row r="154" spans="1:23">
+        <v>-87.809700000000007</v>
+      </c>
+    </row>
+    <row r="154" spans="1:27">
       <c r="A154" s="1">
         <v>33592</v>
       </c>
@@ -12080,10 +12087,10 @@
         <v>18</v>
       </c>
       <c r="F154" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G154" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G154" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H154" s="1" t="s">
         <v>27</v>
@@ -12092,28 +12099,28 @@
         <v>4</v>
       </c>
       <c r="J154" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K154" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K154" s="1" t="s">
+      <c r="L154" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M154" s="1">
+        <v>1</v>
+      </c>
+      <c r="N154" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L154" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M154" s="1">
-        <v>1</v>
-      </c>
-      <c r="N154" s="1" t="s">
+      <c r="O154" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P154" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q154" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O154" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P154" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q154" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R154" s="1" t="s">
         <v>34</v>
@@ -12125,13 +12132,13 @@
         <v>106</v>
       </c>
       <c r="V154" s="2">
-        <v>15.3978</v>
+        <v>15.4011</v>
       </c>
       <c r="W154" s="2">
-        <v>-87.800399999999996</v>
-      </c>
-    </row>
-    <row r="155" spans="1:23">
+        <v>-87.809600000000003</v>
+      </c>
+    </row>
+    <row r="155" spans="1:27">
       <c r="A155" s="1">
         <v>33598</v>
       </c>
@@ -12148,10 +12155,10 @@
         <v>18</v>
       </c>
       <c r="F155" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G155" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G155" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H155" s="1" t="s">
         <v>27</v>
@@ -12160,28 +12167,28 @@
         <v>4</v>
       </c>
       <c r="J155" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K155" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K155" s="1" t="s">
+      <c r="L155" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M155" s="1">
+        <v>1</v>
+      </c>
+      <c r="N155" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L155" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M155" s="1">
-        <v>1</v>
-      </c>
-      <c r="N155" s="1" t="s">
+      <c r="O155" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P155" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q155" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O155" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P155" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q155" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R155" s="1" t="s">
         <v>34</v>
@@ -12193,13 +12200,13 @@
         <v>120</v>
       </c>
       <c r="V155" s="2">
-        <v>15.398099999999999</v>
+        <v>15.401400000000001</v>
       </c>
       <c r="W155" s="2">
-        <v>-87.814400000000006</v>
-      </c>
-    </row>
-    <row r="156" spans="1:23">
+        <v>-87.806600000000003</v>
+      </c>
+    </row>
+    <row r="156" spans="1:27">
       <c r="A156" s="1">
         <v>33636</v>
       </c>
@@ -12216,10 +12223,10 @@
         <v>18</v>
       </c>
       <c r="F156" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G156" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G156" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H156" s="1" t="s">
         <v>27</v>
@@ -12228,28 +12235,28 @@
         <v>4</v>
       </c>
       <c r="J156" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K156" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K156" s="1" t="s">
+      <c r="L156" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M156" s="1">
+        <v>1</v>
+      </c>
+      <c r="N156" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L156" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M156" s="1">
-        <v>1</v>
-      </c>
-      <c r="N156" s="1" t="s">
+      <c r="O156" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P156" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q156" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O156" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P156" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q156" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R156" s="1" t="s">
         <v>34</v>
@@ -12261,13 +12268,13 @@
         <v>104</v>
       </c>
       <c r="V156" s="2">
-        <v>15.398199999999999</v>
+        <v>15.402799999999999</v>
       </c>
       <c r="W156" s="2">
-        <v>-87.801699999999997</v>
-      </c>
-    </row>
-    <row r="157" spans="1:23">
+        <v>-87.806399999999996</v>
+      </c>
+    </row>
+    <row r="157" spans="1:27">
       <c r="A157" s="1">
         <v>33637</v>
       </c>
@@ -12284,10 +12291,10 @@
         <v>18</v>
       </c>
       <c r="F157" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G157" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G157" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H157" s="1" t="s">
         <v>27</v>
@@ -12296,28 +12303,28 @@
         <v>4</v>
       </c>
       <c r="J157" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K157" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K157" s="1" t="s">
+      <c r="L157" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M157" s="1">
+        <v>1</v>
+      </c>
+      <c r="N157" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L157" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M157" s="1">
-        <v>1</v>
-      </c>
-      <c r="N157" s="1" t="s">
+      <c r="O157" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P157" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q157" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O157" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P157" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q157" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R157" s="1" t="s">
         <v>34</v>
@@ -12329,13 +12336,13 @@
         <v>104</v>
       </c>
       <c r="V157" s="2">
-        <v>15.398300000000001</v>
+        <v>15.402900000000001</v>
       </c>
       <c r="W157" s="2">
-        <v>-87.809299999999993</v>
-      </c>
-    </row>
-    <row r="158" spans="1:23">
+        <v>-87.806399999999996</v>
+      </c>
+    </row>
+    <row r="158" spans="1:27">
       <c r="A158" s="1">
         <v>33638</v>
       </c>
@@ -12352,10 +12359,10 @@
         <v>18</v>
       </c>
       <c r="F158" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G158" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G158" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H158" s="1" t="s">
         <v>27</v>
@@ -12364,28 +12371,28 @@
         <v>4</v>
       </c>
       <c r="J158" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K158" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K158" s="1" t="s">
+      <c r="L158" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M158" s="1">
+        <v>1</v>
+      </c>
+      <c r="N158" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L158" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M158" s="1">
-        <v>1</v>
-      </c>
-      <c r="N158" s="1" t="s">
+      <c r="O158" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P158" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q158" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O158" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P158" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q158" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R158" s="1" t="s">
         <v>34</v>
@@ -12397,13 +12404,13 @@
         <v>104</v>
       </c>
       <c r="V158" s="2">
-        <v>15.398300000000001</v>
+        <v>15.402900000000001</v>
       </c>
       <c r="W158" s="2">
-        <v>-87.809299999999993</v>
-      </c>
-    </row>
-    <row r="159" spans="1:23">
+        <v>-87.806399999999996</v>
+      </c>
+    </row>
+    <row r="159" spans="1:27">
       <c r="A159" s="1">
         <v>33647</v>
       </c>
@@ -12420,10 +12427,10 @@
         <v>18</v>
       </c>
       <c r="F159" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G159" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G159" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H159" s="1" t="s">
         <v>27</v>
@@ -12432,46 +12439,46 @@
         <v>4</v>
       </c>
       <c r="J159" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K159" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K159" s="1" t="s">
+      <c r="L159" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M159" s="1">
+        <v>1</v>
+      </c>
+      <c r="N159" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L159" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M159" s="1">
-        <v>1</v>
-      </c>
-      <c r="N159" s="1" t="s">
+      <c r="O159" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P159" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q159" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="O159" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P159" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q159" s="1" t="s">
+      <c r="R159" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S159" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U159" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="R159" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S159" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U159" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="V159" s="2">
-        <v>15.399100000000001</v>
+        <v>15.403</v>
       </c>
       <c r="W159" s="2">
-        <v>-87.803799999999995</v>
-      </c>
-    </row>
-    <row r="160" spans="1:23">
+        <v>-87.805800000000005</v>
+      </c>
+    </row>
+    <row r="160" spans="1:27">
       <c r="A160" s="1">
         <v>33654</v>
       </c>
@@ -12488,10 +12495,10 @@
         <v>18</v>
       </c>
       <c r="F160" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G160" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G160" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>27</v>
@@ -12500,29 +12507,29 @@
         <v>4</v>
       </c>
       <c r="J160" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K160" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K160" s="1" t="s">
+      <c r="L160" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M160" s="1">
+        <v>1</v>
+      </c>
+      <c r="N160" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L160" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M160" s="1">
-        <v>1</v>
-      </c>
-      <c r="N160" s="1" t="s">
+      <c r="O160" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P160" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q160" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="O160" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P160" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q160" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="R160" s="1" t="s">
         <v>34</v>
       </c>
@@ -12530,16 +12537,16 @@
         <v>35</v>
       </c>
       <c r="U160" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="V160" s="2">
-        <v>15.3992</v>
+        <v>15.4034</v>
       </c>
       <c r="W160" s="2">
-        <v>-87.804299999999998</v>
-      </c>
-    </row>
-    <row r="161" spans="1:23">
+        <v>-87.798599999999993</v>
+      </c>
+    </row>
+    <row r="161" spans="1:27">
       <c r="A161" s="1">
         <v>33662</v>
       </c>
@@ -12556,10 +12563,10 @@
         <v>18</v>
       </c>
       <c r="F161" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G161" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G161" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H161" s="1" t="s">
         <v>27</v>
@@ -12568,28 +12575,28 @@
         <v>4</v>
       </c>
       <c r="J161" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K161" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K161" s="1" t="s">
+      <c r="L161" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M161" s="1">
+        <v>1</v>
+      </c>
+      <c r="N161" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L161" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M161" s="1">
-        <v>1</v>
-      </c>
-      <c r="N161" s="1" t="s">
+      <c r="O161" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P161" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q161" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O161" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P161" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q161" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R161" s="1" t="s">
         <v>34</v>
@@ -12601,13 +12608,13 @@
         <v>37</v>
       </c>
       <c r="V161" s="2">
-        <v>15.3995</v>
+        <v>15.404199999999999</v>
       </c>
       <c r="W161" s="2">
-        <v>-87.8078</v>
-      </c>
-    </row>
-    <row r="162" spans="1:23">
+        <v>-87.812100000000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:27" ht="15">
       <c r="A162" s="1">
         <v>33664</v>
       </c>
@@ -12624,10 +12631,10 @@
         <v>18</v>
       </c>
       <c r="F162" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G162" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G162" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H162" s="1" t="s">
         <v>27</v>
@@ -12636,28 +12643,28 @@
         <v>4</v>
       </c>
       <c r="J162" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K162" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="K162" s="1" t="s">
+      <c r="L162" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M162" s="1">
+        <v>1</v>
+      </c>
+      <c r="N162" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L162" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M162" s="1">
-        <v>1</v>
-      </c>
-      <c r="N162" s="1" t="s">
+      <c r="O162" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P162" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q162" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="O162" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P162" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q162" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="R162" s="1" t="s">
         <v>34</v>
@@ -12669,11 +12676,12 @@
         <v>62</v>
       </c>
       <c r="V162" s="2">
-        <v>15.399699999999999</v>
+        <v>15.404500000000001</v>
       </c>
       <c r="W162" s="2">
-        <v>-87.811000000000007</v>
-      </c>
+        <v>-87.808999999999997</v>
+      </c>
+      <c r="AA162" s="8"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U162">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-22-2020 15-06-19
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="478" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2959EC4F-AEF0-4A40-8DB9-92839F6B497D}"/>
+  <xr:revisionPtr revIDLastSave="639" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{133B870B-09C0-4216-8C99-C73D3287A0DA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="FARMACIAS" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FARMACIAS!$A$1:$W$162</definedName>
-    <definedName name="_xlnm.Database">FARMACIAS!$A$1:$U$162</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FARMACIAS!$A$1:$W$179</definedName>
+    <definedName name="_xlnm.Database">FARMACIAS!$A$1:$U$160</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="221">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -279,15 +279,15 @@
     <t>Comayagua</t>
   </si>
   <si>
+    <t>030101</t>
+  </si>
+  <si>
+    <t>HND-0301</t>
+  </si>
+  <si>
     <t>0301</t>
   </si>
   <si>
-    <t>030101</t>
-  </si>
-  <si>
-    <t>HND-0301</t>
-  </si>
-  <si>
     <t>Farmacia Colonial</t>
   </si>
   <si>
@@ -643,6 +643,60 @@
   </si>
   <si>
     <t>HND-1102</t>
+  </si>
+  <si>
+    <t>aldea</t>
+  </si>
+  <si>
+    <t>Farmacias kielsa Siguatepeque</t>
+  </si>
+  <si>
+    <t>Farmacia Simán Siguatepeque #1</t>
+  </si>
+  <si>
+    <t>Farmacia Montecristo</t>
+  </si>
+  <si>
+    <t>Farmacia Kielsa</t>
+  </si>
+  <si>
+    <t>Farmacia Simán Siguatepeque #3</t>
+  </si>
+  <si>
+    <t>Farmacia el Angel</t>
+  </si>
+  <si>
+    <t>Farmacia Simán Siguatepeque #4</t>
+  </si>
+  <si>
+    <t>Farmacia Recinos</t>
+  </si>
+  <si>
+    <t>Farmacia Nuevo Sol</t>
+  </si>
+  <si>
+    <t>Tochis Farmacia</t>
+  </si>
+  <si>
+    <t>Pronavida</t>
+  </si>
+  <si>
+    <t>Farmacia Milla</t>
+  </si>
+  <si>
+    <t>farmacia city</t>
+  </si>
+  <si>
+    <t>Kielsa</t>
+  </si>
+  <si>
+    <t>Farmacia Nahualí</t>
+  </si>
+  <si>
+    <t>Medi7</t>
+  </si>
+  <si>
+    <t>FarmaCity Calle 21 de agosto</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1197,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1153,6 +1207,8 @@
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1301,10 +1357,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F90EE072-0F9D-4F60-9697-FDBBEB228828}" name="FARMACIAS_HN" displayName="FARMACIAS_HN" ref="A1:W162" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:W162" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W162">
-    <sortCondition ref="A1:A162"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F90EE072-0F9D-4F60-9697-FDBBEB228828}" name="FARMACIAS_HN" displayName="FARMACIAS_HN" ref="A1:W179" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:W179" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W160">
+    <sortCondition ref="A1:A160"/>
   </sortState>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{C232FE6F-7903-4FC5-93EC-F7BD24958957}" name="OBJECTID_1" dataDxfId="22"/>
@@ -1632,11 +1688,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA162"/>
+  <dimension ref="A1:AA185"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z26" sqref="Z26"/>
+      <pane ySplit="1" topLeftCell="P167" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F172" sqref="F172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -6252,8 +6308,8 @@
       <c r="I68" s="1">
         <v>1</v>
       </c>
-      <c r="J68" s="1" t="s">
-        <v>81</v>
+      <c r="J68" s="1">
+        <v>301</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>80</v>
@@ -6265,7 +6321,7 @@
         <v>1</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O68" s="1" t="s">
         <v>80</v>
@@ -6274,7 +6330,7 @@
         <v>33</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R68" s="1" t="s">
         <v>35</v>
@@ -6321,7 +6377,7 @@
         <v>1</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>80</v>
@@ -6333,7 +6389,7 @@
         <v>1</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O69" s="1" t="s">
         <v>80</v>
@@ -6342,7 +6398,7 @@
         <v>33</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R69" s="1" t="s">
         <v>35</v>
@@ -6389,7 +6445,7 @@
         <v>1</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>80</v>
@@ -6401,7 +6457,7 @@
         <v>1</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O70" s="1" t="s">
         <v>80</v>
@@ -6410,7 +6466,7 @@
         <v>33</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R70" s="1" t="s">
         <v>35</v>
@@ -6457,7 +6513,7 @@
         <v>1</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>80</v>
@@ -6469,7 +6525,7 @@
         <v>1</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O71" s="1" t="s">
         <v>80</v>
@@ -6478,7 +6534,7 @@
         <v>33</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R71" s="1" t="s">
         <v>35</v>
@@ -6525,7 +6581,7 @@
         <v>1</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>80</v>
@@ -6537,7 +6593,7 @@
         <v>1</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O72" s="1" t="s">
         <v>80</v>
@@ -6546,7 +6602,7 @@
         <v>33</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R72" s="1" t="s">
         <v>35</v>
@@ -6593,7 +6649,7 @@
         <v>1</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>80</v>
@@ -6605,7 +6661,7 @@
         <v>1</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O73" s="1" t="s">
         <v>80</v>
@@ -6614,7 +6670,7 @@
         <v>33</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R73" s="1" t="s">
         <v>35</v>
@@ -7518,7 +7574,7 @@
     </row>
     <row r="87" spans="1:23">
       <c r="A87" s="1">
-        <v>28499</v>
+        <v>28512</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>23</v>
@@ -7575,86 +7631,87 @@
         <v>36</v>
       </c>
       <c r="U87" s="1" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="V87" s="2">
-        <v>14.596399999999999</v>
+        <v>14.596500000000001</v>
       </c>
       <c r="W87" s="2">
-        <v>-87.831199999999995</v>
-      </c>
-    </row>
-    <row r="88" spans="1:23">
-      <c r="A88" s="1">
-        <v>28512</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D88" s="1">
-        <v>3</v>
-      </c>
-      <c r="E88" s="1">
-        <v>3</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I88" s="1">
-        <v>18</v>
-      </c>
-      <c r="J88" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K88" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L88" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M88" s="1">
-        <v>1</v>
-      </c>
-      <c r="N88" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="O88" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="P88" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q88" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="R88" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S88" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U88" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="V88" s="2">
-        <v>14.596500000000001</v>
-      </c>
-      <c r="W88" s="2">
         <v>-87.832300000000004</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" s="8" customFormat="1" ht="15">
+      <c r="A88" s="9">
+        <v>31814</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D88" s="9">
+        <v>3</v>
+      </c>
+      <c r="E88" s="9">
+        <v>4</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G88" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="H88" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I88" s="9">
+        <v>1</v>
+      </c>
+      <c r="J88" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="K88" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="L88" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M88" s="9">
+        <v>1</v>
+      </c>
+      <c r="N88" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="O88" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="P88" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q88" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="R88" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="S88" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T88" s="9"/>
+      <c r="U88" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="V88" s="10">
+        <v>14.767799999999999</v>
+      </c>
+      <c r="W88" s="10">
+        <v>-88.779300000000006</v>
       </c>
     </row>
     <row r="89" spans="1:23">
       <c r="A89" s="1">
-        <v>28641</v>
+        <v>31817</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>23</v>
@@ -7666,25 +7723,25 @@
         <v>3</v>
       </c>
       <c r="E89" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I89" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="L89" s="1" t="s">
         <v>30</v>
@@ -7693,16 +7750,16 @@
         <v>1</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="O89" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="P89" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q89" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="R89" s="1" t="s">
         <v>35</v>
@@ -7711,18 +7768,18 @@
         <v>36</v>
       </c>
       <c r="U89" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="V89" s="2">
-        <v>14.598699999999999</v>
+        <v>14.7681</v>
       </c>
       <c r="W89" s="2">
-        <v>-87.831400000000002</v>
+        <v>-88.777600000000007</v>
       </c>
     </row>
     <row r="90" spans="1:23">
       <c r="A90" s="1">
-        <v>31814</v>
+        <v>31819</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>23</v>
@@ -7779,18 +7836,18 @@
         <v>36</v>
       </c>
       <c r="U90" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V90" s="2">
-        <v>14.767799999999999</v>
+        <v>14.7681</v>
       </c>
       <c r="W90" s="2">
-        <v>-88.779300000000006</v>
+        <v>-88.777500000000003</v>
       </c>
     </row>
     <row r="91" spans="1:23">
       <c r="A91" s="1">
-        <v>31817</v>
+        <v>32195</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>23</v>
@@ -7814,13 +7871,13 @@
         <v>27</v>
       </c>
       <c r="I91" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L91" s="1" t="s">
         <v>30</v>
@@ -7829,16 +7886,16 @@
         <v>1</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O91" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="P91" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q91" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="R91" s="1" t="s">
         <v>35</v>
@@ -7847,18 +7904,18 @@
         <v>36</v>
       </c>
       <c r="U91" s="1" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
       <c r="V91" s="2">
-        <v>14.7681</v>
+        <v>14.832100000000001</v>
       </c>
       <c r="W91" s="2">
-        <v>-88.777600000000007</v>
+        <v>-89.093999999999994</v>
       </c>
     </row>
     <row r="92" spans="1:23">
       <c r="A92" s="1">
-        <v>31819</v>
+        <v>32419</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>23</v>
@@ -7882,13 +7939,13 @@
         <v>27</v>
       </c>
       <c r="I92" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="L92" s="1" t="s">
         <v>30</v>
@@ -7897,16 +7954,16 @@
         <v>1</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="O92" s="1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="P92" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q92" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="R92" s="1" t="s">
         <v>35</v>
@@ -7915,18 +7972,18 @@
         <v>36</v>
       </c>
       <c r="U92" s="1" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="V92" s="2">
-        <v>14.7681</v>
+        <v>14.8384</v>
       </c>
       <c r="W92" s="2">
-        <v>-88.777500000000003</v>
+        <v>-89.1554</v>
       </c>
     </row>
     <row r="93" spans="1:23">
       <c r="A93" s="1">
-        <v>32195</v>
+        <v>33156</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>23</v>
@@ -7950,13 +8007,13 @@
         <v>27</v>
       </c>
       <c r="I93" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="L93" s="1" t="s">
         <v>30</v>
@@ -7965,16 +8022,16 @@
         <v>1</v>
       </c>
       <c r="N93" s="1" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="O93" s="1" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="P93" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q93" s="1" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="R93" s="1" t="s">
         <v>35</v>
@@ -7983,18 +8040,18 @@
         <v>36</v>
       </c>
       <c r="U93" s="1" t="s">
-        <v>123</v>
+        <v>48</v>
       </c>
       <c r="V93" s="2">
-        <v>14.832100000000001</v>
+        <v>15.065799999999999</v>
       </c>
       <c r="W93" s="2">
-        <v>-89.093999999999994</v>
+        <v>-88.747100000000003</v>
       </c>
     </row>
     <row r="94" spans="1:23">
       <c r="A94" s="1">
-        <v>32419</v>
+        <v>33366</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>23</v>
@@ -8006,25 +8063,25 @@
         <v>3</v>
       </c>
       <c r="E94" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I94" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="L94" s="1" t="s">
         <v>30</v>
@@ -8033,16 +8090,16 @@
         <v>1</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="O94" s="1" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="P94" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q94" s="1" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="R94" s="1" t="s">
         <v>35</v>
@@ -8051,18 +8108,18 @@
         <v>36</v>
       </c>
       <c r="U94" s="1" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="V94" s="2">
-        <v>14.8384</v>
+        <v>15.316800000000001</v>
       </c>
       <c r="W94" s="2">
-        <v>-89.1554</v>
+        <v>-87.990300000000005</v>
       </c>
     </row>
     <row r="95" spans="1:23">
       <c r="A95" s="1">
-        <v>33156</v>
+        <v>33574</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>23</v>
@@ -8074,25 +8131,25 @@
         <v>3</v>
       </c>
       <c r="E95" s="1">
+        <v>18</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I95" s="1">
         <v>4</v>
       </c>
-      <c r="F95" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I95" s="1">
-        <v>13</v>
-      </c>
       <c r="J95" s="1" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="L95" s="1" t="s">
         <v>30</v>
@@ -8101,16 +8158,16 @@
         <v>1</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="O95" s="1" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="P95" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q95" s="1" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="R95" s="1" t="s">
         <v>35</v>
@@ -8119,18 +8176,18 @@
         <v>36</v>
       </c>
       <c r="U95" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="V95" s="2">
-        <v>15.065799999999999</v>
+        <v>15.3992</v>
       </c>
       <c r="W95" s="2">
-        <v>-88.747100000000003</v>
+        <v>-87.804299999999998</v>
       </c>
     </row>
     <row r="96" spans="1:23">
       <c r="A96" s="1">
-        <v>33366</v>
+        <v>33581</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>23</v>
@@ -8142,25 +8199,25 @@
         <v>3</v>
       </c>
       <c r="E96" s="1">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I96" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="L96" s="1" t="s">
         <v>30</v>
@@ -8169,16 +8226,16 @@
         <v>1</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="O96" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="P96" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q96" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="R96" s="1" t="s">
         <v>35</v>
@@ -8187,18 +8244,18 @@
         <v>36</v>
       </c>
       <c r="U96" s="1" t="s">
-        <v>56</v>
+        <v>146</v>
       </c>
       <c r="V96" s="2">
-        <v>15.316800000000001</v>
+        <v>15.400499999999999</v>
       </c>
       <c r="W96" s="2">
-        <v>-87.990300000000005</v>
+        <v>-87.809700000000007</v>
       </c>
     </row>
     <row r="97" spans="1:23">
       <c r="A97" s="1">
-        <v>33574</v>
+        <v>33592</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>23</v>
@@ -8255,18 +8312,18 @@
         <v>36</v>
       </c>
       <c r="U97" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="V97" s="2">
-        <v>15.3992</v>
+        <v>15.4011</v>
       </c>
       <c r="W97" s="2">
-        <v>-87.804299999999998</v>
+        <v>-87.809600000000003</v>
       </c>
     </row>
     <row r="98" spans="1:23">
       <c r="A98" s="1">
-        <v>33581</v>
+        <v>33598</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>23</v>
@@ -8323,18 +8380,18 @@
         <v>36</v>
       </c>
       <c r="U98" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="V98" s="2">
-        <v>15.400499999999999</v>
+        <v>15.401400000000001</v>
       </c>
       <c r="W98" s="2">
-        <v>-87.809700000000007</v>
+        <v>-87.806600000000003</v>
       </c>
     </row>
     <row r="99" spans="1:23">
       <c r="A99" s="1">
-        <v>33592</v>
+        <v>33636</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>23</v>
@@ -8391,18 +8448,18 @@
         <v>36</v>
       </c>
       <c r="U99" s="1" t="s">
-        <v>50</v>
+        <v>146</v>
       </c>
       <c r="V99" s="2">
-        <v>15.4011</v>
+        <v>15.402799999999999</v>
       </c>
       <c r="W99" s="2">
-        <v>-87.809600000000003</v>
+        <v>-87.806399999999996</v>
       </c>
     </row>
     <row r="100" spans="1:23">
       <c r="A100" s="1">
-        <v>33598</v>
+        <v>33637</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>23</v>
@@ -8459,18 +8516,18 @@
         <v>36</v>
       </c>
       <c r="U100" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="V100" s="2">
-        <v>15.401400000000001</v>
+        <v>15.402900000000001</v>
       </c>
       <c r="W100" s="2">
-        <v>-87.806600000000003</v>
+        <v>-87.806399999999996</v>
       </c>
     </row>
     <row r="101" spans="1:23">
       <c r="A101" s="1">
-        <v>33636</v>
+        <v>33638</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>23</v>
@@ -8530,7 +8587,7 @@
         <v>146</v>
       </c>
       <c r="V101" s="2">
-        <v>15.402799999999999</v>
+        <v>15.402900000000001</v>
       </c>
       <c r="W101" s="2">
         <v>-87.806399999999996</v>
@@ -8538,7 +8595,7 @@
     </row>
     <row r="102" spans="1:23">
       <c r="A102" s="1">
-        <v>33637</v>
+        <v>33647</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>23</v>
@@ -8595,18 +8652,18 @@
         <v>36</v>
       </c>
       <c r="U102" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="V102" s="2">
-        <v>15.402900000000001</v>
+        <v>15.403</v>
       </c>
       <c r="W102" s="2">
-        <v>-87.806399999999996</v>
+        <v>-87.805800000000005</v>
       </c>
     </row>
     <row r="103" spans="1:23">
       <c r="A103" s="1">
-        <v>33638</v>
+        <v>33654</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>23</v>
@@ -8663,18 +8720,18 @@
         <v>36</v>
       </c>
       <c r="U103" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="V103" s="2">
-        <v>15.402900000000001</v>
+        <v>15.4034</v>
       </c>
       <c r="W103" s="2">
-        <v>-87.806399999999996</v>
+        <v>-87.798599999999993</v>
       </c>
     </row>
     <row r="104" spans="1:23">
       <c r="A104" s="1">
-        <v>33647</v>
+        <v>33662</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>23</v>
@@ -8731,18 +8788,18 @@
         <v>36</v>
       </c>
       <c r="U104" s="1" t="s">
-        <v>148</v>
+        <v>41</v>
       </c>
       <c r="V104" s="2">
-        <v>15.403</v>
+        <v>15.404199999999999</v>
       </c>
       <c r="W104" s="2">
-        <v>-87.805800000000005</v>
+        <v>-87.812100000000001</v>
       </c>
     </row>
     <row r="105" spans="1:23">
       <c r="A105" s="1">
-        <v>33654</v>
+        <v>33664</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>23</v>
@@ -8799,18 +8856,18 @@
         <v>36</v>
       </c>
       <c r="U105" s="1" t="s">
-        <v>149</v>
+        <v>56</v>
       </c>
       <c r="V105" s="2">
-        <v>15.4034</v>
+        <v>15.404500000000001</v>
       </c>
       <c r="W105" s="2">
-        <v>-87.798599999999993</v>
+        <v>-87.808999999999997</v>
       </c>
     </row>
     <row r="106" spans="1:23">
       <c r="A106" s="1">
-        <v>33662</v>
+        <v>33766</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>23</v>
@@ -8822,25 +8879,25 @@
         <v>3</v>
       </c>
       <c r="E106" s="1">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I106" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="K106" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="L106" s="1" t="s">
         <v>30</v>
@@ -8849,16 +8906,16 @@
         <v>1</v>
       </c>
       <c r="N106" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="O106" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="P106" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q106" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="R106" s="1" t="s">
         <v>35</v>
@@ -8870,15 +8927,15 @@
         <v>41</v>
       </c>
       <c r="V106" s="2">
-        <v>15.404199999999999</v>
+        <v>15.4361</v>
       </c>
       <c r="W106" s="2">
-        <v>-87.812100000000001</v>
+        <v>-87.921099999999996</v>
       </c>
     </row>
     <row r="107" spans="1:23">
       <c r="A107" s="1">
-        <v>33664</v>
+        <v>33767</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>23</v>
@@ -8890,25 +8947,25 @@
         <v>3</v>
       </c>
       <c r="E107" s="1">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I107" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="L107" s="1" t="s">
         <v>30</v>
@@ -8917,16 +8974,16 @@
         <v>1</v>
       </c>
       <c r="N107" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="O107" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="P107" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q107" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="R107" s="1" t="s">
         <v>35</v>
@@ -8938,15 +8995,15 @@
         <v>56</v>
       </c>
       <c r="V107" s="2">
-        <v>15.404500000000001</v>
+        <v>15.436500000000001</v>
       </c>
       <c r="W107" s="2">
-        <v>-87.808999999999997</v>
+        <v>-87.924300000000002</v>
       </c>
     </row>
     <row r="108" spans="1:23">
       <c r="A108" s="1">
-        <v>33766</v>
+        <v>33773</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>23</v>
@@ -9006,15 +9063,15 @@
         <v>41</v>
       </c>
       <c r="V108" s="2">
-        <v>15.4361</v>
+        <v>15.438499999999999</v>
       </c>
       <c r="W108" s="2">
-        <v>-87.921099999999996</v>
+        <v>-87.926900000000003</v>
       </c>
     </row>
     <row r="109" spans="1:23">
       <c r="A109" s="1">
-        <v>33767</v>
+        <v>33778</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>23</v>
@@ -9071,18 +9128,18 @@
         <v>36</v>
       </c>
       <c r="U109" s="1" t="s">
-        <v>56</v>
+        <v>147</v>
       </c>
       <c r="V109" s="2">
-        <v>15.436500000000001</v>
+        <v>15.4405</v>
       </c>
       <c r="W109" s="2">
-        <v>-87.924300000000002</v>
+        <v>-87.929100000000005</v>
       </c>
     </row>
     <row r="110" spans="1:23">
       <c r="A110" s="1">
-        <v>33773</v>
+        <v>33918</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>23</v>
@@ -9106,13 +9163,13 @@
         <v>27</v>
       </c>
       <c r="I110" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="L110" s="1" t="s">
         <v>30</v>
@@ -9121,16 +9178,16 @@
         <v>1</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="O110" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="P110" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q110" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="R110" s="1" t="s">
         <v>35</v>
@@ -9142,15 +9199,15 @@
         <v>41</v>
       </c>
       <c r="V110" s="2">
-        <v>15.438499999999999</v>
+        <v>15.477399999999999</v>
       </c>
       <c r="W110" s="2">
-        <v>-87.926900000000003</v>
+        <v>-87.985699999999994</v>
       </c>
     </row>
     <row r="111" spans="1:23">
       <c r="A111" s="1">
-        <v>33778</v>
+        <v>33929</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>23</v>
@@ -9174,13 +9231,13 @@
         <v>27</v>
       </c>
       <c r="I111" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="L111" s="1" t="s">
         <v>30</v>
@@ -9189,16 +9246,16 @@
         <v>1</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="O111" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="P111" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q111" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="R111" s="1" t="s">
         <v>35</v>
@@ -9207,18 +9264,18 @@
         <v>36</v>
       </c>
       <c r="U111" s="1" t="s">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="V111" s="2">
-        <v>15.4405</v>
+        <v>15.4787</v>
       </c>
       <c r="W111" s="2">
-        <v>-87.929100000000005</v>
+        <v>-87.975099999999998</v>
       </c>
     </row>
     <row r="112" spans="1:23">
       <c r="A112" s="1">
-        <v>33918</v>
+        <v>33941</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>23</v>
@@ -9275,18 +9332,18 @@
         <v>36</v>
       </c>
       <c r="U112" s="1" t="s">
-        <v>41</v>
+        <v>158</v>
       </c>
       <c r="V112" s="2">
-        <v>15.477399999999999</v>
+        <v>15.4796</v>
       </c>
       <c r="W112" s="2">
-        <v>-87.985699999999994</v>
+        <v>-88.011200000000002</v>
       </c>
     </row>
     <row r="113" spans="1:23">
       <c r="A113" s="1">
-        <v>33929</v>
+        <v>33960</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>23</v>
@@ -9343,18 +9400,18 @@
         <v>36</v>
       </c>
       <c r="U113" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="V113" s="2">
-        <v>15.4787</v>
+        <v>15.4854</v>
       </c>
       <c r="W113" s="2">
-        <v>-87.975099999999998</v>
+        <v>-88.034099999999995</v>
       </c>
     </row>
     <row r="114" spans="1:23">
       <c r="A114" s="1">
-        <v>33941</v>
+        <v>33962</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>23</v>
@@ -9411,18 +9468,18 @@
         <v>36</v>
       </c>
       <c r="U114" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="V114" s="2">
-        <v>15.4796</v>
+        <v>15.4855</v>
       </c>
       <c r="W114" s="2">
-        <v>-88.011200000000002</v>
+        <v>-87.984399999999994</v>
       </c>
     </row>
     <row r="115" spans="1:23">
       <c r="A115" s="1">
-        <v>33960</v>
+        <v>33987</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>23</v>
@@ -9479,18 +9536,18 @@
         <v>36</v>
       </c>
       <c r="U115" s="1" t="s">
-        <v>49</v>
+        <v>160</v>
       </c>
       <c r="V115" s="2">
-        <v>15.4854</v>
+        <v>15.489800000000001</v>
       </c>
       <c r="W115" s="2">
-        <v>-88.034099999999995</v>
+        <v>-87.986000000000004</v>
       </c>
     </row>
     <row r="116" spans="1:23">
       <c r="A116" s="1">
-        <v>33962</v>
+        <v>34003</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>23</v>
@@ -9547,18 +9604,18 @@
         <v>36</v>
       </c>
       <c r="U116" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="V116" s="2">
-        <v>15.4855</v>
+        <v>15.492599999999999</v>
       </c>
       <c r="W116" s="2">
-        <v>-87.984399999999994</v>
+        <v>-88.011499999999998</v>
       </c>
     </row>
     <row r="117" spans="1:23">
       <c r="A117" s="1">
-        <v>33987</v>
+        <v>34007</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>23</v>
@@ -9615,18 +9672,18 @@
         <v>36</v>
       </c>
       <c r="U117" s="1" t="s">
-        <v>160</v>
+        <v>41</v>
       </c>
       <c r="V117" s="2">
-        <v>15.489800000000001</v>
+        <v>15.492699999999999</v>
       </c>
       <c r="W117" s="2">
-        <v>-87.986000000000004</v>
+        <v>-88.016499999999994</v>
       </c>
     </row>
     <row r="118" spans="1:23">
       <c r="A118" s="1">
-        <v>34003</v>
+        <v>34010</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>23</v>
@@ -9683,18 +9740,18 @@
         <v>36</v>
       </c>
       <c r="U118" s="1" t="s">
-        <v>161</v>
+        <v>41</v>
       </c>
       <c r="V118" s="2">
-        <v>15.492599999999999</v>
+        <v>15.4933</v>
       </c>
       <c r="W118" s="2">
-        <v>-88.011499999999998</v>
+        <v>-87.986500000000007</v>
       </c>
     </row>
     <row r="119" spans="1:23">
       <c r="A119" s="1">
-        <v>34007</v>
+        <v>34011</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>23</v>
@@ -9754,15 +9811,15 @@
         <v>41</v>
       </c>
       <c r="V119" s="2">
-        <v>15.492699999999999</v>
+        <v>15.493399999999999</v>
       </c>
       <c r="W119" s="2">
-        <v>-88.016499999999994</v>
+        <v>-87.984800000000007</v>
       </c>
     </row>
     <row r="120" spans="1:23">
       <c r="A120" s="1">
-        <v>34010</v>
+        <v>34016</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>23</v>
@@ -9822,15 +9879,15 @@
         <v>41</v>
       </c>
       <c r="V120" s="2">
-        <v>15.4933</v>
+        <v>15.493600000000001</v>
       </c>
       <c r="W120" s="2">
-        <v>-87.986500000000007</v>
+        <v>-87.984099999999998</v>
       </c>
     </row>
     <row r="121" spans="1:23">
       <c r="A121" s="1">
-        <v>34011</v>
+        <v>34030</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>23</v>
@@ -9887,18 +9944,18 @@
         <v>36</v>
       </c>
       <c r="U121" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="V121" s="2">
-        <v>15.493399999999999</v>
+        <v>15.494300000000001</v>
       </c>
       <c r="W121" s="2">
-        <v>-87.984800000000007</v>
+        <v>-88.034099999999995</v>
       </c>
     </row>
     <row r="122" spans="1:23">
       <c r="A122" s="1">
-        <v>34016</v>
+        <v>34134</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>23</v>
@@ -9955,18 +10012,18 @@
         <v>36</v>
       </c>
       <c r="U122" s="1" t="s">
-        <v>41</v>
+        <v>162</v>
       </c>
       <c r="V122" s="2">
-        <v>15.493600000000001</v>
+        <v>15.499700000000001</v>
       </c>
       <c r="W122" s="2">
-        <v>-87.984099999999998</v>
+        <v>-88.025000000000006</v>
       </c>
     </row>
     <row r="123" spans="1:23">
       <c r="A123" s="1">
-        <v>34030</v>
+        <v>34144</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>23</v>
@@ -10023,18 +10080,18 @@
         <v>36</v>
       </c>
       <c r="U123" s="1" t="s">
-        <v>48</v>
+        <v>163</v>
       </c>
       <c r="V123" s="2">
-        <v>15.494300000000001</v>
+        <v>15.4999</v>
       </c>
       <c r="W123" s="2">
-        <v>-88.034099999999995</v>
+        <v>-88.037499999999994</v>
       </c>
     </row>
     <row r="124" spans="1:23">
       <c r="A124" s="1">
-        <v>34134</v>
+        <v>34146</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>23</v>
@@ -10091,18 +10148,18 @@
         <v>36</v>
       </c>
       <c r="U124" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="V124" s="2">
-        <v>15.499700000000001</v>
+        <v>15.5</v>
       </c>
       <c r="W124" s="2">
-        <v>-88.025000000000006</v>
+        <v>-88.020700000000005</v>
       </c>
     </row>
     <row r="125" spans="1:23">
       <c r="A125" s="1">
-        <v>34144</v>
+        <v>34160</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>23</v>
@@ -10159,18 +10216,18 @@
         <v>36</v>
       </c>
       <c r="U125" s="1" t="s">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="V125" s="2">
-        <v>15.4999</v>
+        <v>15.500299999999999</v>
       </c>
       <c r="W125" s="2">
-        <v>-88.037499999999994</v>
+        <v>-88.038399999999996</v>
       </c>
     </row>
     <row r="126" spans="1:23">
       <c r="A126" s="1">
-        <v>34146</v>
+        <v>34204</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>23</v>
@@ -10227,18 +10284,18 @@
         <v>36</v>
       </c>
       <c r="U126" s="1" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="V126" s="2">
-        <v>15.5</v>
+        <v>15.501799999999999</v>
       </c>
       <c r="W126" s="2">
-        <v>-88.020700000000005</v>
+        <v>-88.027100000000004</v>
       </c>
     </row>
     <row r="127" spans="1:23">
       <c r="A127" s="1">
-        <v>34160</v>
+        <v>34249</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>23</v>
@@ -10295,18 +10352,18 @@
         <v>36</v>
       </c>
       <c r="U127" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="V127" s="2">
-        <v>15.500299999999999</v>
+        <v>15.504099999999999</v>
       </c>
       <c r="W127" s="2">
-        <v>-88.038399999999996</v>
+        <v>-88.014200000000002</v>
       </c>
     </row>
     <row r="128" spans="1:23">
       <c r="A128" s="1">
-        <v>34204</v>
+        <v>34269</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>23</v>
@@ -10363,18 +10420,18 @@
         <v>36</v>
       </c>
       <c r="U128" s="1" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="V128" s="2">
-        <v>15.501799999999999</v>
+        <v>15.505100000000001</v>
       </c>
       <c r="W128" s="2">
-        <v>-88.027100000000004</v>
+        <v>-88.022300000000001</v>
       </c>
     </row>
     <row r="129" spans="1:23">
       <c r="A129" s="1">
-        <v>34249</v>
+        <v>34306</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>23</v>
@@ -10431,18 +10488,18 @@
         <v>36</v>
       </c>
       <c r="U129" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="V129" s="2">
-        <v>15.504099999999999</v>
+        <v>15.5061</v>
       </c>
       <c r="W129" s="2">
-        <v>-88.014200000000002</v>
+        <v>-88.027199999999993</v>
       </c>
     </row>
     <row r="130" spans="1:23">
       <c r="A130" s="1">
-        <v>34269</v>
+        <v>34359</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>23</v>
@@ -10499,18 +10556,18 @@
         <v>36</v>
       </c>
       <c r="U130" s="1" t="s">
-        <v>165</v>
+        <v>84</v>
       </c>
       <c r="V130" s="2">
-        <v>15.505100000000001</v>
+        <v>15.5105</v>
       </c>
       <c r="W130" s="2">
-        <v>-88.022300000000001</v>
+        <v>-88.012699999999995</v>
       </c>
     </row>
     <row r="131" spans="1:23">
       <c r="A131" s="1">
-        <v>34306</v>
+        <v>34373</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>23</v>
@@ -10567,18 +10624,18 @@
         <v>36</v>
       </c>
       <c r="U131" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="V131" s="2">
-        <v>15.5061</v>
+        <v>15.5124</v>
       </c>
       <c r="W131" s="2">
-        <v>-88.027199999999993</v>
+        <v>-88.037000000000006</v>
       </c>
     </row>
     <row r="132" spans="1:23">
       <c r="A132" s="1">
-        <v>34359</v>
+        <v>34389</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>23</v>
@@ -10635,18 +10692,18 @@
         <v>36</v>
       </c>
       <c r="U132" s="1" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="V132" s="2">
-        <v>15.5105</v>
+        <v>15.5146</v>
       </c>
       <c r="W132" s="2">
-        <v>-88.012699999999995</v>
+        <v>-88.033600000000007</v>
       </c>
     </row>
     <row r="133" spans="1:23">
       <c r="A133" s="1">
-        <v>34373</v>
+        <v>34401</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>23</v>
@@ -10706,15 +10763,15 @@
         <v>41</v>
       </c>
       <c r="V133" s="2">
-        <v>15.5124</v>
+        <v>15.5159</v>
       </c>
       <c r="W133" s="2">
-        <v>-88.037000000000006</v>
+        <v>-88.028400000000005</v>
       </c>
     </row>
     <row r="134" spans="1:23">
       <c r="A134" s="1">
-        <v>34389</v>
+        <v>34445</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>23</v>
@@ -10771,18 +10828,18 @@
         <v>36</v>
       </c>
       <c r="U134" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="V134" s="2">
-        <v>15.5146</v>
+        <v>15.5244</v>
       </c>
       <c r="W134" s="2">
-        <v>-88.033600000000007</v>
+        <v>-88.038499999999999</v>
       </c>
     </row>
     <row r="135" spans="1:23">
       <c r="A135" s="1">
-        <v>34401</v>
+        <v>34466</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>23</v>
@@ -10839,18 +10896,18 @@
         <v>36</v>
       </c>
       <c r="U135" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="V135" s="2">
-        <v>15.5159</v>
+        <v>15.5298</v>
       </c>
       <c r="W135" s="2">
-        <v>-88.028400000000005</v>
+        <v>-88.032700000000006</v>
       </c>
     </row>
     <row r="136" spans="1:23">
       <c r="A136" s="1">
-        <v>34445</v>
+        <v>34471</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>23</v>
@@ -10907,18 +10964,18 @@
         <v>36</v>
       </c>
       <c r="U136" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="V136" s="2">
-        <v>15.5244</v>
+        <v>15.5299</v>
       </c>
       <c r="W136" s="2">
-        <v>-88.038499999999999</v>
+        <v>-88.026499999999999</v>
       </c>
     </row>
     <row r="137" spans="1:23">
       <c r="A137" s="1">
-        <v>34466</v>
+        <v>34475</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>23</v>
@@ -10975,18 +11032,18 @@
         <v>36</v>
       </c>
       <c r="U137" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="V137" s="2">
-        <v>15.5298</v>
+        <v>15.5299</v>
       </c>
       <c r="W137" s="2">
-        <v>-88.032700000000006</v>
+        <v>-88.025499999999994</v>
       </c>
     </row>
     <row r="138" spans="1:23">
       <c r="A138" s="1">
-        <v>34471</v>
+        <v>34521</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>23</v>
@@ -11043,18 +11100,18 @@
         <v>36</v>
       </c>
       <c r="U138" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="V138" s="2">
-        <v>15.5299</v>
+        <v>15.5306</v>
       </c>
       <c r="W138" s="2">
-        <v>-88.026499999999999</v>
+        <v>-88.029399999999995</v>
       </c>
     </row>
     <row r="139" spans="1:23">
       <c r="A139" s="1">
-        <v>34475</v>
+        <v>34533</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>23</v>
@@ -11111,18 +11168,18 @@
         <v>36</v>
       </c>
       <c r="U139" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="V139" s="2">
-        <v>15.5299</v>
+        <v>15.5341</v>
       </c>
       <c r="W139" s="2">
-        <v>-88.025499999999994</v>
+        <v>-88.019300000000001</v>
       </c>
     </row>
     <row r="140" spans="1:23">
       <c r="A140" s="1">
-        <v>34521</v>
+        <v>34539</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>23</v>
@@ -11182,15 +11239,15 @@
         <v>48</v>
       </c>
       <c r="V140" s="2">
-        <v>15.5306</v>
+        <v>15.537100000000001</v>
       </c>
       <c r="W140" s="2">
-        <v>-88.029399999999995</v>
+        <v>-88.014899999999997</v>
       </c>
     </row>
     <row r="141" spans="1:23">
       <c r="A141" s="1">
-        <v>34533</v>
+        <v>34554</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>23</v>
@@ -11250,15 +11307,15 @@
         <v>41</v>
       </c>
       <c r="V141" s="2">
-        <v>15.5341</v>
+        <v>15.542899999999999</v>
       </c>
       <c r="W141" s="2">
-        <v>-88.019300000000001</v>
+        <v>-88.023099999999999</v>
       </c>
     </row>
     <row r="142" spans="1:23">
       <c r="A142" s="1">
-        <v>34539</v>
+        <v>34576</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>23</v>
@@ -11315,18 +11372,18 @@
         <v>36</v>
       </c>
       <c r="U142" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="V142" s="2">
-        <v>15.537100000000001</v>
+        <v>15.549099999999999</v>
       </c>
       <c r="W142" s="2">
-        <v>-88.014899999999997</v>
+        <v>-88.035899999999998</v>
       </c>
     </row>
     <row r="143" spans="1:23">
       <c r="A143" s="1">
-        <v>34554</v>
+        <v>34583</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>23</v>
@@ -11386,15 +11443,15 @@
         <v>41</v>
       </c>
       <c r="V143" s="2">
-        <v>15.542899999999999</v>
+        <v>15.5505</v>
       </c>
       <c r="W143" s="2">
-        <v>-88.023099999999999</v>
+        <v>-88.004800000000003</v>
       </c>
     </row>
     <row r="144" spans="1:23">
       <c r="A144" s="1">
-        <v>34576</v>
+        <v>34671</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>23</v>
@@ -11406,43 +11463,43 @@
         <v>3</v>
       </c>
       <c r="E144" s="1">
+        <v>1</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H144" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I144" s="1">
         <v>5</v>
       </c>
-      <c r="F144" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G144" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H144" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I144" s="1">
-        <v>1</v>
-      </c>
       <c r="J144" s="1" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="K144" s="1" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="L144" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M144" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="N144" s="1" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="O144" s="1" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P144" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q144" s="1" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="R144" s="1" t="s">
         <v>35</v>
@@ -11451,18 +11508,18 @@
         <v>36</v>
       </c>
       <c r="U144" s="1" t="s">
-        <v>41</v>
+        <v>173</v>
       </c>
       <c r="V144" s="2">
-        <v>15.549099999999999</v>
+        <v>15.5989</v>
       </c>
       <c r="W144" s="2">
-        <v>-88.035899999999998</v>
-      </c>
-    </row>
-    <row r="145" spans="1:27">
+        <v>-87.208799999999997</v>
+      </c>
+    </row>
+    <row r="145" spans="1:27" ht="15">
       <c r="A145" s="1">
-        <v>34583</v>
+        <v>34675</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>23</v>
@@ -11474,43 +11531,43 @@
         <v>3</v>
       </c>
       <c r="E145" s="1">
+        <v>1</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H145" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I145" s="1">
         <v>5</v>
       </c>
-      <c r="F145" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H145" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I145" s="1">
-        <v>1</v>
-      </c>
       <c r="J145" s="1" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="L145" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M145" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="N145" s="1" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="O145" s="1" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P145" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q145" s="1" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="R145" s="1" t="s">
         <v>35</v>
@@ -11519,18 +11576,19 @@
         <v>36</v>
       </c>
       <c r="U145" s="1" t="s">
-        <v>41</v>
+        <v>174</v>
       </c>
       <c r="V145" s="2">
-        <v>15.5505</v>
+        <v>15.599</v>
       </c>
       <c r="W145" s="2">
-        <v>-88.004800000000003</v>
-      </c>
+        <v>-88.659800000000004</v>
+      </c>
+      <c r="AA145" s="8"/>
     </row>
     <row r="146" spans="1:27">
       <c r="A146" s="1">
-        <v>34671</v>
+        <v>34726</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>23</v>
@@ -11542,43 +11600,43 @@
         <v>3</v>
       </c>
       <c r="E146" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I146" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="K146" s="1" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="L146" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M146" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="N146" s="1" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="O146" s="1" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="P146" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q146" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="R146" s="1" t="s">
         <v>35</v>
@@ -11587,18 +11645,18 @@
         <v>36</v>
       </c>
       <c r="U146" s="1" t="s">
-        <v>173</v>
+        <v>56</v>
       </c>
       <c r="V146" s="2">
-        <v>15.5989</v>
+        <v>15.6119</v>
       </c>
       <c r="W146" s="2">
-        <v>-87.208799999999997</v>
-      </c>
-    </row>
-    <row r="147" spans="1:27" ht="15">
+        <v>-87.956299999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:27">
       <c r="A147" s="1">
-        <v>34675</v>
+        <v>35080</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>23</v>
@@ -11622,31 +11680,31 @@
         <v>27</v>
       </c>
       <c r="I147" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J147" s="1" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="K147" s="1" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="L147" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M147" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="N147" s="1" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="O147" s="1" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="P147" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q147" s="1" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="R147" s="1" t="s">
         <v>35</v>
@@ -11655,19 +11713,18 @@
         <v>36</v>
       </c>
       <c r="U147" s="1" t="s">
-        <v>174</v>
+        <v>57</v>
       </c>
       <c r="V147" s="2">
-        <v>15.599</v>
+        <v>15.7738</v>
       </c>
       <c r="W147" s="2">
-        <v>-88.659800000000004</v>
-      </c>
-      <c r="AA147" s="8"/>
+        <v>-87.475499999999997</v>
+      </c>
     </row>
     <row r="148" spans="1:27">
       <c r="A148" s="1">
-        <v>34726</v>
+        <v>35085</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>23</v>
@@ -11679,25 +11736,25 @@
         <v>3</v>
       </c>
       <c r="E148" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="H148" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I148" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J148" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="K148" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="L148" s="1" t="s">
         <v>30</v>
@@ -11706,16 +11763,16 @@
         <v>1</v>
       </c>
       <c r="N148" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="O148" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="P148" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q148" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="R148" s="1" t="s">
         <v>35</v>
@@ -11724,18 +11781,18 @@
         <v>36</v>
       </c>
       <c r="U148" s="1" t="s">
-        <v>56</v>
+        <v>183</v>
       </c>
       <c r="V148" s="2">
-        <v>15.6119</v>
+        <v>15.7744</v>
       </c>
       <c r="W148" s="2">
-        <v>-87.956299999999999</v>
+        <v>-87.446799999999996</v>
       </c>
     </row>
     <row r="149" spans="1:27">
       <c r="A149" s="1">
-        <v>35080</v>
+        <v>35108</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>23</v>
@@ -11759,13 +11816,13 @@
         <v>27</v>
       </c>
       <c r="I149" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J149" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="K149" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="L149" s="1" t="s">
         <v>30</v>
@@ -11774,16 +11831,16 @@
         <v>1</v>
       </c>
       <c r="N149" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="O149" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="P149" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q149" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="R149" s="1" t="s">
         <v>35</v>
@@ -11792,18 +11849,18 @@
         <v>36</v>
       </c>
       <c r="U149" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="V149" s="2">
-        <v>15.7738</v>
+        <v>15.5989</v>
       </c>
       <c r="W149" s="2">
-        <v>-87.475499999999997</v>
+        <v>-87.208799999999997</v>
       </c>
     </row>
     <row r="150" spans="1:27">
       <c r="A150" s="1">
-        <v>35085</v>
+        <v>35182</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>23</v>
@@ -11860,18 +11917,18 @@
         <v>36</v>
       </c>
       <c r="U150" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="V150" s="2">
-        <v>15.7744</v>
+        <v>15.781700000000001</v>
       </c>
       <c r="W150" s="2">
-        <v>-87.446799999999996</v>
+        <v>-87.453400000000002</v>
       </c>
     </row>
     <row r="151" spans="1:27">
       <c r="A151" s="1">
-        <v>35108</v>
+        <v>35243</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>23</v>
@@ -11895,13 +11952,13 @@
         <v>27</v>
       </c>
       <c r="I151" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J151" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="K151" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L151" s="1" t="s">
         <v>30</v>
@@ -11910,16 +11967,16 @@
         <v>1</v>
       </c>
       <c r="N151" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="O151" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="P151" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q151" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="R151" s="1" t="s">
         <v>35</v>
@@ -11928,18 +11985,18 @@
         <v>36</v>
       </c>
       <c r="U151" s="1" t="s">
-        <v>48</v>
+        <v>189</v>
       </c>
       <c r="V151" s="2">
-        <v>15.5989</v>
+        <v>15.783300000000001</v>
       </c>
       <c r="W151" s="2">
-        <v>-87.208799999999997</v>
+        <v>-87.452100000000002</v>
       </c>
     </row>
     <row r="152" spans="1:27">
       <c r="A152" s="1">
-        <v>35182</v>
+        <v>35246</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>23</v>
@@ -11996,18 +12053,18 @@
         <v>36</v>
       </c>
       <c r="U152" s="1" t="s">
-        <v>188</v>
+        <v>41</v>
       </c>
       <c r="V152" s="2">
-        <v>15.781700000000001</v>
+        <v>15.7834</v>
       </c>
       <c r="W152" s="2">
-        <v>-87.453400000000002</v>
+        <v>-87.449399999999997</v>
       </c>
     </row>
     <row r="153" spans="1:27">
       <c r="A153" s="1">
-        <v>35243</v>
+        <v>35257</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>23</v>
@@ -12031,13 +12088,13 @@
         <v>27</v>
       </c>
       <c r="I153" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J153" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="K153" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="L153" s="1" t="s">
         <v>30</v>
@@ -12046,16 +12103,16 @@
         <v>1</v>
       </c>
       <c r="N153" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="O153" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="P153" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q153" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="R153" s="1" t="s">
         <v>35</v>
@@ -12064,18 +12121,18 @@
         <v>36</v>
       </c>
       <c r="U153" s="1" t="s">
-        <v>189</v>
+        <v>41</v>
       </c>
       <c r="V153" s="2">
-        <v>15.783300000000001</v>
+        <v>15.7836</v>
       </c>
       <c r="W153" s="2">
-        <v>-87.452100000000002</v>
+        <v>-86.792500000000004</v>
       </c>
     </row>
     <row r="154" spans="1:27">
       <c r="A154" s="1">
-        <v>35246</v>
+        <v>35269</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>23</v>
@@ -12132,18 +12189,18 @@
         <v>36</v>
       </c>
       <c r="U154" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="V154" s="2">
-        <v>15.7834</v>
+        <v>15.783899999999999</v>
       </c>
       <c r="W154" s="2">
-        <v>-87.449399999999997</v>
+        <v>-87.449700000000007</v>
       </c>
     </row>
     <row r="155" spans="1:27">
       <c r="A155" s="1">
-        <v>35257</v>
+        <v>35275</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>23</v>
@@ -12167,13 +12224,13 @@
         <v>27</v>
       </c>
       <c r="I155" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J155" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="K155" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L155" s="1" t="s">
         <v>30</v>
@@ -12182,16 +12239,16 @@
         <v>1</v>
       </c>
       <c r="N155" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="O155" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="P155" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q155" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="R155" s="1" t="s">
         <v>35</v>
@@ -12203,15 +12260,15 @@
         <v>41</v>
       </c>
       <c r="V155" s="2">
-        <v>15.7836</v>
+        <v>15.7841</v>
       </c>
       <c r="W155" s="2">
-        <v>-86.792500000000004</v>
+        <v>-87.450699999999998</v>
       </c>
     </row>
     <row r="156" spans="1:27">
       <c r="A156" s="1">
-        <v>35269</v>
+        <v>35290</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>23</v>
@@ -12268,18 +12325,18 @@
         <v>36</v>
       </c>
       <c r="U156" s="1" t="s">
-        <v>49</v>
+        <v>190</v>
       </c>
       <c r="V156" s="2">
-        <v>15.783899999999999</v>
+        <v>15.7845</v>
       </c>
       <c r="W156" s="2">
-        <v>-87.449700000000007</v>
+        <v>-87.451599999999999</v>
       </c>
     </row>
     <row r="157" spans="1:27">
       <c r="A157" s="1">
-        <v>35275</v>
+        <v>35304</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>23</v>
@@ -12303,13 +12360,13 @@
         <v>27</v>
       </c>
       <c r="I157" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J157" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="K157" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="L157" s="1" t="s">
         <v>30</v>
@@ -12318,16 +12375,16 @@
         <v>1</v>
       </c>
       <c r="N157" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="O157" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="P157" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q157" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="R157" s="1" t="s">
         <v>35</v>
@@ -12336,18 +12393,18 @@
         <v>36</v>
       </c>
       <c r="U157" s="1" t="s">
-        <v>41</v>
+        <v>191</v>
       </c>
       <c r="V157" s="2">
-        <v>15.7841</v>
+        <v>15.784800000000001</v>
       </c>
       <c r="W157" s="2">
-        <v>-87.450699999999998</v>
+        <v>-86.792900000000003</v>
       </c>
     </row>
     <row r="158" spans="1:27">
       <c r="A158" s="1">
-        <v>35290</v>
+        <v>35307</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>23</v>
@@ -12371,13 +12428,13 @@
         <v>27</v>
       </c>
       <c r="I158" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J158" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="K158" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="L158" s="1" t="s">
         <v>30</v>
@@ -12386,16 +12443,16 @@
         <v>1</v>
       </c>
       <c r="N158" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="O158" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="P158" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q158" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="R158" s="1" t="s">
         <v>35</v>
@@ -12403,19 +12460,19 @@
       <c r="S158" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U158" s="1" t="s">
-        <v>190</v>
+      <c r="U158" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="V158" s="2">
-        <v>15.7845</v>
+        <v>15.7849</v>
       </c>
       <c r="W158" s="2">
-        <v>-87.451599999999999</v>
+        <v>-86.791899999999998</v>
       </c>
     </row>
     <row r="159" spans="1:27">
       <c r="A159" s="1">
-        <v>35304</v>
+        <v>35819</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>23</v>
@@ -12427,13 +12484,13 @@
         <v>3</v>
       </c>
       <c r="E159" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="H159" s="1" t="s">
         <v>27</v>
@@ -12442,10 +12499,10 @@
         <v>1</v>
       </c>
       <c r="J159" s="1" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="K159" s="1" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="L159" s="1" t="s">
         <v>30</v>
@@ -12454,16 +12511,16 @@
         <v>1</v>
       </c>
       <c r="N159" s="1" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="O159" s="1" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="P159" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q159" s="1" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="R159" s="1" t="s">
         <v>35</v>
@@ -12472,18 +12529,18 @@
         <v>36</v>
       </c>
       <c r="U159" s="1" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="V159" s="2">
-        <v>15.784800000000001</v>
+        <v>16.319299999999998</v>
       </c>
       <c r="W159" s="2">
-        <v>-86.792900000000003</v>
-      </c>
-    </row>
-    <row r="160" spans="1:27">
+        <v>-86.538700000000006</v>
+      </c>
+    </row>
+    <row r="160" spans="1:27" ht="15">
       <c r="A160" s="1">
-        <v>35307</v>
+        <v>35879</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>23</v>
@@ -12495,25 +12552,25 @@
         <v>3</v>
       </c>
       <c r="E160" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I160" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J160" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="L160" s="1" t="s">
         <v>30</v>
@@ -12522,16 +12579,16 @@
         <v>1</v>
       </c>
       <c r="N160" s="1" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="O160" s="1" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="P160" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q160" s="1" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="R160" s="1" t="s">
         <v>35</v>
@@ -12543,15 +12600,16 @@
         <v>78</v>
       </c>
       <c r="V160" s="2">
-        <v>15.7849</v>
+        <v>16.442499999999999</v>
       </c>
       <c r="W160" s="2">
-        <v>-86.791899999999998</v>
-      </c>
-    </row>
-    <row r="161" spans="1:27">
+        <v>-85.887699999999995</v>
+      </c>
+      <c r="AA160" s="8"/>
+    </row>
+    <row r="161" spans="1:23">
       <c r="A161" s="1">
-        <v>35819</v>
+        <v>50001</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>23</v>
@@ -12563,25 +12621,25 @@
         <v>3</v>
       </c>
       <c r="E161" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>192</v>
+        <v>79</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>193</v>
+        <v>80</v>
       </c>
       <c r="H161" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I161" s="1">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>194</v>
+        <v>108</v>
       </c>
       <c r="K161" s="1" t="s">
-        <v>195</v>
+        <v>109</v>
       </c>
       <c r="L161" s="1" t="s">
         <v>30</v>
@@ -12590,16 +12648,16 @@
         <v>1</v>
       </c>
       <c r="N161" s="1" t="s">
-        <v>196</v>
+        <v>110</v>
       </c>
       <c r="O161" s="1" t="s">
-        <v>195</v>
+        <v>109</v>
       </c>
       <c r="P161" s="1" t="s">
-        <v>33</v>
+        <v>203</v>
       </c>
       <c r="Q161" s="1" t="s">
-        <v>197</v>
+        <v>111</v>
       </c>
       <c r="R161" s="1" t="s">
         <v>35</v>
@@ -12608,18 +12666,18 @@
         <v>36</v>
       </c>
       <c r="U161" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="V161" s="2">
-        <v>16.319299999999998</v>
+        <v>14.5968988</v>
       </c>
       <c r="W161" s="2">
-        <v>-86.538700000000006</v>
-      </c>
-    </row>
-    <row r="162" spans="1:27" ht="15">
+        <v>-87.831554999999994</v>
+      </c>
+    </row>
+    <row r="162" spans="1:23">
       <c r="A162" s="1">
-        <v>35879</v>
+        <v>50002</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>23</v>
@@ -12631,25 +12689,25 @@
         <v>3</v>
       </c>
       <c r="E162" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>192</v>
+        <v>79</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>193</v>
+        <v>80</v>
       </c>
       <c r="H162" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I162" s="1">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="J162" s="1" t="s">
-        <v>199</v>
+        <v>108</v>
       </c>
       <c r="K162" s="1" t="s">
-        <v>200</v>
+        <v>109</v>
       </c>
       <c r="L162" s="1" t="s">
         <v>30</v>
@@ -12658,16 +12716,16 @@
         <v>1</v>
       </c>
       <c r="N162" s="1" t="s">
-        <v>201</v>
+        <v>110</v>
       </c>
       <c r="O162" s="1" t="s">
-        <v>200</v>
+        <v>109</v>
       </c>
       <c r="P162" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q162" s="1" t="s">
-        <v>202</v>
+        <v>111</v>
       </c>
       <c r="R162" s="1" t="s">
         <v>35</v>
@@ -12675,21 +12733,1181 @@
       <c r="S162" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U162" s="7" t="s">
-        <v>78</v>
+      <c r="U162" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="V162" s="2">
-        <v>16.442499999999999</v>
+        <v>14.597671699999999</v>
       </c>
       <c r="W162" s="2">
-        <v>-85.887699999999995</v>
-      </c>
-      <c r="AA162" s="8"/>
-    </row>
+        <v>-87.831420600000001</v>
+      </c>
+    </row>
+    <row r="163" spans="1:23" ht="15">
+      <c r="A163" s="1">
+        <v>50003</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D163" s="1">
+        <v>3</v>
+      </c>
+      <c r="E163" s="1">
+        <v>3</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H163" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I163" s="1">
+        <v>18</v>
+      </c>
+      <c r="J163" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K163" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L163" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M163" s="1">
+        <v>1</v>
+      </c>
+      <c r="N163" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O163" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P163" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q163" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R163" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S163" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U163" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="V163" s="2">
+        <v>14.596547299999999</v>
+      </c>
+      <c r="W163" s="2">
+        <v>-87.828834999999998</v>
+      </c>
+    </row>
+    <row r="164" spans="1:23">
+      <c r="A164" s="1">
+        <v>50004</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D164" s="1">
+        <v>3</v>
+      </c>
+      <c r="E164" s="1">
+        <v>3</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I164" s="1">
+        <v>18</v>
+      </c>
+      <c r="J164" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K164" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L164" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M164" s="1">
+        <v>1</v>
+      </c>
+      <c r="N164" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O164" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P164" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q164" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R164" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S164" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U164" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V164" s="2">
+        <v>14.596470500000001</v>
+      </c>
+      <c r="W164" s="2">
+        <v>-87.8321428</v>
+      </c>
+    </row>
+    <row r="165" spans="1:23">
+      <c r="A165" s="1">
+        <v>50005</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D165" s="1">
+        <v>3</v>
+      </c>
+      <c r="E165" s="1">
+        <v>3</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I165" s="1">
+        <v>18</v>
+      </c>
+      <c r="J165" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K165" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L165" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M165" s="1">
+        <v>1</v>
+      </c>
+      <c r="N165" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O165" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P165" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q165" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R165" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S165" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U165" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="V165" s="2">
+        <v>14.6011212</v>
+      </c>
+      <c r="W165" s="2">
+        <v>-87.842944000000003</v>
+      </c>
+    </row>
+    <row r="166" spans="1:23" ht="15">
+      <c r="A166" s="1">
+        <v>50006</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D166" s="1">
+        <v>3</v>
+      </c>
+      <c r="E166" s="1">
+        <v>3</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I166" s="1">
+        <v>18</v>
+      </c>
+      <c r="J166" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K166" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L166" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M166" s="1">
+        <v>1</v>
+      </c>
+      <c r="N166" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O166" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P166" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q166" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R166" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S166" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U166" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="V166" s="2">
+        <v>14.596408200000001</v>
+      </c>
+      <c r="W166" s="2">
+        <v>-87.8313287</v>
+      </c>
+    </row>
+    <row r="167" spans="1:23">
+      <c r="A167" s="1">
+        <v>50007</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D167" s="1">
+        <v>3</v>
+      </c>
+      <c r="E167" s="1">
+        <v>3</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I167" s="1">
+        <v>18</v>
+      </c>
+      <c r="J167" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K167" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L167" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M167" s="1">
+        <v>1</v>
+      </c>
+      <c r="N167" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O167" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P167" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q167" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R167" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S167" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U167" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="V167" s="2">
+        <v>14.5942943</v>
+      </c>
+      <c r="W167" s="2">
+        <v>-87.829985600000001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:23">
+      <c r="A168" s="1">
+        <v>50008</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D168" s="1">
+        <v>3</v>
+      </c>
+      <c r="E168" s="1">
+        <v>3</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I168" s="1">
+        <v>18</v>
+      </c>
+      <c r="J168" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K168" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L168" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M168" s="1">
+        <v>1</v>
+      </c>
+      <c r="N168" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O168" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P168" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q168" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R168" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S168" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U168" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="V168" s="2">
+        <v>14.5972314</v>
+      </c>
+      <c r="W168" s="2">
+        <v>-87.838980399999997</v>
+      </c>
+    </row>
+    <row r="169" spans="1:23">
+      <c r="A169" s="1">
+        <v>50009</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D169" s="1">
+        <v>3</v>
+      </c>
+      <c r="E169" s="1">
+        <v>3</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I169" s="1">
+        <v>18</v>
+      </c>
+      <c r="J169" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K169" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L169" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M169" s="1">
+        <v>1</v>
+      </c>
+      <c r="N169" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O169" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P169" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q169" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R169" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S169" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U169" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="V169" s="2">
+        <v>14.601276</v>
+      </c>
+      <c r="W169" s="2">
+        <v>-87.837087800000006</v>
+      </c>
+    </row>
+    <row r="170" spans="1:23">
+      <c r="A170" s="1">
+        <v>50010</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D170" s="1">
+        <v>3</v>
+      </c>
+      <c r="E170" s="1">
+        <v>3</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I170" s="1">
+        <v>18</v>
+      </c>
+      <c r="J170" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K170" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L170" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M170" s="1">
+        <v>1</v>
+      </c>
+      <c r="N170" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O170" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P170" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q170" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R170" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S170" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U170" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V170" s="2">
+        <v>14.593768300000001</v>
+      </c>
+      <c r="W170" s="2">
+        <v>-87.831689600000004</v>
+      </c>
+    </row>
+    <row r="171" spans="1:23">
+      <c r="A171" s="1">
+        <v>50011</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D171" s="1">
+        <v>3</v>
+      </c>
+      <c r="E171" s="1">
+        <v>3</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G171" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I171" s="1">
+        <v>18</v>
+      </c>
+      <c r="J171" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K171" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L171" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M171" s="1">
+        <v>1</v>
+      </c>
+      <c r="N171" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O171" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P171" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q171" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R171" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S171" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U171" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="V171" s="2">
+        <v>14.587884600000001</v>
+      </c>
+      <c r="W171" s="2">
+        <v>-87.836289500000007</v>
+      </c>
+    </row>
+    <row r="172" spans="1:23">
+      <c r="A172" s="1">
+        <v>50012</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D172" s="1">
+        <v>3</v>
+      </c>
+      <c r="E172" s="1">
+        <v>3</v>
+      </c>
+      <c r="F172" s="1">
+        <v>3</v>
+      </c>
+      <c r="G172" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I172" s="1">
+        <v>18</v>
+      </c>
+      <c r="J172" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K172" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L172" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M172" s="1">
+        <v>1</v>
+      </c>
+      <c r="N172" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O172" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P172" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q172" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R172" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S172" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U172" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="V172" s="2">
+        <v>14.5971791</v>
+      </c>
+      <c r="W172" s="2">
+        <v>-87.838133499999998</v>
+      </c>
+    </row>
+    <row r="173" spans="1:23">
+      <c r="A173" s="1">
+        <v>50013</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D173" s="1">
+        <v>3</v>
+      </c>
+      <c r="E173" s="1">
+        <v>3</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H173" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I173" s="1">
+        <v>18</v>
+      </c>
+      <c r="J173" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K173" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L173" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M173" s="1">
+        <v>1</v>
+      </c>
+      <c r="N173" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O173" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P173" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q173" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R173" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S173" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U173" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="V173" s="2">
+        <v>14.5936644</v>
+      </c>
+      <c r="W173" s="2">
+        <v>-87.831741600000001</v>
+      </c>
+    </row>
+    <row r="174" spans="1:23">
+      <c r="A174" s="1">
+        <v>50014</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D174" s="1">
+        <v>3</v>
+      </c>
+      <c r="E174" s="1">
+        <v>3</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G174" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H174" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I174" s="1">
+        <v>18</v>
+      </c>
+      <c r="J174" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K174" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L174" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M174" s="1">
+        <v>1</v>
+      </c>
+      <c r="N174" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O174" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P174" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q174" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R174" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S174" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U174" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="V174" s="2">
+        <v>14.598122099999999</v>
+      </c>
+      <c r="W174" s="2">
+        <v>-87.831477599999999</v>
+      </c>
+    </row>
+    <row r="175" spans="1:23">
+      <c r="A175" s="1">
+        <v>50015</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D175" s="1">
+        <v>3</v>
+      </c>
+      <c r="E175" s="1">
+        <v>3</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H175" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I175" s="1">
+        <v>18</v>
+      </c>
+      <c r="J175" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K175" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L175" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M175" s="1">
+        <v>1</v>
+      </c>
+      <c r="N175" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O175" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P175" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q175" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R175" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S175" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U175" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="V175" s="2">
+        <v>14.596882600000001</v>
+      </c>
+      <c r="W175" s="2">
+        <v>-87.840906599999997</v>
+      </c>
+    </row>
+    <row r="176" spans="1:23">
+      <c r="A176" s="1">
+        <v>50016</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D176" s="1">
+        <v>3</v>
+      </c>
+      <c r="E176" s="1">
+        <v>3</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H176" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I176" s="1">
+        <v>18</v>
+      </c>
+      <c r="J176" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K176" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L176" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M176" s="1">
+        <v>1</v>
+      </c>
+      <c r="N176" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O176" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P176" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q176" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R176" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S176" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U176" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="V176" s="2">
+        <v>14.5838927</v>
+      </c>
+      <c r="W176" s="2">
+        <v>-87.846112700000006</v>
+      </c>
+    </row>
+    <row r="177" spans="1:23">
+      <c r="A177" s="1">
+        <v>50017</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D177" s="1">
+        <v>3</v>
+      </c>
+      <c r="E177" s="1">
+        <v>3</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H177" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I177" s="1">
+        <v>18</v>
+      </c>
+      <c r="J177" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K177" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L177" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M177" s="1">
+        <v>1</v>
+      </c>
+      <c r="N177" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O177" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P177" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q177" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R177" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S177" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U177" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="V177" s="2">
+        <v>14.5993443</v>
+      </c>
+      <c r="W177" s="2">
+        <v>-87.8429754</v>
+      </c>
+    </row>
+    <row r="178" spans="1:23">
+      <c r="A178" s="1">
+        <v>50018</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D178" s="1">
+        <v>3</v>
+      </c>
+      <c r="E178" s="1">
+        <v>3</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G178" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H178" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I178" s="1">
+        <v>18</v>
+      </c>
+      <c r="J178" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K178" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L178" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M178" s="1">
+        <v>1</v>
+      </c>
+      <c r="N178" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O178" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P178" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q178" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R178" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S178" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U178" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="V178" s="2">
+        <v>14.5966769</v>
+      </c>
+      <c r="W178" s="2">
+        <v>-87.832520599999995</v>
+      </c>
+    </row>
+    <row r="179" spans="1:23">
+      <c r="A179" s="1">
+        <v>50019</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D179" s="1">
+        <v>3</v>
+      </c>
+      <c r="E179" s="1">
+        <v>3</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I179" s="1">
+        <v>18</v>
+      </c>
+      <c r="J179" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K179" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L179" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M179" s="1">
+        <v>1</v>
+      </c>
+      <c r="N179" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O179" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P179" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q179" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R179" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S179" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U179" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="V179" s="2">
+        <v>14.5967611</v>
+      </c>
+      <c r="W179" s="2">
+        <v>-87.840956000000006</v>
+      </c>
+    </row>
+    <row r="183" spans="1:23" ht="15">
+      <c r="T183" s="9"/>
+    </row>
+    <row r="184" spans="1:23" ht="15"/>
+    <row r="185" spans="1:23" ht="15"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U162">
-    <sortCondition ref="R2:R162"/>
-    <sortCondition ref="S2:S162"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U160">
+    <sortCondition ref="R2:R160"/>
+    <sortCondition ref="S2:S160"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-23-2020 15-09-18
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="639" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{133B870B-09C0-4216-8C99-C73D3287A0DA}"/>
+  <xr:revisionPtr revIDLastSave="1076" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E23114E6-42EE-4963-A0BA-734DCF680552}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="FARMACIAS" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FARMACIAS!$A$1:$W$179</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FARMACIAS!$A$1:$W$233</definedName>
     <definedName name="_xlnm.Database">FARMACIAS!$A$1:$U$160</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3340" uniqueCount="287">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -697,6 +697,204 @@
   </si>
   <si>
     <t>FarmaCity Calle 21 de agosto</t>
+  </si>
+  <si>
+    <t>Gracias a Dios</t>
+  </si>
+  <si>
+    <t>Puerto Lempira</t>
+  </si>
+  <si>
+    <t>HND-0901</t>
+  </si>
+  <si>
+    <t>Clinica medica JOZAM</t>
+  </si>
+  <si>
+    <t>Olancho</t>
+  </si>
+  <si>
+    <t>Catacamas</t>
+  </si>
+  <si>
+    <t>HND-1503</t>
+  </si>
+  <si>
+    <t>Farmacia y Clínica Eva</t>
+  </si>
+  <si>
+    <t>La union</t>
+  </si>
+  <si>
+    <t>La Union</t>
+  </si>
+  <si>
+    <t>HND-1513</t>
+  </si>
+  <si>
+    <t>Farmacia Regis La Unión</t>
+  </si>
+  <si>
+    <t>Dulce Nombre de Culmi</t>
+  </si>
+  <si>
+    <t>HND-1505</t>
+  </si>
+  <si>
+    <t>Farmacia Regis Culmi</t>
+  </si>
+  <si>
+    <t>Gualaco</t>
+  </si>
+  <si>
+    <t>HND-1508</t>
+  </si>
+  <si>
+    <t>Farmatodo</t>
+  </si>
+  <si>
+    <t>Farmacia Sol Farma</t>
+  </si>
+  <si>
+    <t>Farmacia Regis Gualaco</t>
+  </si>
+  <si>
+    <t>Juticalpa</t>
+  </si>
+  <si>
+    <t>HND-1501</t>
+  </si>
+  <si>
+    <t>Farmacia Santa Gertrudis</t>
+  </si>
+  <si>
+    <t>Farmacias del ahorro #88</t>
+  </si>
+  <si>
+    <t>Farmacia Y Clinica Samaritana</t>
+  </si>
+  <si>
+    <t>Farmacia Simán El Castaño</t>
+  </si>
+  <si>
+    <t>Farmacia Siman Blvd Los Poetas</t>
+  </si>
+  <si>
+    <t>farmacia santa teresa</t>
+  </si>
+  <si>
+    <t>San Francisco de la Paz</t>
+  </si>
+  <si>
+    <t>HND-1519</t>
+  </si>
+  <si>
+    <t>Farmacia Humana</t>
+  </si>
+  <si>
+    <t>San Esteban</t>
+  </si>
+  <si>
+    <t>HND-1517</t>
+  </si>
+  <si>
+    <t>FARMACIA REGIS 1</t>
+  </si>
+  <si>
+    <t>Farmacia San Pedro</t>
+  </si>
+  <si>
+    <t>Farmacia Barahona</t>
+  </si>
+  <si>
+    <t>Farmacia Simán Catacamas #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Juticalpa</t>
+  </si>
+  <si>
+    <t>Farmacias del Ahorro #3</t>
+  </si>
+  <si>
+    <t>Farmacia Central</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> La Unión</t>
+  </si>
+  <si>
+    <t>Farmacia Regis La Union Olancho</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> San Esteban</t>
+  </si>
+  <si>
+    <t>FARMACIA REGIS 2 SAN ESTEBAN</t>
+  </si>
+  <si>
+    <t>Farmacia Catacamas N.1</t>
+  </si>
+  <si>
+    <t>Farmacia Catacamas N.2</t>
+  </si>
+  <si>
+    <t>Farmacia Mishel</t>
+  </si>
+  <si>
+    <t>Farmacia Pharmavida</t>
+  </si>
+  <si>
+    <t>Guarizama</t>
+  </si>
+  <si>
+    <t>HND-1509</t>
+  </si>
+  <si>
+    <t>Comedor Y Farmacias Meylin</t>
+  </si>
+  <si>
+    <t>Farmacia Simán Juticalpa Barrio El Centro</t>
+  </si>
+  <si>
+    <t>Farmacia Simán Juticalpa Plaza Miromar</t>
+  </si>
+  <si>
+    <t>Farmacia Santa Fe</t>
+  </si>
+  <si>
+    <t>Farmacias del Ahorro Juticalpa 3</t>
+  </si>
+  <si>
+    <t>Farmacia del Ahorro</t>
+  </si>
+  <si>
+    <t>Farmacia Juticalpa</t>
+  </si>
+  <si>
+    <t>Farmacia Los Angeles</t>
+  </si>
+  <si>
+    <t>Farmacia Romely</t>
+  </si>
+  <si>
+    <t>Farmacia San Francisco</t>
+  </si>
+  <si>
+    <t>Farmacia Simán Juticalpa Blvd. Los Próceres</t>
+  </si>
+  <si>
+    <t>Farmacia Siman</t>
+  </si>
+  <si>
+    <t>Farmacia Suyapa #1</t>
+  </si>
+  <si>
+    <t>Farmacias Del Ahorro</t>
+  </si>
+  <si>
+    <t>Santa Maria del Real</t>
+  </si>
+  <si>
+    <t>HND-1520</t>
   </si>
 </sst>
 </file>
@@ -1357,8 +1555,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F90EE072-0F9D-4F60-9697-FDBBEB228828}" name="FARMACIAS_HN" displayName="FARMACIAS_HN" ref="A1:W179" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:W179" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F90EE072-0F9D-4F60-9697-FDBBEB228828}" name="FARMACIAS_HN" displayName="FARMACIAS_HN" ref="A1:W233" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:W233" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W160">
     <sortCondition ref="A1:A160"/>
   </sortState>
@@ -1688,11 +1886,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA185"/>
+  <dimension ref="A1:AA235"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="P167" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F172" sqref="F172"/>
+      <pane ySplit="1" topLeftCell="Q223" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S235" sqref="S235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -13371,8 +13569,8 @@
       <c r="E172" s="1">
         <v>3</v>
       </c>
-      <c r="F172" s="1">
-        <v>3</v>
+      <c r="F172" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="G172" s="1" t="s">
         <v>80</v>
@@ -13899,11 +14097,3681 @@
         <v>-87.840956000000006</v>
       </c>
     </row>
+    <row r="180" spans="1:23">
+      <c r="A180" s="1">
+        <v>50020</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D180" s="1">
+        <v>3</v>
+      </c>
+      <c r="E180" s="1">
+        <v>9</v>
+      </c>
+      <c r="F180" s="1">
+        <v>9</v>
+      </c>
+      <c r="G180" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H180" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I180" s="1">
+        <v>1</v>
+      </c>
+      <c r="J180" s="1">
+        <v>901</v>
+      </c>
+      <c r="K180" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="L180" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M180" s="1">
+        <v>1</v>
+      </c>
+      <c r="N180" s="1">
+        <v>90101</v>
+      </c>
+      <c r="O180" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="P180" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q180" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R180" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S180" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U180" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V180" s="2">
+        <v>15.257429999999999</v>
+      </c>
+      <c r="W180" s="2">
+        <v>-83.780617000000007</v>
+      </c>
+    </row>
+    <row r="181" spans="1:23">
+      <c r="A181" s="1">
+        <v>50021</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D181" s="1">
+        <v>3</v>
+      </c>
+      <c r="E181" s="1">
+        <v>9</v>
+      </c>
+      <c r="F181" s="1">
+        <v>9</v>
+      </c>
+      <c r="G181" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H181" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I181" s="1">
+        <v>1</v>
+      </c>
+      <c r="J181" s="1">
+        <v>901</v>
+      </c>
+      <c r="K181" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="L181" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M181" s="1">
+        <v>1</v>
+      </c>
+      <c r="N181" s="1">
+        <v>90101</v>
+      </c>
+      <c r="O181" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="P181" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q181" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="R181" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S181" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U181" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="V181" s="2">
+        <v>15.266281599999999</v>
+      </c>
+      <c r="W181" s="2">
+        <v>-83.772572199999999</v>
+      </c>
+    </row>
+    <row r="182" spans="1:23">
+      <c r="A182" s="1">
+        <v>50022</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D182" s="1">
+        <v>3</v>
+      </c>
+      <c r="E182" s="1">
+        <v>15</v>
+      </c>
+      <c r="F182" s="1">
+        <v>15</v>
+      </c>
+      <c r="G182" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H182" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I182" s="1">
+        <v>3</v>
+      </c>
+      <c r="J182" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K182" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L182" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M182" s="1">
+        <v>1</v>
+      </c>
+      <c r="N182" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O182" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P182" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q182" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R182" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S182" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U182" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="V182" s="2">
+        <v>14.8959817</v>
+      </c>
+      <c r="W182" s="2">
+        <v>-85.7856022</v>
+      </c>
+    </row>
     <row r="183" spans="1:23" ht="15">
-      <c r="T183" s="9"/>
-    </row>
-    <row r="184" spans="1:23" ht="15"/>
-    <row r="185" spans="1:23" ht="15"/>
+      <c r="A183" s="1">
+        <v>50023</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D183" s="1">
+        <v>3</v>
+      </c>
+      <c r="E183" s="1">
+        <v>15</v>
+      </c>
+      <c r="F183" s="1">
+        <v>15</v>
+      </c>
+      <c r="G183" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H183" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I183" s="1">
+        <v>13</v>
+      </c>
+      <c r="J183" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K183" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L183" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M183" s="1">
+        <v>1</v>
+      </c>
+      <c r="N183" s="1">
+        <v>151301</v>
+      </c>
+      <c r="O183" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="P183" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q183" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="R183" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S183" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U183" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="V183" s="2">
+        <v>15.022712</v>
+      </c>
+      <c r="W183" s="2">
+        <v>-86.709926899999999</v>
+      </c>
+    </row>
+    <row r="184" spans="1:23" ht="15">
+      <c r="A184" s="1">
+        <v>50024</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D184" s="1">
+        <v>3</v>
+      </c>
+      <c r="E184" s="1">
+        <v>15</v>
+      </c>
+      <c r="F184" s="1">
+        <v>15</v>
+      </c>
+      <c r="G184" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H184" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I184" s="1">
+        <v>5</v>
+      </c>
+      <c r="J184" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K184" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="L184" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M184" s="1">
+        <v>1</v>
+      </c>
+      <c r="N184" s="1">
+        <v>150501</v>
+      </c>
+      <c r="O184" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="P184" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q184" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="R184" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S184" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U184" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="V184" s="2">
+        <v>15.0837658</v>
+      </c>
+      <c r="W184" s="2">
+        <v>-85.556933099999995</v>
+      </c>
+    </row>
+    <row r="185" spans="1:23" ht="15">
+      <c r="A185" s="1">
+        <v>50025</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D185" s="1">
+        <v>3</v>
+      </c>
+      <c r="E185" s="1">
+        <v>15</v>
+      </c>
+      <c r="F185" s="1">
+        <v>15</v>
+      </c>
+      <c r="G185" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H185" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I185" s="1">
+        <v>8</v>
+      </c>
+      <c r="J185" s="1">
+        <v>1508</v>
+      </c>
+      <c r="K185" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="L185" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M185" s="1">
+        <v>1</v>
+      </c>
+      <c r="N185" s="1">
+        <v>150801</v>
+      </c>
+      <c r="O185" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="P185" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q185" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="R185" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S185" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U185" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="V185" s="2">
+        <v>15.025620699999999</v>
+      </c>
+      <c r="W185" s="2">
+        <v>-86.071155000000005</v>
+      </c>
+    </row>
+    <row r="186" spans="1:23">
+      <c r="A186" s="1">
+        <v>50026</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D186" s="1">
+        <v>3</v>
+      </c>
+      <c r="E186" s="1">
+        <v>15</v>
+      </c>
+      <c r="F186" s="1">
+        <v>15</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H186" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I186" s="1">
+        <v>8</v>
+      </c>
+      <c r="J186" s="1">
+        <v>1508</v>
+      </c>
+      <c r="K186" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="L186" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M186" s="1">
+        <v>1</v>
+      </c>
+      <c r="N186" s="1">
+        <v>150801</v>
+      </c>
+      <c r="O186" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="P186" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q186" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="R186" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S186" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U186" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="V186" s="2">
+        <v>15.023555399999999</v>
+      </c>
+      <c r="W186" s="2">
+        <v>-86.069538199999997</v>
+      </c>
+    </row>
+    <row r="187" spans="1:23">
+      <c r="A187" s="1">
+        <v>50027</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D187" s="1">
+        <v>3</v>
+      </c>
+      <c r="E187" s="1">
+        <v>15</v>
+      </c>
+      <c r="F187" s="1">
+        <v>15</v>
+      </c>
+      <c r="G187" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H187" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I187" s="1">
+        <v>8</v>
+      </c>
+      <c r="J187" s="1">
+        <v>1508</v>
+      </c>
+      <c r="K187" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="L187" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M187" s="1">
+        <v>1</v>
+      </c>
+      <c r="N187" s="1">
+        <v>150801</v>
+      </c>
+      <c r="O187" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="P187" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q187" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="R187" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S187" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U187" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="V187" s="2">
+        <v>15.027041000000001</v>
+      </c>
+      <c r="W187" s="2">
+        <v>-86.070589999999996</v>
+      </c>
+    </row>
+    <row r="188" spans="1:23">
+      <c r="A188" s="1">
+        <v>50028</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D188" s="1">
+        <v>3</v>
+      </c>
+      <c r="E188" s="1">
+        <v>15</v>
+      </c>
+      <c r="F188" s="1">
+        <v>15</v>
+      </c>
+      <c r="G188" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H188" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I188" s="1">
+        <v>1</v>
+      </c>
+      <c r="J188" s="1">
+        <v>1501</v>
+      </c>
+      <c r="K188" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L188" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M188" s="1">
+        <v>1</v>
+      </c>
+      <c r="N188" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O188" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P188" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q188" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R188" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S188" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U188" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="V188" s="2">
+        <v>14.670859399999999</v>
+      </c>
+      <c r="W188" s="2">
+        <v>-86.220775200000006</v>
+      </c>
+    </row>
+    <row r="189" spans="1:23">
+      <c r="A189" s="1">
+        <v>50029</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D189" s="1">
+        <v>3</v>
+      </c>
+      <c r="E189" s="1">
+        <v>15</v>
+      </c>
+      <c r="F189" s="1">
+        <v>15</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H189" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I189" s="1">
+        <v>3</v>
+      </c>
+      <c r="J189" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K189" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L189" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M189" s="1">
+        <v>1</v>
+      </c>
+      <c r="N189" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O189" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P189" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q189" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R189" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S189" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U189" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="V189" s="2">
+        <v>14.8461187</v>
+      </c>
+      <c r="W189" s="2">
+        <v>-85.890722999999994</v>
+      </c>
+    </row>
+    <row r="190" spans="1:23">
+      <c r="A190" s="1">
+        <v>50030</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D190" s="1">
+        <v>3</v>
+      </c>
+      <c r="E190" s="1">
+        <v>15</v>
+      </c>
+      <c r="F190" s="1">
+        <v>15</v>
+      </c>
+      <c r="G190" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H190" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I190" s="1">
+        <v>3</v>
+      </c>
+      <c r="J190" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K190" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L190" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M190" s="1">
+        <v>1</v>
+      </c>
+      <c r="N190" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O190" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P190" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q190" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R190" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S190" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U190" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="V190" s="2">
+        <v>14.850028</v>
+      </c>
+      <c r="W190" s="2">
+        <v>-85.896107000000001</v>
+      </c>
+    </row>
+    <row r="191" spans="1:23">
+      <c r="A191" s="1">
+        <v>50031</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D191" s="1">
+        <v>3</v>
+      </c>
+      <c r="E191" s="1">
+        <v>15</v>
+      </c>
+      <c r="F191" s="1">
+        <v>15</v>
+      </c>
+      <c r="G191" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H191" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I191" s="1">
+        <v>1</v>
+      </c>
+      <c r="J191" s="1">
+        <v>1501</v>
+      </c>
+      <c r="K191" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L191" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M191" s="1">
+        <v>1</v>
+      </c>
+      <c r="N191" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O191" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P191" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q191" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R191" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S191" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U191" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="V191" s="2">
+        <v>14.6652643</v>
+      </c>
+      <c r="W191" s="2">
+        <v>-86.215434599999995</v>
+      </c>
+    </row>
+    <row r="192" spans="1:23">
+      <c r="A192" s="1">
+        <v>50032</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D192" s="1">
+        <v>3</v>
+      </c>
+      <c r="E192" s="1">
+        <v>15</v>
+      </c>
+      <c r="F192" s="1">
+        <v>15</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H192" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I192" s="1">
+        <v>1</v>
+      </c>
+      <c r="J192" s="1">
+        <v>1501</v>
+      </c>
+      <c r="K192" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L192" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M192" s="1">
+        <v>1</v>
+      </c>
+      <c r="N192" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O192" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P192" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q192" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R192" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S192" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U192" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="V192" s="2">
+        <v>14.6666597</v>
+      </c>
+      <c r="W192" s="2">
+        <v>-86.217124400000003</v>
+      </c>
+    </row>
+    <row r="193" spans="1:23">
+      <c r="A193" s="1">
+        <v>50033</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D193" s="1">
+        <v>3</v>
+      </c>
+      <c r="E193" s="1">
+        <v>15</v>
+      </c>
+      <c r="F193" s="1">
+        <v>15</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H193" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I193" s="1">
+        <v>1</v>
+      </c>
+      <c r="J193" s="1">
+        <v>1501</v>
+      </c>
+      <c r="K193" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L193" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M193" s="1">
+        <v>1</v>
+      </c>
+      <c r="N193" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O193" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P193" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q193" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R193" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S193" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U193" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="V193" s="2">
+        <v>14.670673000000001</v>
+      </c>
+      <c r="W193" s="2">
+        <v>-86.218761299999997</v>
+      </c>
+    </row>
+    <row r="194" spans="1:23">
+      <c r="A194" s="1">
+        <v>50034</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D194" s="1">
+        <v>3</v>
+      </c>
+      <c r="E194" s="1">
+        <v>15</v>
+      </c>
+      <c r="F194" s="1">
+        <v>15</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H194" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I194" s="1">
+        <v>19</v>
+      </c>
+      <c r="J194" s="1">
+        <v>1519</v>
+      </c>
+      <c r="K194" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L194" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M194" s="1">
+        <v>1</v>
+      </c>
+      <c r="N194" s="1">
+        <v>151901</v>
+      </c>
+      <c r="O194" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="P194" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q194" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="R194" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S194" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U194" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V194" s="2">
+        <v>14.7413898</v>
+      </c>
+      <c r="W194" s="2">
+        <v>-86.0980481</v>
+      </c>
+    </row>
+    <row r="195" spans="1:23">
+      <c r="A195" s="1">
+        <v>50035</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D195" s="1">
+        <v>3</v>
+      </c>
+      <c r="E195" s="1">
+        <v>15</v>
+      </c>
+      <c r="F195" s="1">
+        <v>15</v>
+      </c>
+      <c r="G195" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H195" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I195" s="1">
+        <v>1</v>
+      </c>
+      <c r="J195" s="1">
+        <v>1501</v>
+      </c>
+      <c r="K195" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L195" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M195" s="1">
+        <v>1</v>
+      </c>
+      <c r="N195" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O195" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P195" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q195" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R195" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S195" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U195" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="V195" s="2">
+        <v>14.669445899999999</v>
+      </c>
+      <c r="W195" s="2">
+        <v>-86.217833799999994</v>
+      </c>
+    </row>
+    <row r="196" spans="1:23">
+      <c r="A196" s="1">
+        <v>50036</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D196" s="1">
+        <v>3</v>
+      </c>
+      <c r="E196" s="1">
+        <v>15</v>
+      </c>
+      <c r="F196" s="1">
+        <v>15</v>
+      </c>
+      <c r="G196" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H196" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I196" s="1">
+        <v>1</v>
+      </c>
+      <c r="J196" s="1">
+        <v>1501</v>
+      </c>
+      <c r="K196" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L196" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M196" s="1">
+        <v>1</v>
+      </c>
+      <c r="N196" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O196" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P196" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q196" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R196" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S196" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U196" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V196" s="2">
+        <v>14.6658057</v>
+      </c>
+      <c r="W196" s="2">
+        <v>-86.216798199999999</v>
+      </c>
+    </row>
+    <row r="197" spans="1:23">
+      <c r="A197" s="1">
+        <v>50037</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D197" s="1">
+        <v>3</v>
+      </c>
+      <c r="E197" s="1">
+        <v>15</v>
+      </c>
+      <c r="F197" s="1">
+        <v>15</v>
+      </c>
+      <c r="G197" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H197" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I197" s="1">
+        <v>17</v>
+      </c>
+      <c r="J197" s="1">
+        <v>1517</v>
+      </c>
+      <c r="K197" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="L197" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M197" s="1">
+        <v>1</v>
+      </c>
+      <c r="N197" s="1">
+        <v>151701</v>
+      </c>
+      <c r="O197" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="P197" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q197" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="R197" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S197" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U197" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="V197" s="2">
+        <v>15.213376999999999</v>
+      </c>
+      <c r="W197" s="2">
+        <v>-85.773096699999996</v>
+      </c>
+    </row>
+    <row r="198" spans="1:23">
+      <c r="A198" s="1">
+        <v>50038</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D198" s="1">
+        <v>3</v>
+      </c>
+      <c r="E198" s="1">
+        <v>15</v>
+      </c>
+      <c r="F198" s="1">
+        <v>15</v>
+      </c>
+      <c r="G198" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H198" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I198" s="1">
+        <v>3</v>
+      </c>
+      <c r="J198" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K198" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L198" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M198" s="1">
+        <v>1</v>
+      </c>
+      <c r="N198" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O198" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P198" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q198" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R198" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S198" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U198" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="V198" s="2">
+        <v>14.850630000000001</v>
+      </c>
+      <c r="W198" s="2">
+        <v>-85.893458499999994</v>
+      </c>
+    </row>
+    <row r="199" spans="1:23">
+      <c r="A199" s="1">
+        <v>50040</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D199" s="1">
+        <v>3</v>
+      </c>
+      <c r="E199" s="1">
+        <v>15</v>
+      </c>
+      <c r="F199" s="1">
+        <v>15</v>
+      </c>
+      <c r="G199" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H199" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I199" s="1">
+        <v>3</v>
+      </c>
+      <c r="J199" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K199" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L199" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M199" s="1">
+        <v>1</v>
+      </c>
+      <c r="N199" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O199" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P199" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q199" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R199" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S199" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U199" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V199" s="2">
+        <v>14.8499228</v>
+      </c>
+      <c r="W199" s="2">
+        <v>-85.893797800000002</v>
+      </c>
+    </row>
+    <row r="200" spans="1:23">
+      <c r="A200" s="1">
+        <v>50041</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D200" s="1">
+        <v>3</v>
+      </c>
+      <c r="E200" s="1">
+        <v>15</v>
+      </c>
+      <c r="F200" s="1">
+        <v>15</v>
+      </c>
+      <c r="G200" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H200" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I200" s="1">
+        <v>3</v>
+      </c>
+      <c r="J200" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K200" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L200" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M200" s="1">
+        <v>1</v>
+      </c>
+      <c r="N200" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O200" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P200" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q200" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R200" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S200" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U200" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="V200" s="2">
+        <v>14.852676000000001</v>
+      </c>
+      <c r="W200" s="2">
+        <v>-85.897805500000004</v>
+      </c>
+    </row>
+    <row r="201" spans="1:23">
+      <c r="A201" s="1">
+        <v>50042</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D201" s="1">
+        <v>3</v>
+      </c>
+      <c r="E201" s="1">
+        <v>15</v>
+      </c>
+      <c r="F201" s="1">
+        <v>15</v>
+      </c>
+      <c r="G201" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H201" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I201" s="1">
+        <v>3</v>
+      </c>
+      <c r="J201" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K201" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L201" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M201" s="1">
+        <v>1</v>
+      </c>
+      <c r="N201" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O201" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P201" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q201" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R201" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S201" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U201" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="V201" s="2">
+        <v>14.8465714</v>
+      </c>
+      <c r="W201" s="2">
+        <v>-85.901921200000004</v>
+      </c>
+    </row>
+    <row r="202" spans="1:23">
+      <c r="A202" s="1">
+        <v>50043</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D202" s="1">
+        <v>3</v>
+      </c>
+      <c r="E202" s="1">
+        <v>15</v>
+      </c>
+      <c r="F202" s="1">
+        <v>15</v>
+      </c>
+      <c r="G202" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H202" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I202" s="1">
+        <v>1</v>
+      </c>
+      <c r="J202" s="1">
+        <v>1501</v>
+      </c>
+      <c r="K202" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="L202" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M202" s="1">
+        <v>1</v>
+      </c>
+      <c r="N202" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O202" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="P202" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q202" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R202" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S202" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U202" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="V202" s="2">
+        <v>14.6666969</v>
+      </c>
+      <c r="W202" s="2">
+        <v>-86.217067700000001</v>
+      </c>
+    </row>
+    <row r="203" spans="1:23">
+      <c r="A203" s="1">
+        <v>50044</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D203" s="1">
+        <v>3</v>
+      </c>
+      <c r="E203" s="1">
+        <v>15</v>
+      </c>
+      <c r="F203" s="1">
+        <v>15</v>
+      </c>
+      <c r="G203" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H203" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I203" s="1">
+        <v>1</v>
+      </c>
+      <c r="J203" s="1">
+        <v>1501</v>
+      </c>
+      <c r="K203" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="L203" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M203" s="1">
+        <v>1</v>
+      </c>
+      <c r="N203" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O203" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="P203" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q203" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R203" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S203" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U203" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="V203" s="2">
+        <v>14.6703492</v>
+      </c>
+      <c r="W203" s="2">
+        <v>-86.219092799999999</v>
+      </c>
+    </row>
+    <row r="204" spans="1:23">
+      <c r="A204" s="1">
+        <v>50045</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D204" s="1">
+        <v>3</v>
+      </c>
+      <c r="E204" s="1">
+        <v>15</v>
+      </c>
+      <c r="F204" s="1">
+        <v>15</v>
+      </c>
+      <c r="G204" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H204" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I204" s="1">
+        <v>1</v>
+      </c>
+      <c r="J204" s="1">
+        <v>1501</v>
+      </c>
+      <c r="K204" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="L204" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M204" s="1">
+        <v>1</v>
+      </c>
+      <c r="N204" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O204" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="P204" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q204" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R204" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S204" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U204" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="V204" s="2">
+        <v>14.6705594</v>
+      </c>
+      <c r="W204" s="2">
+        <v>-86.210598099999999</v>
+      </c>
+    </row>
+    <row r="205" spans="1:23">
+      <c r="A205" s="1">
+        <v>50046</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D205" s="1">
+        <v>3</v>
+      </c>
+      <c r="E205" s="1">
+        <v>15</v>
+      </c>
+      <c r="F205" s="1">
+        <v>15</v>
+      </c>
+      <c r="G205" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H205" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I205" s="1">
+        <v>1</v>
+      </c>
+      <c r="J205" s="1">
+        <v>1501</v>
+      </c>
+      <c r="K205" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="L205" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M205" s="1">
+        <v>1</v>
+      </c>
+      <c r="N205" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O205" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="P205" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q205" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R205" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S205" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U205" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="V205" s="2">
+        <v>14.670534999999999</v>
+      </c>
+      <c r="W205" s="2">
+        <v>-86.219764699999999</v>
+      </c>
+    </row>
+    <row r="206" spans="1:23">
+      <c r="A206" s="1">
+        <v>50047</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D206" s="1">
+        <v>3</v>
+      </c>
+      <c r="E206" s="1">
+        <v>15</v>
+      </c>
+      <c r="F206" s="1">
+        <v>15</v>
+      </c>
+      <c r="G206" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H206" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I206" s="1">
+        <v>13</v>
+      </c>
+      <c r="J206" s="1">
+        <v>1513</v>
+      </c>
+      <c r="K206" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="L206" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M206" s="1">
+        <v>1</v>
+      </c>
+      <c r="N206" s="1">
+        <v>151301</v>
+      </c>
+      <c r="O206" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="P206" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q206" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="R206" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S206" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U206" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="V206" s="2">
+        <v>15.0225922</v>
+      </c>
+      <c r="W206" s="2">
+        <v>-86.709874200000002</v>
+      </c>
+    </row>
+    <row r="207" spans="1:23">
+      <c r="A207" s="1">
+        <v>50048</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D207" s="1">
+        <v>3</v>
+      </c>
+      <c r="E207" s="1">
+        <v>15</v>
+      </c>
+      <c r="F207" s="1">
+        <v>15</v>
+      </c>
+      <c r="G207" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H207" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I207" s="1">
+        <v>17</v>
+      </c>
+      <c r="J207" s="1">
+        <v>1517</v>
+      </c>
+      <c r="K207" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="L207" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M207" s="1">
+        <v>1</v>
+      </c>
+      <c r="N207" s="1">
+        <v>151701</v>
+      </c>
+      <c r="O207" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="P207" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q207" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="R207" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S207" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U207" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="V207" s="2">
+        <v>15.211404699999999</v>
+      </c>
+      <c r="W207" s="2">
+        <v>-85.771201599999998</v>
+      </c>
+    </row>
+    <row r="208" spans="1:23">
+      <c r="A208" s="1">
+        <v>50049</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D208" s="1">
+        <v>3</v>
+      </c>
+      <c r="E208" s="1">
+        <v>15</v>
+      </c>
+      <c r="F208" s="1">
+        <v>15</v>
+      </c>
+      <c r="G208" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H208" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I208" s="1">
+        <v>3</v>
+      </c>
+      <c r="J208" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K208" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L208" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M208" s="1">
+        <v>1</v>
+      </c>
+      <c r="N208" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O208" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P208" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q208" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R208" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S208" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U208" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="V208" s="2">
+        <v>14.847903799999999</v>
+      </c>
+      <c r="W208" s="2">
+        <v>-85.894117399999999</v>
+      </c>
+    </row>
+    <row r="209" spans="1:23">
+      <c r="A209" s="1">
+        <v>50050</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D209" s="1">
+        <v>3</v>
+      </c>
+      <c r="E209" s="1">
+        <v>15</v>
+      </c>
+      <c r="F209" s="1">
+        <v>15</v>
+      </c>
+      <c r="G209" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H209" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I209" s="1">
+        <v>3</v>
+      </c>
+      <c r="J209" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K209" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L209" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M209" s="1">
+        <v>1</v>
+      </c>
+      <c r="N209" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O209" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P209" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q209" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R209" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S209" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U209" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="V209" s="2">
+        <v>14.850289</v>
+      </c>
+      <c r="W209" s="2">
+        <v>-85.897228699999999</v>
+      </c>
+    </row>
+    <row r="210" spans="1:23">
+      <c r="A210" s="1">
+        <v>50051</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D210" s="1">
+        <v>3</v>
+      </c>
+      <c r="E210" s="1">
+        <v>15</v>
+      </c>
+      <c r="F210" s="1">
+        <v>15</v>
+      </c>
+      <c r="G210" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H210" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I210" s="1">
+        <v>3</v>
+      </c>
+      <c r="J210" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K210" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L210" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M210" s="1">
+        <v>1</v>
+      </c>
+      <c r="N210" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O210" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P210" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q210" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R210" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S210" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U210" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="V210" s="2">
+        <v>14.8437223</v>
+      </c>
+      <c r="W210" s="2">
+        <v>-85.879325199999997</v>
+      </c>
+    </row>
+    <row r="211" spans="1:23">
+      <c r="A211" s="1">
+        <v>50052</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D211" s="1">
+        <v>3</v>
+      </c>
+      <c r="E211" s="1">
+        <v>15</v>
+      </c>
+      <c r="F211" s="1">
+        <v>15</v>
+      </c>
+      <c r="G211" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H211" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I211" s="1">
+        <v>3</v>
+      </c>
+      <c r="J211" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K211" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L211" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M211" s="1">
+        <v>1</v>
+      </c>
+      <c r="N211" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O211" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P211" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q211" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R211" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S211" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U211" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="V211" s="2">
+        <v>14.846057800000001</v>
+      </c>
+      <c r="W211" s="2">
+        <v>-85.892754800000006</v>
+      </c>
+    </row>
+    <row r="212" spans="1:23">
+      <c r="A212" s="1">
+        <v>50053</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D212" s="1">
+        <v>3</v>
+      </c>
+      <c r="E212" s="1">
+        <v>15</v>
+      </c>
+      <c r="F212" s="1">
+        <v>15</v>
+      </c>
+      <c r="G212" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H212" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I212" s="1">
+        <v>3</v>
+      </c>
+      <c r="J212" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K212" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L212" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M212" s="1">
+        <v>1</v>
+      </c>
+      <c r="N212" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O212" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P212" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q212" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R212" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S212" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U212" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V212" s="2">
+        <v>14.8511802</v>
+      </c>
+      <c r="W212" s="2">
+        <v>-85.893879600000005</v>
+      </c>
+    </row>
+    <row r="213" spans="1:23">
+      <c r="A213" s="1">
+        <v>50054</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D213" s="1">
+        <v>3</v>
+      </c>
+      <c r="E213" s="1">
+        <v>15</v>
+      </c>
+      <c r="F213" s="1">
+        <v>15</v>
+      </c>
+      <c r="G213" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H213" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I213" s="1">
+        <v>3</v>
+      </c>
+      <c r="J213" s="1">
+        <v>1503</v>
+      </c>
+      <c r="K213" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L213" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M213" s="1">
+        <v>1</v>
+      </c>
+      <c r="N213" s="1">
+        <v>150301</v>
+      </c>
+      <c r="O213" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P213" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q213" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R213" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S213" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U213" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V213" s="2">
+        <v>14.8493031</v>
+      </c>
+      <c r="W213" s="2">
+        <v>-85.894384900000006</v>
+      </c>
+    </row>
+    <row r="214" spans="1:23">
+      <c r="A214" s="1">
+        <v>50055</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D214" s="1">
+        <v>3</v>
+      </c>
+      <c r="E214" s="1">
+        <v>15</v>
+      </c>
+      <c r="F214" s="1">
+        <v>15</v>
+      </c>
+      <c r="G214" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H214" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I214" s="1">
+        <v>9</v>
+      </c>
+      <c r="J214" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K214" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="L214" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M214" s="1">
+        <v>1</v>
+      </c>
+      <c r="N214" s="1">
+        <v>150901</v>
+      </c>
+      <c r="O214" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="P214" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q214" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="R214" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S214" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U214" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="V214" s="2">
+        <v>14.913563</v>
+      </c>
+      <c r="W214" s="2">
+        <v>-86.303442000000004</v>
+      </c>
+    </row>
+    <row r="215" spans="1:23">
+      <c r="A215" s="1">
+        <v>50056</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D215" s="1">
+        <v>3</v>
+      </c>
+      <c r="E215" s="1">
+        <v>15</v>
+      </c>
+      <c r="F215" s="1">
+        <v>15</v>
+      </c>
+      <c r="G215" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H215" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I215" s="1">
+        <v>9</v>
+      </c>
+      <c r="J215" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K215" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L215" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M215" s="1">
+        <v>1</v>
+      </c>
+      <c r="N215" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O215" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P215" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q215" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R215" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S215" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U215" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="V215" s="2">
+        <v>14.664275399999999</v>
+      </c>
+      <c r="W215" s="2">
+        <v>-86.215106700000007</v>
+      </c>
+    </row>
+    <row r="216" spans="1:23">
+      <c r="A216" s="1">
+        <v>50057</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D216" s="1">
+        <v>3</v>
+      </c>
+      <c r="E216" s="1">
+        <v>15</v>
+      </c>
+      <c r="F216" s="1">
+        <v>15</v>
+      </c>
+      <c r="G216" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H216" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I216" s="1">
+        <v>9</v>
+      </c>
+      <c r="J216" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K216" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L216" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M216" s="1">
+        <v>1</v>
+      </c>
+      <c r="N216" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O216" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P216" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q216" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R216" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S216" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U216" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="V216" s="2">
+        <v>14.6702645</v>
+      </c>
+      <c r="W216" s="2">
+        <v>-86.2208574</v>
+      </c>
+    </row>
+    <row r="217" spans="1:23">
+      <c r="A217" s="1">
+        <v>50058</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D217" s="1">
+        <v>3</v>
+      </c>
+      <c r="E217" s="1">
+        <v>15</v>
+      </c>
+      <c r="F217" s="1">
+        <v>15</v>
+      </c>
+      <c r="G217" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H217" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I217" s="1">
+        <v>9</v>
+      </c>
+      <c r="J217" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K217" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L217" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M217" s="1">
+        <v>1</v>
+      </c>
+      <c r="N217" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O217" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P217" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q217" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R217" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S217" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U217" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="V217" s="2">
+        <v>14.658246500000001</v>
+      </c>
+      <c r="W217" s="2">
+        <v>-86.215311900000003</v>
+      </c>
+    </row>
+    <row r="218" spans="1:23">
+      <c r="A218" s="1">
+        <v>50059</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D218" s="1">
+        <v>3</v>
+      </c>
+      <c r="E218" s="1">
+        <v>15</v>
+      </c>
+      <c r="F218" s="1">
+        <v>15</v>
+      </c>
+      <c r="G218" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H218" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I218" s="1">
+        <v>9</v>
+      </c>
+      <c r="J218" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K218" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L218" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M218" s="1">
+        <v>1</v>
+      </c>
+      <c r="N218" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O218" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P218" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q218" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R218" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S218" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U218" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="V218" s="2">
+        <v>14.6697212</v>
+      </c>
+      <c r="W218" s="2">
+        <v>-86.222785900000005</v>
+      </c>
+    </row>
+    <row r="219" spans="1:23">
+      <c r="A219" s="1">
+        <v>50060</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D219" s="1">
+        <v>3</v>
+      </c>
+      <c r="E219" s="1">
+        <v>15</v>
+      </c>
+      <c r="F219" s="1">
+        <v>15</v>
+      </c>
+      <c r="G219" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H219" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I219" s="1">
+        <v>9</v>
+      </c>
+      <c r="J219" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K219" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L219" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M219" s="1">
+        <v>1</v>
+      </c>
+      <c r="N219" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O219" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P219" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q219" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R219" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S219" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U219" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V219" s="2">
+        <v>14.666747300000001</v>
+      </c>
+      <c r="W219" s="2">
+        <v>-86.225702100000007</v>
+      </c>
+    </row>
+    <row r="220" spans="1:23">
+      <c r="A220" s="1">
+        <v>50061</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D220" s="1">
+        <v>3</v>
+      </c>
+      <c r="E220" s="1">
+        <v>15</v>
+      </c>
+      <c r="F220" s="1">
+        <v>15</v>
+      </c>
+      <c r="G220" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H220" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I220" s="1">
+        <v>9</v>
+      </c>
+      <c r="J220" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K220" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L220" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M220" s="1">
+        <v>1</v>
+      </c>
+      <c r="N220" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O220" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P220" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q220" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R220" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S220" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U220" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="V220" s="2">
+        <v>14.6667962</v>
+      </c>
+      <c r="W220" s="2">
+        <v>-86.225291299999995</v>
+      </c>
+    </row>
+    <row r="221" spans="1:23">
+      <c r="A221" s="1">
+        <v>50062</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D221" s="1">
+        <v>3</v>
+      </c>
+      <c r="E221" s="1">
+        <v>15</v>
+      </c>
+      <c r="F221" s="1">
+        <v>15</v>
+      </c>
+      <c r="G221" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H221" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I221" s="1">
+        <v>9</v>
+      </c>
+      <c r="J221" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K221" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L221" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M221" s="1">
+        <v>1</v>
+      </c>
+      <c r="N221" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O221" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P221" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q221" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R221" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S221" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U221" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="V221" s="2">
+        <v>14.6669065</v>
+      </c>
+      <c r="W221" s="2">
+        <v>-86.226855099999995</v>
+      </c>
+    </row>
+    <row r="222" spans="1:23">
+      <c r="A222" s="1">
+        <v>50063</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D222" s="1">
+        <v>3</v>
+      </c>
+      <c r="E222" s="1">
+        <v>15</v>
+      </c>
+      <c r="F222" s="1">
+        <v>15</v>
+      </c>
+      <c r="G222" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H222" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I222" s="1">
+        <v>9</v>
+      </c>
+      <c r="J222" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K222" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L222" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M222" s="1">
+        <v>1</v>
+      </c>
+      <c r="N222" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O222" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P222" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q222" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R222" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S222" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U222" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="V222" s="2">
+        <v>14.671393200000001</v>
+      </c>
+      <c r="W222" s="2">
+        <v>-86.219501500000007</v>
+      </c>
+    </row>
+    <row r="223" spans="1:23">
+      <c r="A223" s="1">
+        <v>50064</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D223" s="1">
+        <v>3</v>
+      </c>
+      <c r="E223" s="1">
+        <v>15</v>
+      </c>
+      <c r="F223" s="1">
+        <v>15</v>
+      </c>
+      <c r="G223" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H223" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I223" s="1">
+        <v>9</v>
+      </c>
+      <c r="J223" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K223" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L223" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M223" s="1">
+        <v>1</v>
+      </c>
+      <c r="N223" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O223" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P223" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q223" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R223" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S223" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U223" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="V223" s="2">
+        <v>14.668580499999999</v>
+      </c>
+      <c r="W223" s="2">
+        <v>-86.217693999999995</v>
+      </c>
+    </row>
+    <row r="224" spans="1:23">
+      <c r="A224" s="1">
+        <v>50065</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D224" s="1">
+        <v>3</v>
+      </c>
+      <c r="E224" s="1">
+        <v>15</v>
+      </c>
+      <c r="F224" s="1">
+        <v>15</v>
+      </c>
+      <c r="G224" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H224" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I224" s="1">
+        <v>9</v>
+      </c>
+      <c r="J224" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K224" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L224" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M224" s="1">
+        <v>1</v>
+      </c>
+      <c r="N224" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O224" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P224" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q224" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R224" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S224" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U224" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="V224" s="2">
+        <v>14.6666107</v>
+      </c>
+      <c r="W224" s="2">
+        <v>-86.225996800000004</v>
+      </c>
+    </row>
+    <row r="225" spans="1:23">
+      <c r="A225" s="1">
+        <v>50066</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D225" s="1">
+        <v>3</v>
+      </c>
+      <c r="E225" s="1">
+        <v>15</v>
+      </c>
+      <c r="F225" s="1">
+        <v>15</v>
+      </c>
+      <c r="G225" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H225" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I225" s="1">
+        <v>9</v>
+      </c>
+      <c r="J225" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K225" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L225" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M225" s="1">
+        <v>1</v>
+      </c>
+      <c r="N225" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O225" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P225" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q225" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R225" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S225" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U225" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="V225" s="2">
+        <v>14.6675375</v>
+      </c>
+      <c r="W225" s="2">
+        <v>-86.2174646</v>
+      </c>
+    </row>
+    <row r="226" spans="1:23">
+      <c r="A226" s="1">
+        <v>50067</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D226" s="1">
+        <v>3</v>
+      </c>
+      <c r="E226" s="1">
+        <v>15</v>
+      </c>
+      <c r="F226" s="1">
+        <v>15</v>
+      </c>
+      <c r="G226" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H226" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I226" s="1">
+        <v>9</v>
+      </c>
+      <c r="J226" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K226" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L226" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M226" s="1">
+        <v>1</v>
+      </c>
+      <c r="N226" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O226" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P226" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q226" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R226" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S226" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U226" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V226" s="2">
+        <v>14.665284099999999</v>
+      </c>
+      <c r="W226" s="2">
+        <v>-86.215462099999996</v>
+      </c>
+    </row>
+    <row r="227" spans="1:23">
+      <c r="A227" s="1">
+        <v>50068</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D227" s="1">
+        <v>3</v>
+      </c>
+      <c r="E227" s="1">
+        <v>15</v>
+      </c>
+      <c r="F227" s="1">
+        <v>15</v>
+      </c>
+      <c r="G227" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H227" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I227" s="1">
+        <v>9</v>
+      </c>
+      <c r="J227" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K227" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L227" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M227" s="1">
+        <v>1</v>
+      </c>
+      <c r="N227" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O227" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P227" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q227" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R227" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S227" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U227" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="V227" s="2">
+        <v>14.666357100000001</v>
+      </c>
+      <c r="W227" s="2">
+        <v>-86.217201000000003</v>
+      </c>
+    </row>
+    <row r="228" spans="1:23">
+      <c r="A228" s="1">
+        <v>50069</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D228" s="1">
+        <v>3</v>
+      </c>
+      <c r="E228" s="1">
+        <v>15</v>
+      </c>
+      <c r="F228" s="1">
+        <v>15</v>
+      </c>
+      <c r="G228" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H228" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I228" s="1">
+        <v>9</v>
+      </c>
+      <c r="J228" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K228" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L228" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M228" s="1">
+        <v>1</v>
+      </c>
+      <c r="N228" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O228" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P228" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q228" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R228" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S228" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U228" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="V228" s="2">
+        <v>14.671502200000001</v>
+      </c>
+      <c r="W228" s="2">
+        <v>-86.221389400000007</v>
+      </c>
+    </row>
+    <row r="229" spans="1:23">
+      <c r="A229" s="1">
+        <v>50070</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D229" s="1">
+        <v>3</v>
+      </c>
+      <c r="E229" s="1">
+        <v>15</v>
+      </c>
+      <c r="F229" s="1">
+        <v>15</v>
+      </c>
+      <c r="G229" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H229" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I229" s="1">
+        <v>9</v>
+      </c>
+      <c r="J229" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K229" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L229" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M229" s="1">
+        <v>1</v>
+      </c>
+      <c r="N229" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O229" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P229" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q229" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R229" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S229" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U229" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="V229" s="2">
+        <v>14.669881500000001</v>
+      </c>
+      <c r="W229" s="2">
+        <v>-86.219860199999999</v>
+      </c>
+    </row>
+    <row r="230" spans="1:23">
+      <c r="A230" s="1">
+        <v>50071</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D230" s="1">
+        <v>3</v>
+      </c>
+      <c r="E230" s="1">
+        <v>15</v>
+      </c>
+      <c r="F230" s="1">
+        <v>15</v>
+      </c>
+      <c r="G230" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H230" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I230" s="1">
+        <v>9</v>
+      </c>
+      <c r="J230" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K230" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L230" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M230" s="1">
+        <v>1</v>
+      </c>
+      <c r="N230" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O230" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P230" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q230" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R230" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S230" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U230" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="V230" s="2">
+        <v>14.6712817</v>
+      </c>
+      <c r="W230" s="2">
+        <v>-86.2198408</v>
+      </c>
+    </row>
+    <row r="231" spans="1:23">
+      <c r="A231" s="1">
+        <v>50072</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D231" s="1">
+        <v>3</v>
+      </c>
+      <c r="E231" s="1">
+        <v>15</v>
+      </c>
+      <c r="F231" s="1">
+        <v>15</v>
+      </c>
+      <c r="G231" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H231" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I231" s="1">
+        <v>9</v>
+      </c>
+      <c r="J231" s="1">
+        <v>1509</v>
+      </c>
+      <c r="K231" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L231" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M231" s="1">
+        <v>1</v>
+      </c>
+      <c r="N231" s="1">
+        <v>150101</v>
+      </c>
+      <c r="O231" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P231" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q231" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R231" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S231" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U231" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="V231" s="2">
+        <v>14.670398499999999</v>
+      </c>
+      <c r="W231" s="2">
+        <v>-86.218262300000006</v>
+      </c>
+    </row>
+    <row r="232" spans="1:23">
+      <c r="A232" s="1">
+        <v>50073</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D232" s="1">
+        <v>3</v>
+      </c>
+      <c r="E232" s="1">
+        <v>15</v>
+      </c>
+      <c r="F232" s="1">
+        <v>15</v>
+      </c>
+      <c r="G232" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H232" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I232" s="1">
+        <v>17</v>
+      </c>
+      <c r="J232" s="1">
+        <v>1517</v>
+      </c>
+      <c r="K232" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="L232" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M232" s="1">
+        <v>1</v>
+      </c>
+      <c r="N232" s="1">
+        <v>151701</v>
+      </c>
+      <c r="O232" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="P232" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q232" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="R232" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S232" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U232" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V232" s="2">
+        <v>15.213129800000001</v>
+      </c>
+      <c r="W232" s="2">
+        <v>-85.771611500000006</v>
+      </c>
+    </row>
+    <row r="233" spans="1:23">
+      <c r="A233" s="1">
+        <v>50074</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D233" s="1">
+        <v>3</v>
+      </c>
+      <c r="E233" s="1">
+        <v>15</v>
+      </c>
+      <c r="F233" s="1">
+        <v>15</v>
+      </c>
+      <c r="G233" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H233" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I233" s="1">
+        <v>20</v>
+      </c>
+      <c r="J233" s="1">
+        <v>1520</v>
+      </c>
+      <c r="K233" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="L233" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M233" s="1">
+        <v>1</v>
+      </c>
+      <c r="N233" s="1">
+        <v>152001</v>
+      </c>
+      <c r="O233" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="P233" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q233" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="R233" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S233" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U233" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V233" s="2">
+        <v>14.8238468</v>
+      </c>
+      <c r="W233" s="2">
+        <v>-85.930354199999996</v>
+      </c>
+    </row>
+    <row r="235" spans="1:23" ht="15">
+      <c r="S235" s="9"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U160">
     <sortCondition ref="R2:R160"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-24-2020 15-06-13
</commit_message>
<xml_diff>
--- a/datacovidhn/FARMACIAS_HN.xlsx
+++ b/datacovidhn/FARMACIAS_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1076" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E23114E6-42EE-4963-A0BA-734DCF680552}"/>
+  <xr:revisionPtr revIDLastSave="1079" documentId="8_{916CAA4F-0C4B-41B0-9C01-872BC023B4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{12CF6402-D76C-49A5-80CF-C39B3C89AB4E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1889,8 +1889,8 @@
   <dimension ref="A1:AA235"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="Q223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S235" sqref="S235"/>
+      <pane ySplit="1" topLeftCell="T128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V144" sqref="V144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -1919,7 +1919,7 @@
     <col min="23" max="23" width="13.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="5" customFormat="1">
+    <row r="1" spans="1:27" s="5" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:27">
       <c r="A2" s="1">
         <v>17840</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>-87.057100000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:27">
       <c r="A3" s="1">
         <v>18049</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>-87.179100000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:27">
       <c r="A4" s="1">
         <v>18065</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>-87.175299999999993</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:27">
       <c r="A5" s="1">
         <v>24496</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>-87.232399999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:27">
       <c r="A6" s="1">
         <v>24554</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>-87.211399999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:27">
       <c r="A7" s="1">
         <v>24613</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>-87.2226</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:27">
       <c r="A8" s="1">
         <v>24618</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>-87.222300000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:27">
       <c r="A9" s="1">
         <v>24623</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>-87.222099999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:27">
       <c r="A10" s="1">
         <v>24627</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>-87.229299999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:27">
       <c r="A11" s="1">
         <v>24646</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>-87.189599999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:27" ht="15">
       <c r="A12" s="1">
         <v>24650</v>
       </c>
@@ -2737,8 +2737,9 @@
       <c r="W12" s="2">
         <v>-87.189400000000006</v>
       </c>
-    </row>
-    <row r="13" spans="1:23">
+      <c r="AA12" s="8"/>
+    </row>
+    <row r="13" spans="1:27">
       <c r="A13" s="1">
         <v>24656</v>
       </c>
@@ -2806,7 +2807,7 @@
         <v>-87.220600000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:27">
       <c r="A14" s="1">
         <v>24667</v>
       </c>
@@ -2871,10 +2872,10 @@
         <v>14.0601</v>
       </c>
       <c r="W14" s="2">
-        <v>-83.400400000000005</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23">
+        <v>-87.400400000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27">
       <c r="A15" s="1">
         <v>24701</v>
       </c>
@@ -2942,7 +2943,7 @@
         <v>-87.209599999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:27">
       <c r="A16" s="1">
         <v>24711</v>
       </c>
@@ -11712,7 +11713,7 @@
         <v>15.5989</v>
       </c>
       <c r="W144" s="2">
-        <v>-87.208799999999997</v>
+        <v>-87.102687200000005</v>
       </c>
     </row>
     <row r="145" spans="1:27" ht="15">

</xml_diff>